<commit_message>
Ergebnisdokumentation zu React erweitern/überarbeiten
</commit_message>
<xml_diff>
--- a/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
+++ b/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yara\Dropbox\Studium\Semester 6\FRONT\FRONT_Projekt\front-projekt\documents\Projektmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA59273-C51B-4BE8-8F37-00C7A2379D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757C826E-AB07-4BEF-ACD8-5FA040663AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1205,13 +1205,13 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="180"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1449,7 +1449,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I68" sqref="I68"/>
+      <selection pane="bottomLeft" activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1584,7 +1584,7 @@
       </c>
       <c r="H6" s="30">
         <f>SUM(H10:H74)</f>
-        <v>66.5</v>
+        <v>67.25</v>
       </c>
       <c r="I6" s="27">
         <f>SUM(I10:I74)</f>
@@ -1620,7 +1620,7 @@
       </c>
       <c r="H7" s="30">
         <f t="shared" ref="H7:J7" si="1">H5-H6</f>
-        <v>53.5</v>
+        <v>52.75</v>
       </c>
       <c r="I7" s="27">
         <f t="shared" si="1"/>
@@ -3299,7 +3299,7 @@
         <v>250</v>
       </c>
       <c r="H66" s="22">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I66" s="22"/>
       <c r="J66" s="22">
@@ -3329,7 +3329,7 @@
         <v>251</v>
       </c>
       <c r="H67" s="22">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="I67" s="22"/>
       <c r="J67" s="22">
@@ -3614,96 +3614,96 @@
       <c r="AK1" s="67"/>
       <c r="AL1" s="67"/>
       <c r="AM1" s="67"/>
-      <c r="AN1" s="64" t="s">
+      <c r="AN1" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="AO1" s="65"/>
-      <c r="AP1" s="65"/>
-      <c r="AQ1" s="65"/>
-      <c r="AR1" s="65"/>
-      <c r="AS1" s="65"/>
-      <c r="AT1" s="65"/>
-      <c r="AU1" s="64" t="s">
+      <c r="AO1" s="64"/>
+      <c r="AP1" s="64"/>
+      <c r="AQ1" s="64"/>
+      <c r="AR1" s="64"/>
+      <c r="AS1" s="64"/>
+      <c r="AT1" s="64"/>
+      <c r="AU1" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="AV1" s="65"/>
-      <c r="AW1" s="65"/>
-      <c r="AX1" s="65"/>
-      <c r="AY1" s="65"/>
-      <c r="AZ1" s="65"/>
-      <c r="BA1" s="65"/>
-      <c r="BB1" s="64" t="s">
+      <c r="AV1" s="64"/>
+      <c r="AW1" s="64"/>
+      <c r="AX1" s="64"/>
+      <c r="AY1" s="64"/>
+      <c r="AZ1" s="64"/>
+      <c r="BA1" s="64"/>
+      <c r="BB1" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="BC1" s="65"/>
-      <c r="BD1" s="65"/>
-      <c r="BE1" s="65"/>
-      <c r="BF1" s="65"/>
-      <c r="BG1" s="65"/>
-      <c r="BH1" s="65"/>
-      <c r="BI1" s="64" t="s">
+      <c r="BC1" s="64"/>
+      <c r="BD1" s="64"/>
+      <c r="BE1" s="64"/>
+      <c r="BF1" s="64"/>
+      <c r="BG1" s="64"/>
+      <c r="BH1" s="64"/>
+      <c r="BI1" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="BJ1" s="65"/>
-      <c r="BK1" s="65"/>
-      <c r="BL1" s="65"/>
-      <c r="BM1" s="65"/>
-      <c r="BN1" s="65"/>
-      <c r="BO1" s="65"/>
-      <c r="BP1" s="64" t="s">
+      <c r="BJ1" s="64"/>
+      <c r="BK1" s="64"/>
+      <c r="BL1" s="64"/>
+      <c r="BM1" s="64"/>
+      <c r="BN1" s="64"/>
+      <c r="BO1" s="64"/>
+      <c r="BP1" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="BQ1" s="65"/>
-      <c r="BR1" s="65"/>
-      <c r="BS1" s="65"/>
-      <c r="BT1" s="65"/>
-      <c r="BU1" s="65"/>
-      <c r="BV1" s="65"/>
-      <c r="BW1" s="64" t="s">
+      <c r="BQ1" s="64"/>
+      <c r="BR1" s="64"/>
+      <c r="BS1" s="64"/>
+      <c r="BT1" s="64"/>
+      <c r="BU1" s="64"/>
+      <c r="BV1" s="64"/>
+      <c r="BW1" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="BX1" s="65"/>
-      <c r="BY1" s="65"/>
-      <c r="BZ1" s="65"/>
-      <c r="CA1" s="65"/>
-      <c r="CB1" s="65"/>
-      <c r="CC1" s="65"/>
-      <c r="CD1" s="64" t="s">
+      <c r="BX1" s="64"/>
+      <c r="BY1" s="64"/>
+      <c r="BZ1" s="64"/>
+      <c r="CA1" s="64"/>
+      <c r="CB1" s="64"/>
+      <c r="CC1" s="64"/>
+      <c r="CD1" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="CE1" s="65"/>
-      <c r="CF1" s="65"/>
-      <c r="CG1" s="65"/>
-      <c r="CH1" s="65"/>
-      <c r="CI1" s="65"/>
-      <c r="CJ1" s="65"/>
-      <c r="CK1" s="64" t="s">
+      <c r="CE1" s="64"/>
+      <c r="CF1" s="64"/>
+      <c r="CG1" s="64"/>
+      <c r="CH1" s="64"/>
+      <c r="CI1" s="64"/>
+      <c r="CJ1" s="64"/>
+      <c r="CK1" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="CL1" s="65"/>
-      <c r="CM1" s="65"/>
-      <c r="CN1" s="65"/>
-      <c r="CO1" s="65"/>
-      <c r="CP1" s="65"/>
-      <c r="CQ1" s="65"/>
-      <c r="CR1" s="64" t="s">
+      <c r="CL1" s="64"/>
+      <c r="CM1" s="64"/>
+      <c r="CN1" s="64"/>
+      <c r="CO1" s="64"/>
+      <c r="CP1" s="64"/>
+      <c r="CQ1" s="64"/>
+      <c r="CR1" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="CS1" s="65"/>
-      <c r="CT1" s="65"/>
-      <c r="CU1" s="65"/>
-      <c r="CV1" s="65"/>
-      <c r="CW1" s="65"/>
-      <c r="CX1" s="65"/>
-      <c r="CY1" s="64" t="s">
+      <c r="CS1" s="64"/>
+      <c r="CT1" s="64"/>
+      <c r="CU1" s="64"/>
+      <c r="CV1" s="64"/>
+      <c r="CW1" s="64"/>
+      <c r="CX1" s="64"/>
+      <c r="CY1" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="CZ1" s="65"/>
-      <c r="DA1" s="65"/>
-      <c r="DB1" s="65"/>
-      <c r="DC1" s="65"/>
-      <c r="DD1" s="65"/>
-      <c r="DE1" s="65"/>
+      <c r="CZ1" s="64"/>
+      <c r="DA1" s="64"/>
+      <c r="DB1" s="64"/>
+      <c r="DC1" s="64"/>
+      <c r="DD1" s="64"/>
+      <c r="DE1" s="64"/>
       <c r="DF1" s="2"/>
       <c r="DG1" s="2"/>
       <c r="DH1" s="2"/>
@@ -5178,7 +5178,7 @@
     </row>
     <row r="46" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
-      <c r="B46" s="63" t="s">
+      <c r="B46" s="65" t="s">
         <v>54</v>
       </c>
       <c r="C46" s="15" t="s">
@@ -5187,21 +5187,21 @@
     </row>
     <row r="47" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
-      <c r="B47" s="63"/>
+      <c r="B47" s="65"/>
       <c r="C47" s="15" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
-      <c r="B48" s="63"/>
+      <c r="B48" s="65"/>
       <c r="C48" s="15" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:71" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
-      <c r="B49" s="63"/>
+      <c r="B49" s="65"/>
       <c r="C49" s="15" t="s">
         <v>224</v>
       </c>
@@ -5211,211 +5211,211 @@
     </row>
     <row r="50" spans="1:71" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A50" s="6"/>
-      <c r="B50" s="63"/>
+      <c r="B50" s="65"/>
       <c r="C50" s="15" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:71" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
-      <c r="B51" s="63"/>
+      <c r="B51" s="65"/>
       <c r="C51" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:71" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B52" s="63"/>
+      <c r="B52" s="65"/>
       <c r="C52" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:71" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B53" s="63"/>
+      <c r="B53" s="65"/>
       <c r="C53" s="15" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:71" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A54" s="6"/>
-      <c r="B54" s="63"/>
+      <c r="B54" s="65"/>
       <c r="C54" s="15" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:71" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A55" s="6"/>
-      <c r="B55" s="63"/>
+      <c r="B55" s="65"/>
       <c r="C55" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:71" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A56" s="6"/>
-      <c r="B56" s="63"/>
+      <c r="B56" s="65"/>
       <c r="C56" s="15" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:71" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A57" s="6"/>
-      <c r="B57" s="63"/>
+      <c r="B57" s="65"/>
       <c r="C57" s="15" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="63"/>
+      <c r="B58" s="65"/>
       <c r="C58" s="15" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:71" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B59" s="63"/>
+      <c r="B59" s="65"/>
       <c r="C59" s="15" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="60" spans="1:71" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B60" s="63"/>
+      <c r="B60" s="65"/>
       <c r="C60" s="15" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="61" spans="1:71" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B61" s="63"/>
+      <c r="B61" s="65"/>
       <c r="C61" s="15" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:71" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B62" s="63"/>
+      <c r="B62" s="65"/>
       <c r="C62" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:71" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B63" s="63"/>
+      <c r="B63" s="65"/>
       <c r="C63" s="15" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:71" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B64" s="63"/>
+      <c r="B64" s="65"/>
       <c r="C64" s="15"/>
     </row>
     <row r="65" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B65" s="63"/>
+      <c r="B65" s="65"/>
       <c r="C65" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="66" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B66" s="63"/>
+      <c r="B66" s="65"/>
       <c r="C66" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="67" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B67" s="63"/>
+      <c r="B67" s="65"/>
       <c r="C67" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="68" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B68" s="63"/>
+      <c r="B68" s="65"/>
       <c r="C68" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="69" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B69" s="63"/>
+      <c r="B69" s="65"/>
       <c r="C69" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="70" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B70" s="63"/>
+      <c r="B70" s="65"/>
       <c r="C70" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="71" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B71" s="63"/>
+      <c r="B71" s="65"/>
       <c r="C71" s="15" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="72" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B72" s="63"/>
+      <c r="B72" s="65"/>
       <c r="C72" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="73" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B73" s="63"/>
+      <c r="B73" s="65"/>
       <c r="C73" s="15" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="74" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B74" s="63"/>
+      <c r="B74" s="65"/>
       <c r="C74" s="16"/>
     </row>
     <row r="75" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B75" s="63"/>
+      <c r="B75" s="65"/>
       <c r="C75" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="76" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B76" s="63"/>
+      <c r="B76" s="65"/>
       <c r="C76" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="77" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B77" s="63"/>
+      <c r="B77" s="65"/>
       <c r="C77" s="15" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="78" spans="2:53" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B78" s="63"/>
+      <c r="B78" s="65"/>
       <c r="C78" s="15" t="s">
         <v>72</v>
       </c>
       <c r="BA78" s="6"/>
     </row>
     <row r="79" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B79" s="63"/>
+      <c r="B79" s="65"/>
       <c r="C79" s="16"/>
     </row>
     <row r="80" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B80" s="63"/>
+      <c r="B80" s="65"/>
       <c r="C80" s="15" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="81" spans="2:75" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B81" s="63"/>
+      <c r="B81" s="65"/>
       <c r="C81" s="60" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="82" spans="2:75" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B82" s="63"/>
+      <c r="B82" s="65"/>
       <c r="C82" s="60" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="83" spans="2:75" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B83" s="63"/>
+      <c r="B83" s="65"/>
       <c r="C83" s="60" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="84" spans="2:75" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B84" s="63"/>
+      <c r="B84" s="65"/>
       <c r="C84" s="15" t="s">
         <v>258</v>
       </c>
@@ -8170,11 +8170,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="CD1:CJ1"/>
-    <mergeCell ref="B79:B84"/>
-    <mergeCell ref="B46:B78"/>
-    <mergeCell ref="CK1:CQ1"/>
-    <mergeCell ref="CR1:CX1"/>
     <mergeCell ref="CY1:DE1"/>
     <mergeCell ref="E1:K1"/>
     <mergeCell ref="L1:R1"/>
@@ -8187,6 +8182,11 @@
     <mergeCell ref="BI1:BO1"/>
     <mergeCell ref="BP1:BV1"/>
     <mergeCell ref="BW1:CC1"/>
+    <mergeCell ref="CD1:CJ1"/>
+    <mergeCell ref="B79:B84"/>
+    <mergeCell ref="B46:B78"/>
+    <mergeCell ref="CK1:CQ1"/>
+    <mergeCell ref="CR1:CX1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:J4 L4:CW4 CY4:EV4">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
@@ -8221,194 +8221,194 @@
   <sheetData>
     <row r="1" spans="1:158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C1" s="1"/>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="64" t="s">
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="64" t="s">
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="64" t="s">
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="64"/>
+      <c r="X1" s="64"/>
+      <c r="Y1" s="64"/>
+      <c r="Z1" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="65"/>
-      <c r="AC1" s="65"/>
-      <c r="AD1" s="65"/>
-      <c r="AE1" s="65"/>
-      <c r="AF1" s="65"/>
-      <c r="AG1" s="64" t="s">
+      <c r="AA1" s="64"/>
+      <c r="AB1" s="64"/>
+      <c r="AC1" s="64"/>
+      <c r="AD1" s="64"/>
+      <c r="AE1" s="64"/>
+      <c r="AF1" s="64"/>
+      <c r="AG1" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="AH1" s="65"/>
-      <c r="AI1" s="65"/>
-      <c r="AJ1" s="65"/>
-      <c r="AK1" s="65"/>
-      <c r="AL1" s="65"/>
-      <c r="AM1" s="65"/>
-      <c r="AN1" s="64" t="s">
+      <c r="AH1" s="64"/>
+      <c r="AI1" s="64"/>
+      <c r="AJ1" s="64"/>
+      <c r="AK1" s="64"/>
+      <c r="AL1" s="64"/>
+      <c r="AM1" s="64"/>
+      <c r="AN1" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="AO1" s="65"/>
-      <c r="AP1" s="65"/>
-      <c r="AQ1" s="65"/>
-      <c r="AR1" s="65"/>
-      <c r="AS1" s="65"/>
-      <c r="AT1" s="65"/>
-      <c r="AU1" s="64" t="s">
+      <c r="AO1" s="64"/>
+      <c r="AP1" s="64"/>
+      <c r="AQ1" s="64"/>
+      <c r="AR1" s="64"/>
+      <c r="AS1" s="64"/>
+      <c r="AT1" s="64"/>
+      <c r="AU1" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="AV1" s="65"/>
-      <c r="AW1" s="65"/>
-      <c r="AX1" s="65"/>
-      <c r="AY1" s="65"/>
-      <c r="AZ1" s="65"/>
-      <c r="BA1" s="65"/>
-      <c r="BB1" s="64" t="s">
+      <c r="AV1" s="64"/>
+      <c r="AW1" s="64"/>
+      <c r="AX1" s="64"/>
+      <c r="AY1" s="64"/>
+      <c r="AZ1" s="64"/>
+      <c r="BA1" s="64"/>
+      <c r="BB1" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="BC1" s="65"/>
-      <c r="BD1" s="65"/>
-      <c r="BE1" s="65"/>
-      <c r="BF1" s="65"/>
-      <c r="BG1" s="65"/>
-      <c r="BH1" s="65"/>
-      <c r="BI1" s="64" t="s">
+      <c r="BC1" s="64"/>
+      <c r="BD1" s="64"/>
+      <c r="BE1" s="64"/>
+      <c r="BF1" s="64"/>
+      <c r="BG1" s="64"/>
+      <c r="BH1" s="64"/>
+      <c r="BI1" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="BJ1" s="65"/>
-      <c r="BK1" s="65"/>
-      <c r="BL1" s="65"/>
-      <c r="BM1" s="65"/>
-      <c r="BN1" s="65"/>
-      <c r="BO1" s="65"/>
-      <c r="BP1" s="64" t="s">
+      <c r="BJ1" s="64"/>
+      <c r="BK1" s="64"/>
+      <c r="BL1" s="64"/>
+      <c r="BM1" s="64"/>
+      <c r="BN1" s="64"/>
+      <c r="BO1" s="64"/>
+      <c r="BP1" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="BQ1" s="65"/>
-      <c r="BR1" s="65"/>
-      <c r="BS1" s="65"/>
-      <c r="BT1" s="65"/>
-      <c r="BU1" s="65"/>
-      <c r="BV1" s="65"/>
-      <c r="BW1" s="64" t="s">
+      <c r="BQ1" s="64"/>
+      <c r="BR1" s="64"/>
+      <c r="BS1" s="64"/>
+      <c r="BT1" s="64"/>
+      <c r="BU1" s="64"/>
+      <c r="BV1" s="64"/>
+      <c r="BW1" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="BX1" s="65"/>
-      <c r="BY1" s="65"/>
-      <c r="BZ1" s="65"/>
-      <c r="CA1" s="65"/>
-      <c r="CB1" s="65"/>
-      <c r="CC1" s="65"/>
-      <c r="CD1" s="64" t="s">
+      <c r="BX1" s="64"/>
+      <c r="BY1" s="64"/>
+      <c r="BZ1" s="64"/>
+      <c r="CA1" s="64"/>
+      <c r="CB1" s="64"/>
+      <c r="CC1" s="64"/>
+      <c r="CD1" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="CE1" s="65"/>
-      <c r="CF1" s="65"/>
-      <c r="CG1" s="65"/>
-      <c r="CH1" s="65"/>
-      <c r="CI1" s="65"/>
-      <c r="CJ1" s="65"/>
-      <c r="CK1" s="64" t="s">
+      <c r="CE1" s="64"/>
+      <c r="CF1" s="64"/>
+      <c r="CG1" s="64"/>
+      <c r="CH1" s="64"/>
+      <c r="CI1" s="64"/>
+      <c r="CJ1" s="64"/>
+      <c r="CK1" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="CL1" s="65"/>
-      <c r="CM1" s="65"/>
-      <c r="CN1" s="65"/>
-      <c r="CO1" s="65"/>
-      <c r="CP1" s="65"/>
-      <c r="CQ1" s="65"/>
-      <c r="CR1" s="64" t="s">
+      <c r="CL1" s="64"/>
+      <c r="CM1" s="64"/>
+      <c r="CN1" s="64"/>
+      <c r="CO1" s="64"/>
+      <c r="CP1" s="64"/>
+      <c r="CQ1" s="64"/>
+      <c r="CR1" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="CS1" s="65"/>
-      <c r="CT1" s="65"/>
-      <c r="CU1" s="65"/>
-      <c r="CV1" s="65"/>
-      <c r="CW1" s="65"/>
-      <c r="CX1" s="65"/>
-      <c r="CY1" s="64" t="s">
+      <c r="CS1" s="64"/>
+      <c r="CT1" s="64"/>
+      <c r="CU1" s="64"/>
+      <c r="CV1" s="64"/>
+      <c r="CW1" s="64"/>
+      <c r="CX1" s="64"/>
+      <c r="CY1" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="CZ1" s="65"/>
-      <c r="DA1" s="65"/>
-      <c r="DB1" s="65"/>
-      <c r="DC1" s="65"/>
-      <c r="DD1" s="65"/>
-      <c r="DE1" s="65"/>
-      <c r="DF1" s="64" t="s">
+      <c r="CZ1" s="64"/>
+      <c r="DA1" s="64"/>
+      <c r="DB1" s="64"/>
+      <c r="DC1" s="64"/>
+      <c r="DD1" s="64"/>
+      <c r="DE1" s="64"/>
+      <c r="DF1" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="DG1" s="65"/>
-      <c r="DH1" s="65"/>
-      <c r="DI1" s="65"/>
-      <c r="DJ1" s="65"/>
-      <c r="DK1" s="65"/>
-      <c r="DL1" s="65"/>
-      <c r="DM1" s="64" t="s">
+      <c r="DG1" s="64"/>
+      <c r="DH1" s="64"/>
+      <c r="DI1" s="64"/>
+      <c r="DJ1" s="64"/>
+      <c r="DK1" s="64"/>
+      <c r="DL1" s="64"/>
+      <c r="DM1" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="DN1" s="65"/>
-      <c r="DO1" s="65"/>
-      <c r="DP1" s="65"/>
-      <c r="DQ1" s="65"/>
-      <c r="DR1" s="65"/>
-      <c r="DS1" s="65"/>
-      <c r="DT1" s="64"/>
-      <c r="DU1" s="65"/>
-      <c r="DV1" s="65"/>
-      <c r="DW1" s="65"/>
-      <c r="DX1" s="65"/>
-      <c r="DY1" s="65"/>
-      <c r="DZ1" s="65"/>
-      <c r="EA1" s="64"/>
-      <c r="EB1" s="65"/>
-      <c r="EC1" s="65"/>
-      <c r="ED1" s="65"/>
-      <c r="EE1" s="65"/>
-      <c r="EF1" s="65"/>
-      <c r="EG1" s="65"/>
-      <c r="EH1" s="64"/>
-      <c r="EI1" s="65"/>
-      <c r="EJ1" s="65"/>
-      <c r="EK1" s="65"/>
-      <c r="EL1" s="65"/>
-      <c r="EM1" s="65"/>
-      <c r="EN1" s="65"/>
-      <c r="EO1" s="64"/>
-      <c r="EP1" s="65"/>
-      <c r="EQ1" s="65"/>
-      <c r="ER1" s="65"/>
-      <c r="ES1" s="65"/>
-      <c r="ET1" s="65"/>
-      <c r="EU1" s="65"/>
-      <c r="EV1" s="64"/>
-      <c r="EW1" s="65"/>
-      <c r="EX1" s="65"/>
-      <c r="EY1" s="65"/>
-      <c r="EZ1" s="65"/>
-      <c r="FA1" s="65"/>
-      <c r="FB1" s="65"/>
+      <c r="DN1" s="64"/>
+      <c r="DO1" s="64"/>
+      <c r="DP1" s="64"/>
+      <c r="DQ1" s="64"/>
+      <c r="DR1" s="64"/>
+      <c r="DS1" s="64"/>
+      <c r="DT1" s="63"/>
+      <c r="DU1" s="64"/>
+      <c r="DV1" s="64"/>
+      <c r="DW1" s="64"/>
+      <c r="DX1" s="64"/>
+      <c r="DY1" s="64"/>
+      <c r="DZ1" s="64"/>
+      <c r="EA1" s="63"/>
+      <c r="EB1" s="64"/>
+      <c r="EC1" s="64"/>
+      <c r="ED1" s="64"/>
+      <c r="EE1" s="64"/>
+      <c r="EF1" s="64"/>
+      <c r="EG1" s="64"/>
+      <c r="EH1" s="63"/>
+      <c r="EI1" s="64"/>
+      <c r="EJ1" s="64"/>
+      <c r="EK1" s="64"/>
+      <c r="EL1" s="64"/>
+      <c r="EM1" s="64"/>
+      <c r="EN1" s="64"/>
+      <c r="EO1" s="63"/>
+      <c r="EP1" s="64"/>
+      <c r="EQ1" s="64"/>
+      <c r="ER1" s="64"/>
+      <c r="ES1" s="64"/>
+      <c r="ET1" s="64"/>
+      <c r="EU1" s="64"/>
+      <c r="EV1" s="63"/>
+      <c r="EW1" s="64"/>
+      <c r="EX1" s="64"/>
+      <c r="EY1" s="64"/>
+      <c r="EZ1" s="64"/>
+      <c r="FA1" s="64"/>
+      <c r="FB1" s="64"/>
     </row>
     <row r="2" spans="1:158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
@@ -10114,13 +10114,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AN1:AT1"/>
-    <mergeCell ref="AU1:BA1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AM1"/>
     <mergeCell ref="EH1:EN1"/>
     <mergeCell ref="EO1:EU1"/>
     <mergeCell ref="EV1:FB1"/>
@@ -10136,6 +10129,13 @@
     <mergeCell ref="DM1:DS1"/>
     <mergeCell ref="DT1:DZ1"/>
     <mergeCell ref="EA1:EG1"/>
+    <mergeCell ref="AN1:AT1"/>
+    <mergeCell ref="AU1:BA1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update Ergebnisdokumentation zu React
</commit_message>
<xml_diff>
--- a/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
+++ b/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yara\Dropbox\Studium\Semester 6\FRONT\FRONT_Projekt\front-projekt\documents\Projektmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757C826E-AB07-4BEF-ACD8-5FA040663AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB604981-B83D-440E-A136-FD2AACE46CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1209,13 +1209,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="180"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1449,7 +1449,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H69" sqref="H69"/>
+      <selection pane="bottomLeft" activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1584,7 +1584,7 @@
       </c>
       <c r="H6" s="30">
         <f>SUM(H10:H74)</f>
-        <v>67.25</v>
+        <v>67.5</v>
       </c>
       <c r="I6" s="27">
         <f>SUM(I10:I74)</f>
@@ -1620,7 +1620,7 @@
       </c>
       <c r="H7" s="30">
         <f t="shared" ref="H7:J7" si="1">H5-H6</f>
-        <v>52.75</v>
+        <v>52.5</v>
       </c>
       <c r="I7" s="27">
         <f t="shared" si="1"/>
@@ -3329,7 +3329,7 @@
         <v>251</v>
       </c>
       <c r="H67" s="22">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="I67" s="22"/>
       <c r="J67" s="22">
@@ -3569,51 +3569,51 @@
   <sheetData>
     <row r="1" spans="1:166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C1" s="1"/>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="66" t="s">
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="66" t="s">
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="67"/>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="66" t="s">
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="67"/>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="66" t="s">
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="AH1" s="67"/>
-      <c r="AI1" s="67"/>
-      <c r="AJ1" s="67"/>
-      <c r="AK1" s="67"/>
-      <c r="AL1" s="67"/>
-      <c r="AM1" s="67"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="66"/>
+      <c r="AJ1" s="66"/>
+      <c r="AK1" s="66"/>
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
       <c r="AN1" s="63" t="s">
         <v>5</v>
       </c>
@@ -5178,7 +5178,7 @@
     </row>
     <row r="46" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
-      <c r="B46" s="65" t="s">
+      <c r="B46" s="67" t="s">
         <v>54</v>
       </c>
       <c r="C46" s="15" t="s">
@@ -5187,21 +5187,21 @@
     </row>
     <row r="47" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
-      <c r="B47" s="65"/>
+      <c r="B47" s="67"/>
       <c r="C47" s="15" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
-      <c r="B48" s="65"/>
+      <c r="B48" s="67"/>
       <c r="C48" s="15" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:71" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
-      <c r="B49" s="65"/>
+      <c r="B49" s="67"/>
       <c r="C49" s="15" t="s">
         <v>224</v>
       </c>
@@ -5211,211 +5211,211 @@
     </row>
     <row r="50" spans="1:71" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A50" s="6"/>
-      <c r="B50" s="65"/>
+      <c r="B50" s="67"/>
       <c r="C50" s="15" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:71" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
-      <c r="B51" s="65"/>
+      <c r="B51" s="67"/>
       <c r="C51" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:71" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B52" s="65"/>
+      <c r="B52" s="67"/>
       <c r="C52" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:71" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B53" s="65"/>
+      <c r="B53" s="67"/>
       <c r="C53" s="15" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:71" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A54" s="6"/>
-      <c r="B54" s="65"/>
+      <c r="B54" s="67"/>
       <c r="C54" s="15" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:71" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A55" s="6"/>
-      <c r="B55" s="65"/>
+      <c r="B55" s="67"/>
       <c r="C55" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:71" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A56" s="6"/>
-      <c r="B56" s="65"/>
+      <c r="B56" s="67"/>
       <c r="C56" s="15" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:71" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A57" s="6"/>
-      <c r="B57" s="65"/>
+      <c r="B57" s="67"/>
       <c r="C57" s="15" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="65"/>
+      <c r="B58" s="67"/>
       <c r="C58" s="15" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:71" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B59" s="65"/>
+      <c r="B59" s="67"/>
       <c r="C59" s="15" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="60" spans="1:71" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B60" s="65"/>
+      <c r="B60" s="67"/>
       <c r="C60" s="15" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="61" spans="1:71" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B61" s="65"/>
+      <c r="B61" s="67"/>
       <c r="C61" s="15" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:71" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B62" s="65"/>
+      <c r="B62" s="67"/>
       <c r="C62" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:71" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B63" s="65"/>
+      <c r="B63" s="67"/>
       <c r="C63" s="15" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:71" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B64" s="65"/>
+      <c r="B64" s="67"/>
       <c r="C64" s="15"/>
     </row>
     <row r="65" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B65" s="65"/>
+      <c r="B65" s="67"/>
       <c r="C65" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="66" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B66" s="65"/>
+      <c r="B66" s="67"/>
       <c r="C66" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="67" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B67" s="65"/>
+      <c r="B67" s="67"/>
       <c r="C67" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="68" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B68" s="65"/>
+      <c r="B68" s="67"/>
       <c r="C68" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="69" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B69" s="65"/>
+      <c r="B69" s="67"/>
       <c r="C69" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="70" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B70" s="65"/>
+      <c r="B70" s="67"/>
       <c r="C70" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="71" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B71" s="65"/>
+      <c r="B71" s="67"/>
       <c r="C71" s="15" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="72" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B72" s="65"/>
+      <c r="B72" s="67"/>
       <c r="C72" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="73" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B73" s="65"/>
+      <c r="B73" s="67"/>
       <c r="C73" s="15" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="74" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B74" s="65"/>
+      <c r="B74" s="67"/>
       <c r="C74" s="16"/>
     </row>
     <row r="75" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B75" s="65"/>
+      <c r="B75" s="67"/>
       <c r="C75" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="76" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B76" s="65"/>
+      <c r="B76" s="67"/>
       <c r="C76" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="77" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B77" s="65"/>
+      <c r="B77" s="67"/>
       <c r="C77" s="15" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="78" spans="2:53" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B78" s="65"/>
+      <c r="B78" s="67"/>
       <c r="C78" s="15" t="s">
         <v>72</v>
       </c>
       <c r="BA78" s="6"/>
     </row>
     <row r="79" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B79" s="65"/>
+      <c r="B79" s="67"/>
       <c r="C79" s="16"/>
     </row>
     <row r="80" spans="2:53" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B80" s="65"/>
+      <c r="B80" s="67"/>
       <c r="C80" s="15" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="81" spans="2:75" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B81" s="65"/>
+      <c r="B81" s="67"/>
       <c r="C81" s="60" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="82" spans="2:75" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B82" s="65"/>
+      <c r="B82" s="67"/>
       <c r="C82" s="60" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="83" spans="2:75" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B83" s="65"/>
+      <c r="B83" s="67"/>
       <c r="C83" s="60" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="84" spans="2:75" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B84" s="65"/>
+      <c r="B84" s="67"/>
       <c r="C84" s="15" t="s">
         <v>258</v>
       </c>
@@ -8170,6 +8170,10 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B79:B84"/>
+    <mergeCell ref="B46:B78"/>
+    <mergeCell ref="CK1:CQ1"/>
+    <mergeCell ref="CR1:CX1"/>
     <mergeCell ref="CY1:DE1"/>
     <mergeCell ref="E1:K1"/>
     <mergeCell ref="L1:R1"/>
@@ -8183,10 +8187,6 @@
     <mergeCell ref="BP1:BV1"/>
     <mergeCell ref="BW1:CC1"/>
     <mergeCell ref="CD1:CJ1"/>
-    <mergeCell ref="B79:B84"/>
-    <mergeCell ref="B46:B78"/>
-    <mergeCell ref="CK1:CQ1"/>
-    <mergeCell ref="CR1:CX1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:J4 L4:CW4 CY4:EV4">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
@@ -10114,6 +10114,13 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="AN1:AT1"/>
+    <mergeCell ref="AU1:BA1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AM1"/>
     <mergeCell ref="EH1:EN1"/>
     <mergeCell ref="EO1:EU1"/>
     <mergeCell ref="EV1:FB1"/>
@@ -10129,13 +10136,6 @@
     <mergeCell ref="DM1:DS1"/>
     <mergeCell ref="DT1:DZ1"/>
     <mergeCell ref="EA1:EG1"/>
-    <mergeCell ref="AN1:AT1"/>
-    <mergeCell ref="AU1:BA1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Einführung des Tauschfeldes (timing funktioniert aber noch nicht)
</commit_message>
<xml_diff>
--- a/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
+++ b/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annastaub/Library/Mobile Documents/com~apple~CloudDocs/FHGR/23 FS/Frontend Development 2/Frontend Development 1/front-projekt/documents/Projektmanagement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32FD5DF-9476-CF44-9627-39BE48471169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AF34CA-3B70-8A4B-BA77-DE0ED0676335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22160" yWindow="500" windowWidth="29040" windowHeight="17800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="500" windowWidth="40200" windowHeight="25140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitbudget" sheetId="4" r:id="rId1"/>
@@ -1208,13 +1208,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="180"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1447,8 +1447,8 @@
   <dimension ref="A1:V78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I50" sqref="I50"/>
+      <pane ySplit="7" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1583,15 +1583,15 @@
       </c>
       <c r="H6" s="30">
         <f>SUM(H10:H74)</f>
-        <v>67.5</v>
+        <v>69.5</v>
       </c>
       <c r="I6" s="27">
         <f>SUM(I10:I74)</f>
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="J6" s="28">
         <f>SUM(J10:J74)</f>
-        <v>60.5</v>
+        <v>62.5</v>
       </c>
       <c r="K6" s="22"/>
       <c r="L6" s="22"/>
@@ -1619,15 +1619,15 @@
       </c>
       <c r="H7" s="30">
         <f t="shared" ref="H7:J7" si="1">H5-H6</f>
-        <v>52.5</v>
+        <v>50.5</v>
       </c>
       <c r="I7" s="27">
         <f t="shared" si="1"/>
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J7" s="28">
         <f t="shared" si="1"/>
-        <v>59.5</v>
+        <v>57.5</v>
       </c>
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
@@ -2861,10 +2861,14 @@
         <v>209</v>
       </c>
       <c r="H50" s="22">
-        <v>2</v>
-      </c>
-      <c r="I50" s="22"/>
-      <c r="J50" s="22"/>
+        <v>3</v>
+      </c>
+      <c r="I50" s="22">
+        <v>4</v>
+      </c>
+      <c r="J50" s="22">
+        <v>1</v>
+      </c>
       <c r="K50" s="22"/>
       <c r="L50" s="22"/>
     </row>
@@ -3336,11 +3340,13 @@
         <v>251</v>
       </c>
       <c r="H67" s="22">
+        <v>2</v>
+      </c>
+      <c r="I67" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="J67" s="22">
         <v>1.5</v>
-      </c>
-      <c r="I67" s="22"/>
-      <c r="J67" s="22">
-        <v>1</v>
       </c>
       <c r="K67" s="22"/>
       <c r="L67" s="22"/>
@@ -3366,10 +3372,14 @@
         <v>252</v>
       </c>
       <c r="H68" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="I68" s="22"/>
-      <c r="J68" s="22"/>
+        <v>2</v>
+      </c>
+      <c r="I68" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="J68" s="22">
+        <v>0.5</v>
+      </c>
       <c r="K68" s="22"/>
       <c r="L68" s="22"/>
     </row>
@@ -3576,51 +3586,51 @@
   <sheetData>
     <row r="1" spans="1:166" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C1" s="1"/>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="64" t="s">
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="64" t="s">
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="64" t="s">
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="65"/>
-      <c r="AC1" s="65"/>
-      <c r="AD1" s="65"/>
-      <c r="AE1" s="65"/>
-      <c r="AF1" s="65"/>
-      <c r="AG1" s="64" t="s">
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="AH1" s="65"/>
-      <c r="AI1" s="65"/>
-      <c r="AJ1" s="65"/>
-      <c r="AK1" s="65"/>
-      <c r="AL1" s="65"/>
-      <c r="AM1" s="65"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="66"/>
+      <c r="AJ1" s="66"/>
+      <c r="AK1" s="66"/>
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
       <c r="AN1" s="62" t="s">
         <v>5</v>
       </c>
@@ -5185,7 +5195,7 @@
     </row>
     <row r="46" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="6"/>
-      <c r="B46" s="66" t="s">
+      <c r="B46" s="64" t="s">
         <v>54</v>
       </c>
       <c r="C46" s="15" t="s">
@@ -5194,21 +5204,21 @@
     </row>
     <row r="47" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="6"/>
-      <c r="B47" s="66"/>
+      <c r="B47" s="64"/>
       <c r="C47" s="15" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="6"/>
-      <c r="B48" s="66"/>
+      <c r="B48" s="64"/>
       <c r="C48" s="15" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:71" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" s="6"/>
-      <c r="B49" s="66"/>
+      <c r="B49" s="64"/>
       <c r="C49" s="15" t="s">
         <v>224</v>
       </c>
@@ -5218,211 +5228,211 @@
     </row>
     <row r="50" spans="1:71" ht="14" x14ac:dyDescent="0.15">
       <c r="A50" s="6"/>
-      <c r="B50" s="66"/>
+      <c r="B50" s="64"/>
       <c r="C50" s="15" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:71" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" s="6"/>
-      <c r="B51" s="66"/>
+      <c r="B51" s="64"/>
       <c r="C51" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:71" ht="13" x14ac:dyDescent="0.15">
-      <c r="B52" s="66"/>
+      <c r="B52" s="64"/>
       <c r="C52" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:71" ht="13" x14ac:dyDescent="0.15">
-      <c r="B53" s="66"/>
+      <c r="B53" s="64"/>
       <c r="C53" s="15" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:71" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="6"/>
-      <c r="B54" s="66"/>
+      <c r="B54" s="64"/>
       <c r="C54" s="15" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:71" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="6"/>
-      <c r="B55" s="66"/>
+      <c r="B55" s="64"/>
       <c r="C55" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:71" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" s="6"/>
-      <c r="B56" s="66"/>
+      <c r="B56" s="64"/>
       <c r="C56" s="15" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:71" ht="14" x14ac:dyDescent="0.15">
       <c r="A57" s="6"/>
-      <c r="B57" s="66"/>
+      <c r="B57" s="64"/>
       <c r="C57" s="15" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B58" s="66"/>
+      <c r="B58" s="64"/>
       <c r="C58" s="15" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:71" ht="13" x14ac:dyDescent="0.15">
-      <c r="B59" s="66"/>
+      <c r="B59" s="64"/>
       <c r="C59" s="15" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="60" spans="1:71" ht="13" x14ac:dyDescent="0.15">
-      <c r="B60" s="66"/>
+      <c r="B60" s="64"/>
       <c r="C60" s="15" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="61" spans="1:71" ht="13" x14ac:dyDescent="0.15">
-      <c r="B61" s="66"/>
+      <c r="B61" s="64"/>
       <c r="C61" s="15" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:71" ht="13" x14ac:dyDescent="0.15">
-      <c r="B62" s="66"/>
+      <c r="B62" s="64"/>
       <c r="C62" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:71" ht="13" x14ac:dyDescent="0.15">
-      <c r="B63" s="66"/>
+      <c r="B63" s="64"/>
       <c r="C63" s="15" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:71" ht="13" x14ac:dyDescent="0.15">
-      <c r="B64" s="66"/>
+      <c r="B64" s="64"/>
       <c r="C64" s="15"/>
     </row>
     <row r="65" spans="2:53" ht="13" x14ac:dyDescent="0.15">
-      <c r="B65" s="66"/>
+      <c r="B65" s="64"/>
       <c r="C65" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="66" spans="2:53" ht="13" x14ac:dyDescent="0.15">
-      <c r="B66" s="66"/>
+      <c r="B66" s="64"/>
       <c r="C66" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="67" spans="2:53" ht="13" x14ac:dyDescent="0.15">
-      <c r="B67" s="66"/>
+      <c r="B67" s="64"/>
       <c r="C67" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="68" spans="2:53" ht="13" x14ac:dyDescent="0.15">
-      <c r="B68" s="66"/>
+      <c r="B68" s="64"/>
       <c r="C68" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="69" spans="2:53" ht="13" x14ac:dyDescent="0.15">
-      <c r="B69" s="66"/>
+      <c r="B69" s="64"/>
       <c r="C69" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="70" spans="2:53" ht="13" x14ac:dyDescent="0.15">
-      <c r="B70" s="66"/>
+      <c r="B70" s="64"/>
       <c r="C70" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="71" spans="2:53" ht="13" x14ac:dyDescent="0.15">
-      <c r="B71" s="66"/>
+      <c r="B71" s="64"/>
       <c r="C71" s="15" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="72" spans="2:53" ht="13" x14ac:dyDescent="0.15">
-      <c r="B72" s="66"/>
+      <c r="B72" s="64"/>
       <c r="C72" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="73" spans="2:53" ht="13" x14ac:dyDescent="0.15">
-      <c r="B73" s="66"/>
+      <c r="B73" s="64"/>
       <c r="C73" s="15" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="74" spans="2:53" ht="13" x14ac:dyDescent="0.15">
-      <c r="B74" s="66"/>
+      <c r="B74" s="64"/>
       <c r="C74" s="16"/>
     </row>
     <row r="75" spans="2:53" ht="13" x14ac:dyDescent="0.15">
-      <c r="B75" s="66"/>
+      <c r="B75" s="64"/>
       <c r="C75" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="76" spans="2:53" ht="13" x14ac:dyDescent="0.15">
-      <c r="B76" s="66"/>
+      <c r="B76" s="64"/>
       <c r="C76" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="77" spans="2:53" ht="13" x14ac:dyDescent="0.15">
-      <c r="B77" s="66"/>
+      <c r="B77" s="64"/>
       <c r="C77" s="15" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="78" spans="2:53" ht="14" x14ac:dyDescent="0.15">
-      <c r="B78" s="66"/>
+      <c r="B78" s="64"/>
       <c r="C78" s="15" t="s">
         <v>72</v>
       </c>
       <c r="BA78" s="6"/>
     </row>
     <row r="79" spans="2:53" ht="13" x14ac:dyDescent="0.15">
-      <c r="B79" s="66"/>
+      <c r="B79" s="64"/>
       <c r="C79" s="16"/>
     </row>
     <row r="80" spans="2:53" ht="13" x14ac:dyDescent="0.15">
-      <c r="B80" s="66"/>
+      <c r="B80" s="64"/>
       <c r="C80" s="15" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="81" spans="2:75" ht="13" x14ac:dyDescent="0.15">
-      <c r="B81" s="66"/>
+      <c r="B81" s="64"/>
       <c r="C81" s="59" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="82" spans="2:75" ht="13" x14ac:dyDescent="0.15">
-      <c r="B82" s="66"/>
+      <c r="B82" s="64"/>
       <c r="C82" s="59" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="83" spans="2:75" ht="13" x14ac:dyDescent="0.15">
-      <c r="B83" s="66"/>
+      <c r="B83" s="64"/>
       <c r="C83" s="59" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="84" spans="2:75" ht="13" x14ac:dyDescent="0.15">
-      <c r="B84" s="66"/>
+      <c r="B84" s="64"/>
       <c r="C84" s="15" t="s">
         <v>258</v>
       </c>
@@ -8177,10 +8187,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B79:B84"/>
-    <mergeCell ref="B46:B78"/>
-    <mergeCell ref="CK1:CQ1"/>
-    <mergeCell ref="CR1:CX1"/>
     <mergeCell ref="CY1:DE1"/>
     <mergeCell ref="E1:K1"/>
     <mergeCell ref="L1:R1"/>
@@ -8194,6 +8200,10 @@
     <mergeCell ref="BP1:BV1"/>
     <mergeCell ref="BW1:CC1"/>
     <mergeCell ref="CD1:CJ1"/>
+    <mergeCell ref="B79:B84"/>
+    <mergeCell ref="B46:B78"/>
+    <mergeCell ref="CK1:CQ1"/>
+    <mergeCell ref="CR1:CX1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:J4 L4:CW4 CY4:EV4">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">

</xml_diff>

<commit_message>
Eingabewerte von Startseite in SessionStorage speichern
</commit_message>
<xml_diff>
--- a/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
+++ b/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Besitzer\Dropbox\Studium\Semester 6\FRONT\FRONT_Projekt\front-projekt\documents\Projektmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAA2072-EE14-43C3-BC00-F5EF107ECB52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B578B5-B204-4091-873B-726D2C92E1FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="263">
   <si>
     <t>17. Oktober 2022</t>
   </si>
@@ -814,6 +814,15 @@
   </si>
   <si>
     <t>8.4 Präsentation</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>5.4.4.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        5.4.4 Storage</t>
   </si>
 </sst>
 </file>
@@ -1204,6 +1213,9 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1212,9 +1224,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="180"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1444,11 +1453,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F6C6EE-1E63-4549-8E9D-BCD03E80ADE4}">
-  <dimension ref="A1:V78"/>
+  <dimension ref="A1:V79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40:XFD40"/>
+      <pane ySplit="7" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1566,31 +1575,31 @@
         <v>109</v>
       </c>
       <c r="C6" s="30">
-        <f>SUM(C10:C69)</f>
-        <v>117.5</v>
+        <f>SUM(C10:C70)</f>
+        <v>118.5</v>
       </c>
       <c r="D6" s="27">
-        <f>SUM(D10:D69)</f>
-        <v>117</v>
+        <f>SUM(D10:D70)</f>
+        <v>118</v>
       </c>
       <c r="E6" s="28">
-        <f>SUM(E10:E69)</f>
-        <v>118</v>
+        <f>SUM(E10:E70)</f>
+        <v>119</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="31" t="s">
         <v>110</v>
       </c>
       <c r="H6" s="30">
-        <f>SUM(H10:H74)</f>
-        <v>70.25</v>
+        <f>SUM(H10:H75)</f>
+        <v>71.5</v>
       </c>
       <c r="I6" s="27">
-        <f>SUM(I10:I74)</f>
+        <f>SUM(I10:I75)</f>
         <v>66</v>
       </c>
       <c r="J6" s="28">
-        <f>SUM(J10:J74)</f>
+        <f>SUM(J10:J75)</f>
         <v>62.5</v>
       </c>
       <c r="K6" s="22"/>
@@ -1603,15 +1612,15 @@
       </c>
       <c r="C7" s="30">
         <f t="shared" ref="C7:E7" si="0">C5-C6</f>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="D7" s="27">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" s="28">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="31" t="s">
@@ -1619,7 +1628,7 @@
       </c>
       <c r="H7" s="30">
         <f t="shared" ref="H7:J7" si="1">H5-H6</f>
-        <v>49.75</v>
+        <v>48.5</v>
       </c>
       <c r="I7" s="27">
         <f t="shared" si="1"/>
@@ -2599,7 +2608,7 @@
         <v>201</v>
       </c>
       <c r="H40" s="22">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="I40" s="22"/>
       <c r="J40" s="22"/>
@@ -2806,7 +2815,9 @@
       <c r="G48" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="H48" s="22"/>
+      <c r="H48" s="22">
+        <v>0.5</v>
+      </c>
       <c r="I48" s="22"/>
       <c r="J48" s="22"/>
       <c r="K48" s="22"/>
@@ -2928,25 +2939,27 @@
     </row>
     <row r="53" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A53" s="22" t="s">
-        <v>155</v>
+        <v>260</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>156</v>
+        <v>261</v>
       </c>
       <c r="C53" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D53" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E53" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" s="22"/>
       <c r="G53" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="H53" s="22"/>
+        <v>261</v>
+      </c>
+      <c r="H53" s="22">
+        <v>0.5</v>
+      </c>
       <c r="I53" s="22"/>
       <c r="J53" s="22"/>
       <c r="K53" s="22"/>
@@ -2954,23 +2967,23 @@
     </row>
     <row r="54" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A54" s="22" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C54" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D54" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E54" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F54" s="22"/>
       <c r="G54" s="22" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H54" s="22"/>
       <c r="I54" s="22"/>
@@ -2980,66 +2993,64 @@
     </row>
     <row r="55" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A55" s="22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C55" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E55" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55" s="22"/>
       <c r="G55" s="22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H55" s="22"/>
       <c r="I55" s="22"/>
-      <c r="J55" s="22">
-        <v>0.5</v>
-      </c>
+      <c r="J55" s="22"/>
       <c r="K55" s="22"/>
       <c r="L55" s="22"/>
     </row>
     <row r="56" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A56" s="22" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C56" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D56" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E56" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" s="22"/>
       <c r="G56" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="H56" s="22">
-        <v>0.25</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="H56" s="22"/>
       <c r="I56" s="22"/>
-      <c r="J56" s="22"/>
+      <c r="J56" s="22">
+        <v>0.5</v>
+      </c>
       <c r="K56" s="22"/>
       <c r="L56" s="22"/>
     </row>
     <row r="57" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A57" s="22" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B57" s="22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C57" s="22">
         <v>2</v>
@@ -3052,61 +3063,63 @@
       </c>
       <c r="F57" s="22"/>
       <c r="G57" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="H57" s="22"/>
+        <v>162</v>
+      </c>
+      <c r="H57" s="22">
+        <v>0.25</v>
+      </c>
       <c r="I57" s="22"/>
-      <c r="J57" s="22">
-        <v>0.25</v>
-      </c>
+      <c r="J57" s="22"/>
       <c r="K57" s="22"/>
       <c r="L57" s="22"/>
     </row>
     <row r="58" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A58" s="22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C58" s="22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D58" s="22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E58" s="22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F58" s="22"/>
       <c r="G58" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H58" s="22"/>
       <c r="I58" s="22"/>
-      <c r="J58" s="22"/>
+      <c r="J58" s="22">
+        <v>0.25</v>
+      </c>
       <c r="K58" s="22"/>
       <c r="L58" s="22"/>
     </row>
     <row r="59" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A59" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C59" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D59" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E59" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F59" s="22"/>
       <c r="G59" s="22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H59" s="22"/>
       <c r="I59" s="22"/>
@@ -3116,42 +3129,39 @@
     </row>
     <row r="60" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A60" s="22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C60" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D60" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E60" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F60" s="22"/>
       <c r="G60" s="22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H60" s="22"/>
       <c r="I60" s="22"/>
       <c r="J60" s="22"/>
       <c r="K60" s="22"/>
       <c r="L60" s="22"/>
-      <c r="T60" s="22"/>
-      <c r="U60" s="22"/>
-      <c r="V60" s="22"/>
     </row>
     <row r="61" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A61" s="22" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C61" s="22">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="D61" s="22">
         <v>0</v>
@@ -3161,17 +3171,11 @@
       </c>
       <c r="F61" s="22"/>
       <c r="G61" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="H61" s="22">
-        <v>0</v>
-      </c>
-      <c r="I61" s="22">
-        <v>0</v>
-      </c>
-      <c r="J61" s="22">
-        <v>0.25</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="H61" s="22"/>
+      <c r="I61" s="22"/>
+      <c r="J61" s="22"/>
       <c r="K61" s="22"/>
       <c r="L61" s="22"/>
       <c r="T61" s="22"/>
@@ -3180,13 +3184,13 @@
     </row>
     <row r="62" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A62" s="22" t="s">
-        <v>101</v>
+        <v>171</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C62" s="22">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D62" s="22">
         <v>0</v>
@@ -3196,11 +3200,17 @@
       </c>
       <c r="F62" s="22"/>
       <c r="G62" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="H62" s="22"/>
-      <c r="I62" s="22"/>
-      <c r="J62" s="22"/>
+        <v>172</v>
+      </c>
+      <c r="H62" s="22">
+        <v>0</v>
+      </c>
+      <c r="I62" s="22">
+        <v>0</v>
+      </c>
+      <c r="J62" s="22">
+        <v>0.25</v>
+      </c>
       <c r="K62" s="22"/>
       <c r="L62" s="22"/>
       <c r="T62" s="22"/>
@@ -3209,10 +3219,10 @@
     </row>
     <row r="63" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A63" s="22" t="s">
-        <v>174</v>
+        <v>101</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C63" s="22">
         <v>0</v>
@@ -3221,11 +3231,11 @@
         <v>0</v>
       </c>
       <c r="E63" s="22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F63" s="22"/>
       <c r="G63" s="22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H63" s="22"/>
       <c r="I63" s="22"/>
@@ -3238,23 +3248,23 @@
     </row>
     <row r="64" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A64" s="22" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C64" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D64" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F64" s="22"/>
       <c r="G64" s="22" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H64" s="22"/>
       <c r="I64" s="22"/>
@@ -3265,12 +3275,12 @@
       <c r="U64" s="22"/>
       <c r="V64" s="22"/>
     </row>
-    <row r="65" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A65" s="22" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C65" s="22">
         <v>1</v>
@@ -3283,50 +3293,49 @@
       </c>
       <c r="F65" s="22"/>
       <c r="G65" s="22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H65" s="22"/>
       <c r="I65" s="22"/>
       <c r="J65" s="22"/>
       <c r="K65" s="22"/>
       <c r="L65" s="22"/>
-    </row>
-    <row r="66" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="T65" s="22"/>
+      <c r="U65" s="22"/>
+      <c r="V65" s="22"/>
+    </row>
+    <row r="66" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A66" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="B66" s="47" t="s">
-        <v>250</v>
+        <v>178</v>
+      </c>
+      <c r="B66" s="22" t="s">
+        <v>179</v>
       </c>
       <c r="C66" s="22">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D66" s="22">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E66" s="22">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="F66" s="22"/>
-      <c r="G66" s="47" t="s">
-        <v>250</v>
-      </c>
-      <c r="H66" s="22">
-        <v>2.5</v>
-      </c>
+      <c r="G66" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="H66" s="22"/>
       <c r="I66" s="22"/>
-      <c r="J66" s="22">
-        <v>1.5</v>
-      </c>
+      <c r="J66" s="22"/>
       <c r="K66" s="22"/>
       <c r="L66" s="22"/>
     </row>
-    <row r="67" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A67" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="B67" s="22" t="s">
-        <v>251</v>
+        <v>245</v>
+      </c>
+      <c r="B67" s="47" t="s">
+        <v>250</v>
       </c>
       <c r="C67" s="22">
         <v>1.5</v>
@@ -3338,40 +3347,38 @@
         <v>1.5</v>
       </c>
       <c r="F67" s="22"/>
-      <c r="G67" s="22" t="s">
-        <v>251</v>
+      <c r="G67" s="47" t="s">
+        <v>250</v>
       </c>
       <c r="H67" s="22">
-        <v>2</v>
-      </c>
-      <c r="I67" s="22">
-        <v>0.5</v>
-      </c>
+        <v>2.5</v>
+      </c>
+      <c r="I67" s="22"/>
       <c r="J67" s="22">
         <v>1.5</v>
       </c>
       <c r="K67" s="22"/>
       <c r="L67" s="22"/>
     </row>
-    <row r="68" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A68" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C68" s="22">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D68" s="22">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E68" s="22">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F68" s="22"/>
       <c r="G68" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H68" s="22">
         <v>2</v>
@@ -3380,17 +3387,17 @@
         <v>0.5</v>
       </c>
       <c r="J68" s="22">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="K68" s="22"/>
       <c r="L68" s="22"/>
     </row>
-    <row r="69" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A69" s="22" t="s">
-        <v>99</v>
+        <v>247</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C69" s="22">
         <v>2</v>
@@ -3403,29 +3410,47 @@
       </c>
       <c r="F69" s="22"/>
       <c r="G69" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="H69" s="22"/>
-      <c r="I69" s="22"/>
-      <c r="J69" s="22"/>
+        <v>252</v>
+      </c>
+      <c r="H69" s="22">
+        <v>2</v>
+      </c>
+      <c r="I69" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="J69" s="22">
+        <v>0.5</v>
+      </c>
       <c r="K69" s="22"/>
       <c r="L69" s="22"/>
     </row>
-    <row r="70" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="22"/>
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="22"/>
-      <c r="E70" s="22"/>
+    <row r="70" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A70" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B70" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="C70" s="22">
+        <v>2</v>
+      </c>
+      <c r="D70" s="22">
+        <v>2</v>
+      </c>
+      <c r="E70" s="22">
+        <v>2</v>
+      </c>
       <c r="F70" s="22"/>
-      <c r="G70" s="22"/>
+      <c r="G70" s="22" t="s">
+        <v>253</v>
+      </c>
       <c r="H70" s="22"/>
       <c r="I70" s="22"/>
       <c r="J70" s="22"/>
       <c r="K70" s="22"/>
       <c r="L70" s="22"/>
     </row>
-    <row r="71" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A71" s="22"/>
       <c r="B71" s="22"/>
       <c r="C71" s="22"/>
@@ -3439,10 +3464,8 @@
       <c r="K71" s="22"/>
       <c r="L71" s="22"/>
     </row>
-    <row r="72" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="22" t="s">
-        <v>242</v>
-      </c>
+    <row r="72" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="22"/>
       <c r="B72" s="22"/>
       <c r="C72" s="22"/>
       <c r="D72" s="22"/>
@@ -3455,8 +3478,10 @@
       <c r="K72" s="22"/>
       <c r="L72" s="22"/>
     </row>
-    <row r="73" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="22"/>
+    <row r="73" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="22" t="s">
+        <v>242</v>
+      </c>
       <c r="B73" s="22"/>
       <c r="C73" s="22"/>
       <c r="D73" s="22"/>
@@ -3469,57 +3494,55 @@
       <c r="K73" s="22"/>
       <c r="L73" s="22"/>
     </row>
-    <row r="74" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="57" t="s">
-        <v>243</v>
-      </c>
-      <c r="B74" s="57" t="s">
-        <v>154</v>
-      </c>
-      <c r="C74" s="57">
-        <v>7</v>
-      </c>
-      <c r="D74" s="57">
-        <v>7</v>
-      </c>
-      <c r="E74" s="57">
-        <v>7</v>
-      </c>
-      <c r="F74" s="57"/>
-      <c r="G74" s="57" t="s">
-        <v>154</v>
-      </c>
-      <c r="H74" s="57">
-        <v>5.5</v>
-      </c>
-      <c r="I74" s="57">
-        <v>3.25</v>
-      </c>
-      <c r="J74" s="57">
-        <v>3.5</v>
-      </c>
+    <row r="74" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="22"/>
+      <c r="B74" s="22"/>
+      <c r="C74" s="22"/>
+      <c r="D74" s="22"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="22"/>
+      <c r="G74" s="22"/>
+      <c r="H74" s="22"/>
+      <c r="I74" s="22"/>
+      <c r="J74" s="22"/>
       <c r="K74" s="22"/>
       <c r="L74" s="22"/>
     </row>
-    <row r="75" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="22"/>
-      <c r="B75" s="47"/>
-      <c r="C75" s="22"/>
-      <c r="D75" s="22"/>
-      <c r="E75" s="22"/>
-      <c r="F75" s="22"/>
-      <c r="G75" s="22"/>
-      <c r="H75" s="22"/>
-      <c r="I75" s="22"/>
-      <c r="J75" s="22"/>
+    <row r="75" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A75" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="B75" s="57" t="s">
+        <v>154</v>
+      </c>
+      <c r="C75" s="57">
+        <v>7</v>
+      </c>
+      <c r="D75" s="57">
+        <v>7</v>
+      </c>
+      <c r="E75" s="57">
+        <v>7</v>
+      </c>
+      <c r="F75" s="57"/>
+      <c r="G75" s="57" t="s">
+        <v>154</v>
+      </c>
+      <c r="H75" s="57">
+        <v>5.5</v>
+      </c>
+      <c r="I75" s="57">
+        <v>3.25</v>
+      </c>
+      <c r="J75" s="57">
+        <v>3.5</v>
+      </c>
       <c r="K75" s="22"/>
       <c r="L75" s="22"/>
     </row>
-    <row r="76" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="57" t="s">
-        <v>244</v>
-      </c>
-      <c r="B76" s="22"/>
+    <row r="76" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A76" s="22"/>
+      <c r="B76" s="47"/>
       <c r="C76" s="22"/>
       <c r="D76" s="22"/>
       <c r="E76" s="22"/>
@@ -3531,8 +3554,10 @@
       <c r="K76" s="22"/>
       <c r="L76" s="22"/>
     </row>
-    <row r="77" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A77" s="22"/>
+    <row r="77" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A77" s="57" t="s">
+        <v>244</v>
+      </c>
       <c r="B77" s="22"/>
       <c r="C77" s="22"/>
       <c r="D77" s="22"/>
@@ -3542,8 +3567,10 @@
       <c r="H77" s="22"/>
       <c r="I77" s="22"/>
       <c r="J77" s="22"/>
-    </row>
-    <row r="78" spans="1:12" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="K77" s="22"/>
+      <c r="L77" s="22"/>
+    </row>
+    <row r="78" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A78" s="22"/>
       <c r="B78" s="22"/>
       <c r="C78" s="22"/>
@@ -3554,6 +3581,18 @@
       <c r="H78" s="22"/>
       <c r="I78" s="22"/>
       <c r="J78" s="22"/>
+    </row>
+    <row r="79" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A79" s="22"/>
+      <c r="B79" s="22"/>
+      <c r="C79" s="22"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="22"/>
+      <c r="F79" s="22"/>
+      <c r="G79" s="22"/>
+      <c r="H79" s="22"/>
+      <c r="I79" s="22"/>
+      <c r="J79" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3566,13 +3605,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:FJ999"/>
+  <dimension ref="A1:FJ1000"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="BV17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="BV38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C80" sqref="C80:C84"/>
+      <selection pane="bottomRight" activeCell="BZ63" sqref="BZ63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.796875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3588,141 +3627,141 @@
   <sheetData>
     <row r="1" spans="1:166" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="1"/>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="64" t="s">
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="64" t="s">
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="64" t="s">
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="65"/>
-      <c r="AC1" s="65"/>
-      <c r="AD1" s="65"/>
-      <c r="AE1" s="65"/>
-      <c r="AF1" s="65"/>
-      <c r="AG1" s="64" t="s">
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="AH1" s="65"/>
-      <c r="AI1" s="65"/>
-      <c r="AJ1" s="65"/>
-      <c r="AK1" s="65"/>
-      <c r="AL1" s="65"/>
-      <c r="AM1" s="65"/>
-      <c r="AN1" s="62" t="s">
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="66"/>
+      <c r="AJ1" s="66"/>
+      <c r="AK1" s="66"/>
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
+      <c r="AN1" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="AO1" s="63"/>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="63"/>
-      <c r="AS1" s="63"/>
-      <c r="AT1" s="63"/>
-      <c r="AU1" s="62" t="s">
+      <c r="AO1" s="64"/>
+      <c r="AP1" s="64"/>
+      <c r="AQ1" s="64"/>
+      <c r="AR1" s="64"/>
+      <c r="AS1" s="64"/>
+      <c r="AT1" s="64"/>
+      <c r="AU1" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="AV1" s="63"/>
-      <c r="AW1" s="63"/>
-      <c r="AX1" s="63"/>
-      <c r="AY1" s="63"/>
-      <c r="AZ1" s="63"/>
-      <c r="BA1" s="63"/>
-      <c r="BB1" s="62" t="s">
+      <c r="AV1" s="64"/>
+      <c r="AW1" s="64"/>
+      <c r="AX1" s="64"/>
+      <c r="AY1" s="64"/>
+      <c r="AZ1" s="64"/>
+      <c r="BA1" s="64"/>
+      <c r="BB1" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="BC1" s="63"/>
-      <c r="BD1" s="63"/>
-      <c r="BE1" s="63"/>
-      <c r="BF1" s="63"/>
-      <c r="BG1" s="63"/>
-      <c r="BH1" s="63"/>
-      <c r="BI1" s="62" t="s">
+      <c r="BC1" s="64"/>
+      <c r="BD1" s="64"/>
+      <c r="BE1" s="64"/>
+      <c r="BF1" s="64"/>
+      <c r="BG1" s="64"/>
+      <c r="BH1" s="64"/>
+      <c r="BI1" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="BJ1" s="63"/>
-      <c r="BK1" s="63"/>
-      <c r="BL1" s="63"/>
-      <c r="BM1" s="63"/>
-      <c r="BN1" s="63"/>
-      <c r="BO1" s="63"/>
-      <c r="BP1" s="62" t="s">
+      <c r="BJ1" s="64"/>
+      <c r="BK1" s="64"/>
+      <c r="BL1" s="64"/>
+      <c r="BM1" s="64"/>
+      <c r="BN1" s="64"/>
+      <c r="BO1" s="64"/>
+      <c r="BP1" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="BQ1" s="63"/>
-      <c r="BR1" s="63"/>
-      <c r="BS1" s="63"/>
-      <c r="BT1" s="63"/>
-      <c r="BU1" s="63"/>
-      <c r="BV1" s="63"/>
-      <c r="BW1" s="62" t="s">
+      <c r="BQ1" s="64"/>
+      <c r="BR1" s="64"/>
+      <c r="BS1" s="64"/>
+      <c r="BT1" s="64"/>
+      <c r="BU1" s="64"/>
+      <c r="BV1" s="64"/>
+      <c r="BW1" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="BX1" s="63"/>
-      <c r="BY1" s="63"/>
-      <c r="BZ1" s="63"/>
-      <c r="CA1" s="63"/>
-      <c r="CB1" s="63"/>
-      <c r="CC1" s="63"/>
-      <c r="CD1" s="62" t="s">
+      <c r="BX1" s="64"/>
+      <c r="BY1" s="64"/>
+      <c r="BZ1" s="64"/>
+      <c r="CA1" s="64"/>
+      <c r="CB1" s="64"/>
+      <c r="CC1" s="64"/>
+      <c r="CD1" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="CE1" s="63"/>
-      <c r="CF1" s="63"/>
-      <c r="CG1" s="63"/>
-      <c r="CH1" s="63"/>
-      <c r="CI1" s="63"/>
-      <c r="CJ1" s="63"/>
-      <c r="CK1" s="62" t="s">
+      <c r="CE1" s="64"/>
+      <c r="CF1" s="64"/>
+      <c r="CG1" s="64"/>
+      <c r="CH1" s="64"/>
+      <c r="CI1" s="64"/>
+      <c r="CJ1" s="64"/>
+      <c r="CK1" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="CL1" s="63"/>
-      <c r="CM1" s="63"/>
-      <c r="CN1" s="63"/>
-      <c r="CO1" s="63"/>
-      <c r="CP1" s="63"/>
-      <c r="CQ1" s="63"/>
-      <c r="CR1" s="62" t="s">
+      <c r="CL1" s="64"/>
+      <c r="CM1" s="64"/>
+      <c r="CN1" s="64"/>
+      <c r="CO1" s="64"/>
+      <c r="CP1" s="64"/>
+      <c r="CQ1" s="64"/>
+      <c r="CR1" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="CS1" s="63"/>
-      <c r="CT1" s="63"/>
-      <c r="CU1" s="63"/>
-      <c r="CV1" s="63"/>
-      <c r="CW1" s="63"/>
-      <c r="CX1" s="63"/>
-      <c r="CY1" s="62" t="s">
+      <c r="CS1" s="64"/>
+      <c r="CT1" s="64"/>
+      <c r="CU1" s="64"/>
+      <c r="CV1" s="64"/>
+      <c r="CW1" s="64"/>
+      <c r="CX1" s="64"/>
+      <c r="CY1" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="CZ1" s="63"/>
-      <c r="DA1" s="63"/>
-      <c r="DB1" s="63"/>
-      <c r="DC1" s="63"/>
-      <c r="DD1" s="63"/>
-      <c r="DE1" s="63"/>
+      <c r="CZ1" s="64"/>
+      <c r="DA1" s="64"/>
+      <c r="DB1" s="64"/>
+      <c r="DC1" s="64"/>
+      <c r="DD1" s="64"/>
+      <c r="DE1" s="64"/>
       <c r="DF1" s="2"/>
       <c r="DG1" s="2"/>
       <c r="DH1" s="2"/>
@@ -5197,7 +5236,7 @@
     </row>
     <row r="46" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
-      <c r="B46" s="66" t="s">
+      <c r="B46" s="62" t="s">
         <v>54</v>
       </c>
       <c r="C46" s="15" t="s">
@@ -5206,21 +5245,21 @@
     </row>
     <row r="47" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
-      <c r="B47" s="66"/>
+      <c r="B47" s="62"/>
       <c r="C47" s="15" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
-      <c r="B48" s="66"/>
+      <c r="B48" s="62"/>
       <c r="C48" s="15" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A49" s="6"/>
-      <c r="B49" s="66"/>
+      <c r="B49" s="62"/>
       <c r="C49" s="15" t="s">
         <v>224</v>
       </c>
@@ -5230,223 +5269,226 @@
     </row>
     <row r="50" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A50" s="6"/>
-      <c r="B50" s="66"/>
+      <c r="B50" s="62"/>
       <c r="C50" s="15" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A51" s="6"/>
-      <c r="B51" s="66"/>
+      <c r="B51" s="62"/>
       <c r="C51" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B52" s="66"/>
+      <c r="B52" s="62"/>
       <c r="C52" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B53" s="66"/>
+      <c r="B53" s="62"/>
       <c r="C53" s="15" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A54" s="6"/>
-      <c r="B54" s="66"/>
+      <c r="B54" s="62"/>
       <c r="C54" s="15" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A55" s="6"/>
-      <c r="B55" s="66"/>
+      <c r="B55" s="62"/>
       <c r="C55" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A56" s="6"/>
-      <c r="B56" s="66"/>
+      <c r="B56" s="62"/>
       <c r="C56" s="15" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
-      <c r="B57" s="66"/>
+      <c r="B57" s="62"/>
       <c r="C57" s="15" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="66"/>
+      <c r="B58" s="62"/>
       <c r="C58" s="15" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B59" s="66"/>
+      <c r="B59" s="62"/>
       <c r="C59" s="15" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="60" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B60" s="66"/>
+      <c r="B60" s="62"/>
       <c r="C60" s="15" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="61" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B61" s="66"/>
+      <c r="B61" s="62"/>
       <c r="C61" s="15" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B62" s="66"/>
+      <c r="B62" s="62"/>
       <c r="C62" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B63" s="66"/>
+      <c r="B63" s="62"/>
       <c r="C63" s="15" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="64" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B64" s="62"/>
+      <c r="C64" s="15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B64" s="66"/>
-      <c r="C64" s="15"/>
-    </row>
     <row r="65" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B65" s="66"/>
-      <c r="C65" s="15" t="s">
+      <c r="B65" s="62"/>
+      <c r="C65" s="15"/>
+    </row>
+    <row r="66" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B66" s="62"/>
+      <c r="C66" s="15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B66" s="66"/>
-      <c r="C66" s="15" t="s">
+    <row r="67" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B67" s="62"/>
+      <c r="C67" s="15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B67" s="66"/>
-      <c r="C67" s="15" t="s">
+    <row r="68" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B68" s="62"/>
+      <c r="C68" s="15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B68" s="66"/>
-      <c r="C68" s="15" t="s">
+    <row r="69" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B69" s="62"/>
+      <c r="C69" s="15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B69" s="66"/>
-      <c r="C69" s="16" t="s">
+    <row r="70" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B70" s="62"/>
+      <c r="C70" s="16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B70" s="66"/>
-      <c r="C70" s="15" t="s">
+    <row r="71" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B71" s="62"/>
+      <c r="C71" s="15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B71" s="66"/>
-      <c r="C71" s="15" t="s">
+    <row r="72" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B72" s="62"/>
+      <c r="C72" s="15" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B72" s="66"/>
-      <c r="C72" s="15" t="s">
+    <row r="73" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B73" s="62"/>
+      <c r="C73" s="15" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B73" s="66"/>
-      <c r="C73" s="15" t="s">
+    <row r="74" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B74" s="62"/>
+      <c r="C74" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B74" s="66"/>
-      <c r="C74" s="16"/>
-    </row>
     <row r="75" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B75" s="66"/>
-      <c r="C75" s="15" t="s">
+      <c r="B75" s="62"/>
+      <c r="C75" s="16"/>
+    </row>
+    <row r="76" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B76" s="62"/>
+      <c r="C76" s="15" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B76" s="66"/>
-      <c r="C76" s="15" t="s">
+    <row r="77" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B77" s="62"/>
+      <c r="C77" s="15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="77" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B77" s="66"/>
-      <c r="C77" s="15" t="s">
+    <row r="78" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B78" s="62"/>
+      <c r="C78" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="78" spans="2:53" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B78" s="66"/>
-      <c r="C78" s="15" t="s">
+    <row r="79" spans="2:53" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B79" s="62"/>
+      <c r="C79" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="BA78" s="6"/>
-    </row>
-    <row r="79" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B79" s="66"/>
-      <c r="C79" s="16"/>
+      <c r="BA79" s="6"/>
     </row>
     <row r="80" spans="2:53" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B80" s="66"/>
-      <c r="C80" s="15" t="s">
+      <c r="B80" s="62"/>
+      <c r="C80" s="16"/>
+    </row>
+    <row r="81" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B81" s="62"/>
+      <c r="C81" s="15" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="81" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B81" s="66"/>
-      <c r="C81" s="59" t="s">
+    <row r="82" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B82" s="62"/>
+      <c r="C82" s="59" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="82" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B82" s="66"/>
-      <c r="C82" s="59" t="s">
+    <row r="83" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B83" s="62"/>
+      <c r="C83" s="59" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="83" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B83" s="66"/>
-      <c r="C83" s="59" t="s">
+    <row r="84" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B84" s="62"/>
+      <c r="C84" s="59" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="84" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B84" s="66"/>
-      <c r="C84" s="15" t="s">
+    <row r="85" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="B85" s="62"/>
+      <c r="C85" s="15" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="85" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="C85" s="1"/>
-      <c r="BW85" s="46" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="86" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
       <c r="C86" s="1"/>
+      <c r="BW86" s="46" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="87" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
       <c r="C87" s="1"/>
@@ -8187,10 +8229,14 @@
     <row r="999" spans="3:3" ht="12.75" x14ac:dyDescent="0.35">
       <c r="C999" s="1"/>
     </row>
+    <row r="1000" spans="3:3" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="C1000" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B79:B84"/>
-    <mergeCell ref="B46:B78"/>
+    <mergeCell ref="CD1:CJ1"/>
+    <mergeCell ref="B80:B85"/>
+    <mergeCell ref="B46:B79"/>
     <mergeCell ref="CK1:CQ1"/>
     <mergeCell ref="CR1:CX1"/>
     <mergeCell ref="CY1:DE1"/>
@@ -8205,7 +8251,6 @@
     <mergeCell ref="BI1:BO1"/>
     <mergeCell ref="BP1:BV1"/>
     <mergeCell ref="BW1:CC1"/>
-    <mergeCell ref="CD1:CJ1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:J4 L4:CW4 CY4:EV4">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
@@ -8221,13 +8266,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:FB43"/>
+  <dimension ref="A1:FB44"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="AR5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="AL5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AV36" sqref="AV36"/>
+      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.796875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -8240,194 +8285,194 @@
   <sheetData>
     <row r="1" spans="1:158" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="1"/>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="62" t="s">
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="62" t="s">
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="63"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="63"/>
-      <c r="Z1" s="62" t="s">
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="64"/>
+      <c r="X1" s="64"/>
+      <c r="Y1" s="64"/>
+      <c r="Z1" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="AA1" s="63"/>
-      <c r="AB1" s="63"/>
-      <c r="AC1" s="63"/>
-      <c r="AD1" s="63"/>
-      <c r="AE1" s="63"/>
-      <c r="AF1" s="63"/>
-      <c r="AG1" s="62" t="s">
+      <c r="AA1" s="64"/>
+      <c r="AB1" s="64"/>
+      <c r="AC1" s="64"/>
+      <c r="AD1" s="64"/>
+      <c r="AE1" s="64"/>
+      <c r="AF1" s="64"/>
+      <c r="AG1" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="AH1" s="63"/>
-      <c r="AI1" s="63"/>
-      <c r="AJ1" s="63"/>
-      <c r="AK1" s="63"/>
-      <c r="AL1" s="63"/>
-      <c r="AM1" s="63"/>
-      <c r="AN1" s="62" t="s">
+      <c r="AH1" s="64"/>
+      <c r="AI1" s="64"/>
+      <c r="AJ1" s="64"/>
+      <c r="AK1" s="64"/>
+      <c r="AL1" s="64"/>
+      <c r="AM1" s="64"/>
+      <c r="AN1" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="AO1" s="63"/>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="63"/>
-      <c r="AS1" s="63"/>
-      <c r="AT1" s="63"/>
-      <c r="AU1" s="62" t="s">
+      <c r="AO1" s="64"/>
+      <c r="AP1" s="64"/>
+      <c r="AQ1" s="64"/>
+      <c r="AR1" s="64"/>
+      <c r="AS1" s="64"/>
+      <c r="AT1" s="64"/>
+      <c r="AU1" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="AV1" s="63"/>
-      <c r="AW1" s="63"/>
-      <c r="AX1" s="63"/>
-      <c r="AY1" s="63"/>
-      <c r="AZ1" s="63"/>
-      <c r="BA1" s="63"/>
-      <c r="BB1" s="62" t="s">
+      <c r="AV1" s="64"/>
+      <c r="AW1" s="64"/>
+      <c r="AX1" s="64"/>
+      <c r="AY1" s="64"/>
+      <c r="AZ1" s="64"/>
+      <c r="BA1" s="64"/>
+      <c r="BB1" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="BC1" s="63"/>
-      <c r="BD1" s="63"/>
-      <c r="BE1" s="63"/>
-      <c r="BF1" s="63"/>
-      <c r="BG1" s="63"/>
-      <c r="BH1" s="63"/>
-      <c r="BI1" s="62" t="s">
+      <c r="BC1" s="64"/>
+      <c r="BD1" s="64"/>
+      <c r="BE1" s="64"/>
+      <c r="BF1" s="64"/>
+      <c r="BG1" s="64"/>
+      <c r="BH1" s="64"/>
+      <c r="BI1" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="BJ1" s="63"/>
-      <c r="BK1" s="63"/>
-      <c r="BL1" s="63"/>
-      <c r="BM1" s="63"/>
-      <c r="BN1" s="63"/>
-      <c r="BO1" s="63"/>
-      <c r="BP1" s="62" t="s">
+      <c r="BJ1" s="64"/>
+      <c r="BK1" s="64"/>
+      <c r="BL1" s="64"/>
+      <c r="BM1" s="64"/>
+      <c r="BN1" s="64"/>
+      <c r="BO1" s="64"/>
+      <c r="BP1" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="BQ1" s="63"/>
-      <c r="BR1" s="63"/>
-      <c r="BS1" s="63"/>
-      <c r="BT1" s="63"/>
-      <c r="BU1" s="63"/>
-      <c r="BV1" s="63"/>
-      <c r="BW1" s="62" t="s">
+      <c r="BQ1" s="64"/>
+      <c r="BR1" s="64"/>
+      <c r="BS1" s="64"/>
+      <c r="BT1" s="64"/>
+      <c r="BU1" s="64"/>
+      <c r="BV1" s="64"/>
+      <c r="BW1" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="BX1" s="63"/>
-      <c r="BY1" s="63"/>
-      <c r="BZ1" s="63"/>
-      <c r="CA1" s="63"/>
-      <c r="CB1" s="63"/>
-      <c r="CC1" s="63"/>
-      <c r="CD1" s="62" t="s">
+      <c r="BX1" s="64"/>
+      <c r="BY1" s="64"/>
+      <c r="BZ1" s="64"/>
+      <c r="CA1" s="64"/>
+      <c r="CB1" s="64"/>
+      <c r="CC1" s="64"/>
+      <c r="CD1" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="CE1" s="63"/>
-      <c r="CF1" s="63"/>
-      <c r="CG1" s="63"/>
-      <c r="CH1" s="63"/>
-      <c r="CI1" s="63"/>
-      <c r="CJ1" s="63"/>
-      <c r="CK1" s="62" t="s">
+      <c r="CE1" s="64"/>
+      <c r="CF1" s="64"/>
+      <c r="CG1" s="64"/>
+      <c r="CH1" s="64"/>
+      <c r="CI1" s="64"/>
+      <c r="CJ1" s="64"/>
+      <c r="CK1" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="CL1" s="63"/>
-      <c r="CM1" s="63"/>
-      <c r="CN1" s="63"/>
-      <c r="CO1" s="63"/>
-      <c r="CP1" s="63"/>
-      <c r="CQ1" s="63"/>
-      <c r="CR1" s="62" t="s">
+      <c r="CL1" s="64"/>
+      <c r="CM1" s="64"/>
+      <c r="CN1" s="64"/>
+      <c r="CO1" s="64"/>
+      <c r="CP1" s="64"/>
+      <c r="CQ1" s="64"/>
+      <c r="CR1" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="CS1" s="63"/>
-      <c r="CT1" s="63"/>
-      <c r="CU1" s="63"/>
-      <c r="CV1" s="63"/>
-      <c r="CW1" s="63"/>
-      <c r="CX1" s="63"/>
-      <c r="CY1" s="62" t="s">
+      <c r="CS1" s="64"/>
+      <c r="CT1" s="64"/>
+      <c r="CU1" s="64"/>
+      <c r="CV1" s="64"/>
+      <c r="CW1" s="64"/>
+      <c r="CX1" s="64"/>
+      <c r="CY1" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="CZ1" s="63"/>
-      <c r="DA1" s="63"/>
-      <c r="DB1" s="63"/>
-      <c r="DC1" s="63"/>
-      <c r="DD1" s="63"/>
-      <c r="DE1" s="63"/>
-      <c r="DF1" s="62" t="s">
+      <c r="CZ1" s="64"/>
+      <c r="DA1" s="64"/>
+      <c r="DB1" s="64"/>
+      <c r="DC1" s="64"/>
+      <c r="DD1" s="64"/>
+      <c r="DE1" s="64"/>
+      <c r="DF1" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="DG1" s="63"/>
-      <c r="DH1" s="63"/>
-      <c r="DI1" s="63"/>
-      <c r="DJ1" s="63"/>
-      <c r="DK1" s="63"/>
-      <c r="DL1" s="63"/>
-      <c r="DM1" s="62" t="s">
+      <c r="DG1" s="64"/>
+      <c r="DH1" s="64"/>
+      <c r="DI1" s="64"/>
+      <c r="DJ1" s="64"/>
+      <c r="DK1" s="64"/>
+      <c r="DL1" s="64"/>
+      <c r="DM1" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="DN1" s="63"/>
-      <c r="DO1" s="63"/>
-      <c r="DP1" s="63"/>
-      <c r="DQ1" s="63"/>
-      <c r="DR1" s="63"/>
-      <c r="DS1" s="63"/>
-      <c r="DT1" s="62"/>
-      <c r="DU1" s="63"/>
-      <c r="DV1" s="63"/>
-      <c r="DW1" s="63"/>
-      <c r="DX1" s="63"/>
-      <c r="DY1" s="63"/>
-      <c r="DZ1" s="63"/>
-      <c r="EA1" s="62"/>
-      <c r="EB1" s="63"/>
-      <c r="EC1" s="63"/>
-      <c r="ED1" s="63"/>
-      <c r="EE1" s="63"/>
-      <c r="EF1" s="63"/>
-      <c r="EG1" s="63"/>
-      <c r="EH1" s="62"/>
-      <c r="EI1" s="63"/>
-      <c r="EJ1" s="63"/>
-      <c r="EK1" s="63"/>
-      <c r="EL1" s="63"/>
-      <c r="EM1" s="63"/>
-      <c r="EN1" s="63"/>
-      <c r="EO1" s="62"/>
-      <c r="EP1" s="63"/>
-      <c r="EQ1" s="63"/>
-      <c r="ER1" s="63"/>
-      <c r="ES1" s="63"/>
-      <c r="ET1" s="63"/>
-      <c r="EU1" s="63"/>
-      <c r="EV1" s="62"/>
-      <c r="EW1" s="63"/>
-      <c r="EX1" s="63"/>
-      <c r="EY1" s="63"/>
-      <c r="EZ1" s="63"/>
-      <c r="FA1" s="63"/>
-      <c r="FB1" s="63"/>
+      <c r="DN1" s="64"/>
+      <c r="DO1" s="64"/>
+      <c r="DP1" s="64"/>
+      <c r="DQ1" s="64"/>
+      <c r="DR1" s="64"/>
+      <c r="DS1" s="64"/>
+      <c r="DT1" s="63"/>
+      <c r="DU1" s="64"/>
+      <c r="DV1" s="64"/>
+      <c r="DW1" s="64"/>
+      <c r="DX1" s="64"/>
+      <c r="DY1" s="64"/>
+      <c r="DZ1" s="64"/>
+      <c r="EA1" s="63"/>
+      <c r="EB1" s="64"/>
+      <c r="EC1" s="64"/>
+      <c r="ED1" s="64"/>
+      <c r="EE1" s="64"/>
+      <c r="EF1" s="64"/>
+      <c r="EG1" s="64"/>
+      <c r="EH1" s="63"/>
+      <c r="EI1" s="64"/>
+      <c r="EJ1" s="64"/>
+      <c r="EK1" s="64"/>
+      <c r="EL1" s="64"/>
+      <c r="EM1" s="64"/>
+      <c r="EN1" s="64"/>
+      <c r="EO1" s="63"/>
+      <c r="EP1" s="64"/>
+      <c r="EQ1" s="64"/>
+      <c r="ER1" s="64"/>
+      <c r="ES1" s="64"/>
+      <c r="ET1" s="64"/>
+      <c r="EU1" s="64"/>
+      <c r="EV1" s="63"/>
+      <c r="EW1" s="64"/>
+      <c r="EX1" s="64"/>
+      <c r="EY1" s="64"/>
+      <c r="EZ1" s="64"/>
+      <c r="FA1" s="64"/>
+      <c r="FB1" s="64"/>
     </row>
     <row r="2" spans="1:158" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="1"/>
@@ -9363,22 +9408,8 @@
     </row>
     <row r="21" spans="3:112" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="39"/>
-      <c r="R21" s="39"/>
+        <v>262</v>
+      </c>
       <c r="S21" s="39"/>
       <c r="T21" s="39"/>
       <c r="U21" s="39"/>
@@ -9475,120 +9506,204 @@
       <c r="DH21" s="39"/>
     </row>
     <row r="22" spans="3:112" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="39"/>
+      <c r="O22" s="39"/>
+      <c r="P22" s="39"/>
+      <c r="Q22" s="39"/>
+      <c r="R22" s="39"/>
+      <c r="S22" s="39"/>
+      <c r="T22" s="39"/>
+      <c r="U22" s="39"/>
+      <c r="V22" s="39"/>
+      <c r="W22" s="39"/>
+      <c r="X22" s="39"/>
+      <c r="Y22" s="39"/>
+      <c r="Z22" s="39"/>
+      <c r="AA22" s="39"/>
+      <c r="AB22" s="39"/>
+      <c r="AC22" s="39"/>
+      <c r="AD22" s="39"/>
+      <c r="AE22" s="39"/>
+      <c r="AF22" s="39"/>
+      <c r="AG22" s="39"/>
+      <c r="AH22" s="39"/>
+      <c r="AI22" s="39"/>
+      <c r="AJ22" s="39"/>
+      <c r="AK22" s="39"/>
+      <c r="AL22" s="39"/>
+      <c r="AM22" s="39"/>
+      <c r="AN22" s="39"/>
+      <c r="AO22" s="39"/>
+      <c r="AP22" s="39"/>
+      <c r="AQ22" s="39"/>
+      <c r="AR22" s="39"/>
+      <c r="AS22" s="39"/>
+      <c r="AT22" s="39"/>
+      <c r="AU22" s="39"/>
+      <c r="AV22" s="39"/>
+      <c r="AW22" s="39"/>
+      <c r="AX22" s="39"/>
+      <c r="AY22" s="39"/>
+      <c r="AZ22" s="39"/>
+      <c r="BA22" s="39"/>
+      <c r="BB22" s="39"/>
+      <c r="BC22" s="39"/>
+      <c r="BD22" s="39"/>
+      <c r="BE22" s="39"/>
+      <c r="BF22" s="39"/>
+      <c r="BG22" s="39"/>
+      <c r="BH22" s="39"/>
+      <c r="BI22" s="39"/>
+      <c r="BJ22" s="39"/>
+      <c r="BK22" s="39"/>
+      <c r="BL22" s="39"/>
+      <c r="BM22" s="39"/>
+      <c r="BN22" s="39"/>
+      <c r="BO22" s="39"/>
+      <c r="BP22" s="39"/>
+      <c r="BQ22" s="39"/>
+      <c r="BR22" s="39"/>
+      <c r="BS22" s="39"/>
+      <c r="BT22" s="39"/>
+      <c r="BU22" s="39"/>
+      <c r="BV22" s="39"/>
+      <c r="BW22" s="39"/>
+      <c r="BX22" s="39"/>
+      <c r="BY22" s="39"/>
+      <c r="BZ22" s="39"/>
+      <c r="CA22" s="39"/>
+      <c r="CB22" s="39"/>
+      <c r="CC22" s="39"/>
+      <c r="CD22" s="39"/>
+      <c r="CE22" s="39"/>
+      <c r="CF22" s="39"/>
+      <c r="CG22" s="39"/>
+      <c r="CH22" s="39"/>
+      <c r="CI22" s="39"/>
+      <c r="CJ22" s="39"/>
+      <c r="CK22" s="39"/>
+      <c r="CL22" s="39"/>
+      <c r="CM22" s="39"/>
+      <c r="CN22" s="39"/>
+      <c r="CO22" s="39"/>
+      <c r="CP22" s="39"/>
+      <c r="CQ22" s="39"/>
+      <c r="CR22" s="39"/>
+      <c r="CS22" s="39"/>
+      <c r="CT22" s="39"/>
+      <c r="CU22" s="39"/>
+      <c r="CV22" s="39"/>
+      <c r="CW22" s="39"/>
+      <c r="CX22" s="39"/>
+      <c r="CY22" s="39"/>
+      <c r="CZ22" s="39"/>
+      <c r="DA22" s="39"/>
+      <c r="DB22" s="39"/>
+      <c r="DC22" s="39"/>
+      <c r="DD22" s="39"/>
+      <c r="DE22" s="39"/>
+      <c r="DF22" s="39"/>
+      <c r="DG22" s="39"/>
+      <c r="DH22" s="39"/>
+    </row>
+    <row r="23" spans="3:112" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="DG22" s="39"/>
-      <c r="DH22" s="52" t="s">
+      <c r="DG23" s="39"/>
+      <c r="DH23" s="52" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="3:112" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="1"/>
-    </row>
     <row r="24" spans="3:112" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="S24" s="39"/>
-      <c r="T24" s="39"/>
-      <c r="U24" s="39"/>
-      <c r="V24" s="39"/>
-      <c r="W24" s="39"/>
-      <c r="X24" s="39"/>
-      <c r="Y24" s="39"/>
-      <c r="Z24" s="39"/>
-      <c r="AA24" s="39"/>
-      <c r="AB24" s="39"/>
-      <c r="AC24" s="39"/>
-      <c r="AD24" s="39"/>
-      <c r="AE24" s="39"/>
-      <c r="AF24" s="39"/>
-      <c r="AG24" s="39"/>
-      <c r="AH24" s="39"/>
-      <c r="AI24" s="39"/>
-      <c r="AJ24" s="39"/>
-      <c r="AK24" s="39"/>
-      <c r="AL24" s="39"/>
-      <c r="AM24" s="39"/>
-      <c r="AN24" s="39"/>
-      <c r="AO24" s="39"/>
-      <c r="AP24" s="39"/>
-      <c r="AQ24" s="39"/>
-      <c r="AR24" s="39"/>
-      <c r="AS24" s="39"/>
-      <c r="AT24" s="39"/>
-      <c r="AU24" s="39"/>
-      <c r="AV24" s="39"/>
-      <c r="AW24" s="39"/>
-      <c r="AX24" s="39"/>
-      <c r="AY24" s="39"/>
-      <c r="AZ24" s="39"/>
-      <c r="BA24" s="39"/>
-      <c r="BB24" s="39"/>
-      <c r="BC24" s="39"/>
-      <c r="BD24" s="39"/>
-      <c r="BE24" s="39"/>
-      <c r="BF24" s="39"/>
-      <c r="BG24" s="39"/>
-      <c r="BH24" s="39"/>
-      <c r="BI24" s="39"/>
-      <c r="BJ24" s="39"/>
-      <c r="BK24" s="39"/>
-      <c r="BL24" s="39"/>
-      <c r="BM24" s="39"/>
-      <c r="BN24" s="39"/>
-      <c r="BO24" s="39"/>
-      <c r="BP24" s="39"/>
-      <c r="BQ24" s="39"/>
-      <c r="BR24" s="39"/>
-      <c r="BS24" s="39"/>
-      <c r="BT24" s="39"/>
-      <c r="BU24" s="39"/>
-      <c r="BV24" s="39"/>
-      <c r="BW24" s="39"/>
-      <c r="BX24" s="39"/>
-      <c r="BY24" s="39"/>
-      <c r="BZ24" s="39"/>
-      <c r="CA24" s="39"/>
-      <c r="CB24" s="39"/>
-      <c r="CC24" s="39"/>
-      <c r="CD24" s="39"/>
-      <c r="CE24" s="39"/>
-      <c r="CF24" s="39"/>
-      <c r="CG24" s="39"/>
-      <c r="CH24" s="39"/>
-      <c r="CI24" s="39"/>
-      <c r="CJ24" s="39"/>
-      <c r="CK24" s="39"/>
-      <c r="CL24" s="39"/>
-      <c r="CM24" s="39"/>
-      <c r="CN24" s="39"/>
-      <c r="CO24" s="39"/>
-      <c r="CP24" s="39"/>
-      <c r="CQ24" s="39"/>
-      <c r="CR24" s="39"/>
-      <c r="CS24" s="39"/>
-      <c r="CT24" s="39"/>
-      <c r="CU24" s="39"/>
-      <c r="CV24" s="39"/>
-      <c r="CW24" s="39"/>
-      <c r="CX24" s="39"/>
-      <c r="CY24" s="39"/>
-      <c r="CZ24" s="39"/>
-      <c r="DA24" s="39"/>
-      <c r="DB24" s="39"/>
-      <c r="DC24" s="39"/>
-      <c r="DD24" s="39"/>
-      <c r="DE24" s="39"/>
-      <c r="DF24" s="39"/>
-      <c r="DG24" s="39"/>
-      <c r="DH24" s="39"/>
+      <c r="C24" s="1"/>
     </row>
     <row r="25" spans="3:112" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="S25" s="39"/>
+      <c r="T25" s="39"/>
+      <c r="U25" s="39"/>
+      <c r="V25" s="39"/>
+      <c r="W25" s="39"/>
+      <c r="X25" s="39"/>
+      <c r="Y25" s="39"/>
+      <c r="Z25" s="39"/>
+      <c r="AA25" s="39"/>
+      <c r="AB25" s="39"/>
+      <c r="AC25" s="39"/>
+      <c r="AD25" s="39"/>
+      <c r="AE25" s="39"/>
+      <c r="AF25" s="39"/>
+      <c r="AG25" s="39"/>
+      <c r="AH25" s="39"/>
+      <c r="AI25" s="39"/>
+      <c r="AJ25" s="39"/>
+      <c r="AK25" s="39"/>
+      <c r="AL25" s="39"/>
+      <c r="AM25" s="39"/>
+      <c r="AN25" s="39"/>
+      <c r="AO25" s="39"/>
+      <c r="AP25" s="39"/>
+      <c r="AQ25" s="39"/>
+      <c r="AR25" s="39"/>
+      <c r="AS25" s="39"/>
+      <c r="AT25" s="39"/>
+      <c r="AU25" s="39"/>
+      <c r="AV25" s="39"/>
+      <c r="AW25" s="39"/>
+      <c r="AX25" s="39"/>
+      <c r="AY25" s="39"/>
+      <c r="AZ25" s="39"/>
+      <c r="BA25" s="39"/>
+      <c r="BB25" s="39"/>
+      <c r="BC25" s="39"/>
+      <c r="BD25" s="39"/>
+      <c r="BE25" s="39"/>
+      <c r="BF25" s="39"/>
+      <c r="BG25" s="39"/>
+      <c r="BH25" s="39"/>
+      <c r="BI25" s="39"/>
+      <c r="BJ25" s="39"/>
+      <c r="BK25" s="39"/>
+      <c r="BL25" s="39"/>
+      <c r="BM25" s="39"/>
+      <c r="BN25" s="39"/>
+      <c r="BO25" s="39"/>
+      <c r="BP25" s="39"/>
+      <c r="BQ25" s="39"/>
+      <c r="BR25" s="39"/>
+      <c r="BS25" s="39"/>
+      <c r="BT25" s="39"/>
+      <c r="BU25" s="39"/>
+      <c r="BV25" s="39"/>
+      <c r="BW25" s="39"/>
+      <c r="BX25" s="39"/>
+      <c r="BY25" s="39"/>
+      <c r="BZ25" s="39"/>
+      <c r="CA25" s="39"/>
+      <c r="CB25" s="39"/>
+      <c r="CC25" s="39"/>
+      <c r="CD25" s="39"/>
+      <c r="CE25" s="39"/>
+      <c r="CF25" s="39"/>
+      <c r="CG25" s="39"/>
+      <c r="CH25" s="39"/>
+      <c r="CI25" s="39"/>
+      <c r="CJ25" s="39"/>
       <c r="CK25" s="39"/>
       <c r="CL25" s="39"/>
       <c r="CM25" s="39"/>
@@ -9616,7 +9731,7 @@
     </row>
     <row r="26" spans="3:112" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C26" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="CK26" s="39"/>
       <c r="CL26" s="39"/>
@@ -9645,78 +9760,8 @@
     </row>
     <row r="27" spans="3:112" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="S27" s="39"/>
-      <c r="T27" s="39"/>
-      <c r="U27" s="39"/>
-      <c r="V27" s="39"/>
-      <c r="W27" s="39"/>
-      <c r="X27" s="39"/>
-      <c r="Y27" s="39"/>
-      <c r="Z27" s="39"/>
-      <c r="AA27" s="39"/>
-      <c r="AB27" s="39"/>
-      <c r="AC27" s="39"/>
-      <c r="AD27" s="39"/>
-      <c r="AE27" s="39"/>
-      <c r="AF27" s="39"/>
-      <c r="AG27" s="39"/>
-      <c r="AH27" s="39"/>
-      <c r="AI27" s="39"/>
-      <c r="AJ27" s="39"/>
-      <c r="AK27" s="39"/>
-      <c r="AL27" s="39"/>
-      <c r="AM27" s="39"/>
-      <c r="AN27" s="39"/>
-      <c r="AO27" s="39"/>
-      <c r="AP27" s="39"/>
-      <c r="AQ27" s="39"/>
-      <c r="AR27" s="39"/>
-      <c r="AS27" s="39"/>
-      <c r="AT27" s="39"/>
-      <c r="AU27" s="39"/>
-      <c r="AV27" s="39"/>
-      <c r="AW27" s="39"/>
-      <c r="AX27" s="39"/>
-      <c r="AY27" s="39"/>
-      <c r="AZ27" s="39"/>
-      <c r="BA27" s="39"/>
-      <c r="BB27" s="39"/>
-      <c r="BC27" s="39"/>
-      <c r="BD27" s="39"/>
-      <c r="BE27" s="39"/>
-      <c r="BF27" s="39"/>
-      <c r="BG27" s="39"/>
-      <c r="BH27" s="39"/>
-      <c r="BI27" s="39"/>
-      <c r="BJ27" s="39"/>
-      <c r="BK27" s="39"/>
-      <c r="BL27" s="39"/>
-      <c r="BM27" s="39"/>
-      <c r="BN27" s="39"/>
-      <c r="BO27" s="39"/>
-      <c r="BP27" s="39"/>
-      <c r="BQ27" s="39"/>
-      <c r="BR27" s="39"/>
-      <c r="BS27" s="39"/>
-      <c r="BT27" s="39"/>
-      <c r="BU27" s="39"/>
-      <c r="BV27" s="39"/>
-      <c r="BW27" s="39"/>
-      <c r="BX27" s="39"/>
-      <c r="BY27" s="39"/>
-      <c r="BZ27" s="39"/>
-      <c r="CA27" s="39"/>
-      <c r="CB27" s="39"/>
-      <c r="CC27" s="39"/>
-      <c r="CD27" s="39"/>
-      <c r="CE27" s="39"/>
-      <c r="CF27" s="39"/>
-      <c r="CG27" s="39"/>
-      <c r="CH27" s="39"/>
-      <c r="CI27" s="39"/>
-      <c r="CJ27" s="39"/>
+        <v>63</v>
+      </c>
       <c r="CK27" s="39"/>
       <c r="CL27" s="39"/>
       <c r="CM27" s="39"/>
@@ -9743,9 +9788,79 @@
       <c r="DH27" s="39"/>
     </row>
     <row r="28" spans="3:112" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="C28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="S28" s="39"/>
+      <c r="T28" s="39"/>
+      <c r="U28" s="39"/>
+      <c r="V28" s="39"/>
+      <c r="W28" s="39"/>
+      <c r="X28" s="39"/>
+      <c r="Y28" s="39"/>
+      <c r="Z28" s="39"/>
+      <c r="AA28" s="39"/>
+      <c r="AB28" s="39"/>
+      <c r="AC28" s="39"/>
+      <c r="AD28" s="39"/>
+      <c r="AE28" s="39"/>
+      <c r="AF28" s="39"/>
+      <c r="AG28" s="39"/>
+      <c r="AH28" s="39"/>
+      <c r="AI28" s="39"/>
+      <c r="AJ28" s="39"/>
+      <c r="AK28" s="39"/>
+      <c r="AL28" s="39"/>
+      <c r="AM28" s="39"/>
+      <c r="AN28" s="39"/>
+      <c r="AO28" s="39"/>
+      <c r="AP28" s="39"/>
+      <c r="AQ28" s="39"/>
+      <c r="AR28" s="39"/>
+      <c r="AS28" s="39"/>
+      <c r="AT28" s="39"/>
+      <c r="AU28" s="39"/>
+      <c r="AV28" s="39"/>
+      <c r="AW28" s="39"/>
+      <c r="AX28" s="39"/>
+      <c r="AY28" s="39"/>
+      <c r="AZ28" s="39"/>
+      <c r="BA28" s="39"/>
+      <c r="BB28" s="39"/>
+      <c r="BC28" s="39"/>
+      <c r="BD28" s="39"/>
+      <c r="BE28" s="39"/>
+      <c r="BF28" s="39"/>
+      <c r="BG28" s="39"/>
+      <c r="BH28" s="39"/>
+      <c r="BI28" s="39"/>
+      <c r="BJ28" s="39"/>
+      <c r="BK28" s="39"/>
+      <c r="BL28" s="39"/>
+      <c r="BM28" s="39"/>
+      <c r="BN28" s="39"/>
+      <c r="BO28" s="39"/>
+      <c r="BP28" s="39"/>
+      <c r="BQ28" s="39"/>
+      <c r="BR28" s="39"/>
+      <c r="BS28" s="39"/>
+      <c r="BT28" s="39"/>
+      <c r="BU28" s="39"/>
+      <c r="BV28" s="39"/>
+      <c r="BW28" s="39"/>
+      <c r="BX28" s="39"/>
+      <c r="BY28" s="39"/>
+      <c r="BZ28" s="39"/>
+      <c r="CA28" s="39"/>
+      <c r="CB28" s="39"/>
+      <c r="CC28" s="39"/>
+      <c r="CD28" s="39"/>
+      <c r="CE28" s="39"/>
+      <c r="CF28" s="39"/>
+      <c r="CG28" s="39"/>
+      <c r="CH28" s="39"/>
+      <c r="CI28" s="39"/>
+      <c r="CJ28" s="39"/>
       <c r="CK28" s="39"/>
       <c r="CL28" s="39"/>
       <c r="CM28" s="39"/>
@@ -9772,79 +9887,9 @@
       <c r="DH28" s="39"/>
     </row>
     <row r="29" spans="3:112" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S29" s="39"/>
-      <c r="T29" s="39"/>
-      <c r="U29" s="39"/>
-      <c r="V29" s="39"/>
-      <c r="W29" s="39"/>
-      <c r="X29" s="39"/>
-      <c r="Y29" s="39"/>
-      <c r="Z29" s="39"/>
-      <c r="AA29" s="39"/>
-      <c r="AB29" s="39"/>
-      <c r="AC29" s="39"/>
-      <c r="AD29" s="39"/>
-      <c r="AE29" s="39"/>
-      <c r="AF29" s="39"/>
-      <c r="AG29" s="39"/>
-      <c r="AH29" s="39"/>
-      <c r="AI29" s="39"/>
-      <c r="AJ29" s="39"/>
-      <c r="AK29" s="39"/>
-      <c r="AL29" s="39"/>
-      <c r="AM29" s="39"/>
-      <c r="AN29" s="39"/>
-      <c r="AO29" s="39"/>
-      <c r="AP29" s="39"/>
-      <c r="AQ29" s="39"/>
-      <c r="AR29" s="39"/>
-      <c r="AS29" s="39"/>
-      <c r="AT29" s="39"/>
-      <c r="AU29" s="39"/>
-      <c r="AV29" s="39"/>
-      <c r="AW29" s="39"/>
-      <c r="AX29" s="39"/>
-      <c r="AY29" s="39"/>
-      <c r="AZ29" s="39"/>
-      <c r="BA29" s="39"/>
-      <c r="BB29" s="39"/>
-      <c r="BC29" s="39"/>
-      <c r="BD29" s="39"/>
-      <c r="BE29" s="39"/>
-      <c r="BF29" s="39"/>
-      <c r="BG29" s="39"/>
-      <c r="BH29" s="39"/>
-      <c r="BI29" s="39"/>
-      <c r="BJ29" s="39"/>
-      <c r="BK29" s="39"/>
-      <c r="BL29" s="39"/>
-      <c r="BM29" s="39"/>
-      <c r="BN29" s="39"/>
-      <c r="BO29" s="39"/>
-      <c r="BP29" s="39"/>
-      <c r="BQ29" s="39"/>
-      <c r="BR29" s="39"/>
-      <c r="BS29" s="39"/>
-      <c r="BT29" s="39"/>
-      <c r="BU29" s="39"/>
-      <c r="BV29" s="39"/>
-      <c r="BW29" s="39"/>
-      <c r="BX29" s="39"/>
-      <c r="BY29" s="39"/>
-      <c r="BZ29" s="39"/>
-      <c r="CA29" s="39"/>
-      <c r="CB29" s="39"/>
-      <c r="CC29" s="39"/>
-      <c r="CD29" s="39"/>
-      <c r="CE29" s="39"/>
-      <c r="CF29" s="39"/>
-      <c r="CG29" s="39"/>
-      <c r="CH29" s="39"/>
-      <c r="CI29" s="39"/>
-      <c r="CJ29" s="39"/>
+      <c r="C29" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="CK29" s="39"/>
       <c r="CL29" s="39"/>
       <c r="CM29" s="39"/>
@@ -9872,55 +9917,132 @@
     </row>
     <row r="30" spans="3:112" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C30" s="1" t="s">
-        <v>67</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="S30" s="39"/>
+      <c r="T30" s="39"/>
+      <c r="U30" s="39"/>
+      <c r="V30" s="39"/>
+      <c r="W30" s="39"/>
+      <c r="X30" s="39"/>
+      <c r="Y30" s="39"/>
+      <c r="Z30" s="39"/>
+      <c r="AA30" s="39"/>
+      <c r="AB30" s="39"/>
+      <c r="AC30" s="39"/>
+      <c r="AD30" s="39"/>
+      <c r="AE30" s="39"/>
+      <c r="AF30" s="39"/>
+      <c r="AG30" s="39"/>
+      <c r="AH30" s="39"/>
+      <c r="AI30" s="39"/>
+      <c r="AJ30" s="39"/>
+      <c r="AK30" s="39"/>
+      <c r="AL30" s="39"/>
+      <c r="AM30" s="39"/>
+      <c r="AN30" s="39"/>
+      <c r="AO30" s="39"/>
+      <c r="AP30" s="39"/>
+      <c r="AQ30" s="39"/>
+      <c r="AR30" s="39"/>
+      <c r="AS30" s="39"/>
+      <c r="AT30" s="39"/>
+      <c r="AU30" s="39"/>
+      <c r="AV30" s="39"/>
+      <c r="AW30" s="39"/>
+      <c r="AX30" s="39"/>
+      <c r="AY30" s="39"/>
+      <c r="AZ30" s="39"/>
+      <c r="BA30" s="39"/>
+      <c r="BB30" s="39"/>
+      <c r="BC30" s="39"/>
+      <c r="BD30" s="39"/>
+      <c r="BE30" s="39"/>
+      <c r="BF30" s="39"/>
+      <c r="BG30" s="39"/>
+      <c r="BH30" s="39"/>
+      <c r="BI30" s="39"/>
+      <c r="BJ30" s="39"/>
+      <c r="BK30" s="39"/>
+      <c r="BL30" s="39"/>
+      <c r="BM30" s="39"/>
+      <c r="BN30" s="39"/>
+      <c r="BO30" s="39"/>
+      <c r="BP30" s="39"/>
+      <c r="BQ30" s="39"/>
+      <c r="BR30" s="39"/>
+      <c r="BS30" s="39"/>
+      <c r="BT30" s="39"/>
+      <c r="BU30" s="39"/>
+      <c r="BV30" s="39"/>
+      <c r="BW30" s="39"/>
+      <c r="BX30" s="39"/>
+      <c r="BY30" s="39"/>
+      <c r="BZ30" s="39"/>
+      <c r="CA30" s="39"/>
+      <c r="CB30" s="39"/>
+      <c r="CC30" s="39"/>
+      <c r="CD30" s="39"/>
+      <c r="CE30" s="39"/>
+      <c r="CF30" s="39"/>
+      <c r="CG30" s="39"/>
+      <c r="CH30" s="39"/>
+      <c r="CI30" s="39"/>
+      <c r="CJ30" s="39"/>
+      <c r="CK30" s="39"/>
+      <c r="CL30" s="39"/>
+      <c r="CM30" s="39"/>
+      <c r="CN30" s="39"/>
+      <c r="CO30" s="39"/>
+      <c r="CP30" s="39"/>
+      <c r="CQ30" s="39"/>
+      <c r="CR30" s="39"/>
+      <c r="CS30" s="39"/>
+      <c r="CT30" s="39"/>
+      <c r="CU30" s="39"/>
+      <c r="CV30" s="39"/>
+      <c r="CW30" s="39"/>
+      <c r="CX30" s="39"/>
+      <c r="CY30" s="39"/>
+      <c r="CZ30" s="39"/>
+      <c r="DA30" s="39"/>
+      <c r="DB30" s="39"/>
+      <c r="DC30" s="39"/>
+      <c r="DD30" s="39"/>
+      <c r="DE30" s="39"/>
+      <c r="DF30" s="39"/>
       <c r="DG30" s="39"/>
       <c r="DH30" s="39"/>
     </row>
     <row r="31" spans="3:112" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C31" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="DG31" s="39"/>
       <c r="DH31" s="39"/>
     </row>
     <row r="32" spans="3:112" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="DG32" s="39"/>
+      <c r="DH32" s="39"/>
+    </row>
+    <row r="33" spans="3:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="DG32" s="39"/>
-      <c r="DH32" s="52" t="s">
+      <c r="DG33" s="39"/>
+      <c r="DH33" s="52" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="3:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C33" s="5"/>
-    </row>
     <row r="34" spans="3:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="3:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="34" t="s">
         <v>69</v>
-      </c>
-      <c r="CY34" s="39"/>
-      <c r="CZ34" s="39"/>
-      <c r="DA34" s="39"/>
-      <c r="DB34" s="39"/>
-      <c r="DC34" s="39"/>
-      <c r="DD34" s="39"/>
-      <c r="DE34" s="39"/>
-      <c r="DF34" s="39"/>
-      <c r="DG34" s="39"/>
-      <c r="DH34" s="39"/>
-      <c r="DI34" s="39"/>
-      <c r="DJ34" s="39"/>
-      <c r="DK34" s="39"/>
-      <c r="DL34" s="39"/>
-      <c r="DM34" s="58" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="35" spans="3:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C35" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="CY35" s="39"/>
       <c r="CZ35" s="39"/>
@@ -9932,10 +10054,17 @@
       <c r="DF35" s="39"/>
       <c r="DG35" s="39"/>
       <c r="DH35" s="39"/>
+      <c r="DI35" s="39"/>
+      <c r="DJ35" s="39"/>
+      <c r="DK35" s="39"/>
+      <c r="DL35" s="39"/>
+      <c r="DM35" s="58" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="36" spans="3:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C36" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="CY36" s="39"/>
       <c r="CZ36" s="39"/>
@@ -9950,67 +10079,42 @@
     </row>
     <row r="37" spans="3:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C37" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="CY37" s="39"/>
+      <c r="CZ37" s="39"/>
+      <c r="DA37" s="39"/>
+      <c r="DB37" s="39"/>
       <c r="DC37" s="39"/>
       <c r="DD37" s="39"/>
       <c r="DE37" s="39"/>
       <c r="DF37" s="39"/>
       <c r="DG37" s="39"/>
       <c r="DH37" s="39"/>
-      <c r="DI37" s="39"/>
-      <c r="DJ37" s="39"/>
-      <c r="DK37" s="39"/>
-      <c r="DL37" s="39"/>
-    </row>
-    <row r="39" spans="3:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C39" s="5" t="s">
+    </row>
+    <row r="38" spans="3:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="DC38" s="39"/>
+      <c r="DD38" s="39"/>
+      <c r="DE38" s="39"/>
+      <c r="DF38" s="39"/>
+      <c r="DG38" s="39"/>
+      <c r="DH38" s="39"/>
+      <c r="DI38" s="39"/>
+      <c r="DJ38" s="39"/>
+      <c r="DK38" s="39"/>
+      <c r="DL38" s="39"/>
+    </row>
+    <row r="40" spans="3:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C40" s="5" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="40" spans="3:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C40" s="60" t="s">
-        <v>255</v>
-      </c>
-      <c r="BB40" s="39"/>
-      <c r="BC40" s="39"/>
-      <c r="BD40" s="39"/>
-      <c r="BE40" s="39"/>
-      <c r="BF40" s="39"/>
-      <c r="BG40" s="39"/>
-      <c r="BH40" s="39"/>
-      <c r="BI40" s="39"/>
-      <c r="BJ40" s="39"/>
-      <c r="BK40" s="39"/>
-      <c r="BL40" s="39"/>
-      <c r="BM40" s="39"/>
-      <c r="BN40" s="39"/>
-      <c r="BO40" s="39"/>
-      <c r="BP40" s="39"/>
-      <c r="BQ40" s="39"/>
-      <c r="BR40" s="39"/>
-      <c r="BS40" s="39"/>
-      <c r="BT40" s="39"/>
-      <c r="BU40" s="39"/>
-      <c r="BV40" s="39"/>
-      <c r="BW40" s="39"/>
-      <c r="BX40" s="39"/>
-      <c r="BY40" s="39"/>
-      <c r="BZ40" s="39"/>
-      <c r="CA40" s="39"/>
-      <c r="CB40" s="39"/>
-      <c r="CC40" s="39"/>
-      <c r="CD40" s="39"/>
-      <c r="CE40" s="39"/>
-      <c r="CF40" s="39"/>
-      <c r="CG40" s="39"/>
-      <c r="CH40" s="39"/>
-      <c r="CI40" s="39"/>
-      <c r="CJ40" s="39"/>
     </row>
     <row r="41" spans="3:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C41" s="60" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="BB41" s="39"/>
       <c r="BC41" s="39"/>
@@ -10050,7 +10154,7 @@
     </row>
     <row r="42" spans="3:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C42" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="BB42" s="39"/>
       <c r="BC42" s="39"/>
@@ -10089,8 +10193,8 @@
       <c r="CJ42" s="39"/>
     </row>
     <row r="43" spans="3:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C43" s="61" t="s">
-        <v>259</v>
+      <c r="C43" s="60" t="s">
+        <v>257</v>
       </c>
       <c r="BB43" s="39"/>
       <c r="BC43" s="39"/>
@@ -10127,19 +10231,52 @@
       <c r="CH43" s="39"/>
       <c r="CI43" s="39"/>
       <c r="CJ43" s="39"/>
-      <c r="CK43" s="52" t="s">
+    </row>
+    <row r="44" spans="3:117" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C44" s="61" t="s">
+        <v>259</v>
+      </c>
+      <c r="BB44" s="39"/>
+      <c r="BC44" s="39"/>
+      <c r="BD44" s="39"/>
+      <c r="BE44" s="39"/>
+      <c r="BF44" s="39"/>
+      <c r="BG44" s="39"/>
+      <c r="BH44" s="39"/>
+      <c r="BI44" s="39"/>
+      <c r="BJ44" s="39"/>
+      <c r="BK44" s="39"/>
+      <c r="BL44" s="39"/>
+      <c r="BM44" s="39"/>
+      <c r="BN44" s="39"/>
+      <c r="BO44" s="39"/>
+      <c r="BP44" s="39"/>
+      <c r="BQ44" s="39"/>
+      <c r="BR44" s="39"/>
+      <c r="BS44" s="39"/>
+      <c r="BT44" s="39"/>
+      <c r="BU44" s="39"/>
+      <c r="BV44" s="39"/>
+      <c r="BW44" s="39"/>
+      <c r="BX44" s="39"/>
+      <c r="BY44" s="39"/>
+      <c r="BZ44" s="39"/>
+      <c r="CA44" s="39"/>
+      <c r="CB44" s="39"/>
+      <c r="CC44" s="39"/>
+      <c r="CD44" s="39"/>
+      <c r="CE44" s="39"/>
+      <c r="CF44" s="39"/>
+      <c r="CG44" s="39"/>
+      <c r="CH44" s="39"/>
+      <c r="CI44" s="39"/>
+      <c r="CJ44" s="39"/>
+      <c r="CK44" s="52" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AN1:AT1"/>
-    <mergeCell ref="AU1:BA1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AM1"/>
     <mergeCell ref="EH1:EN1"/>
     <mergeCell ref="EO1:EU1"/>
     <mergeCell ref="EV1:FB1"/>
@@ -10155,6 +10292,13 @@
     <mergeCell ref="DM1:DS1"/>
     <mergeCell ref="DT1:DZ1"/>
     <mergeCell ref="EA1:EG1"/>
+    <mergeCell ref="AN1:AT1"/>
+    <mergeCell ref="AU1:BA1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
gespeicherten Spielstand bei Reload beibehalten
</commit_message>
<xml_diff>
--- a/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
+++ b/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Besitzer\Dropbox\Studium\Semester 6\FRONT\FRONT_Projekt\front-projekt\documents\Projektmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1FAAF0-8899-4067-AA60-84175D29AB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA17ABF-8DFC-440D-B850-8FA977C56ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1247,6 +1247,9 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1255,9 +1258,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="180"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1490,8 +1490,8 @@
   <dimension ref="A1:V81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K50" sqref="K50"/>
+      <pane ySplit="7" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="H6" s="30">
         <f>SUM(H10:H77)</f>
-        <v>85.5</v>
+        <v>87</v>
       </c>
       <c r="I6" s="27">
         <f>SUM(I10:I77)</f>
@@ -1662,7 +1662,7 @@
       </c>
       <c r="H7" s="30">
         <f t="shared" ref="H7:J7" si="1">H5-H6</f>
-        <v>34.5</v>
+        <v>33</v>
       </c>
       <c r="I7" s="27">
         <f t="shared" si="1"/>
@@ -3026,7 +3026,7 @@
         <v>262</v>
       </c>
       <c r="H54" s="22">
-        <v>3.75</v>
+        <v>5.25</v>
       </c>
       <c r="I54" s="22">
         <v>1</v>
@@ -3741,141 +3741,141 @@
   <sheetData>
     <row r="1" spans="1:166" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="1"/>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="68" t="s">
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="68" t="s">
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="69"/>
-      <c r="X1" s="69"/>
-      <c r="Y1" s="69"/>
-      <c r="Z1" s="68" t="s">
+      <c r="T1" s="70"/>
+      <c r="U1" s="70"/>
+      <c r="V1" s="70"/>
+      <c r="W1" s="70"/>
+      <c r="X1" s="70"/>
+      <c r="Y1" s="70"/>
+      <c r="Z1" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="AA1" s="69"/>
-      <c r="AB1" s="69"/>
-      <c r="AC1" s="69"/>
-      <c r="AD1" s="69"/>
-      <c r="AE1" s="69"/>
-      <c r="AF1" s="69"/>
-      <c r="AG1" s="68" t="s">
+      <c r="AA1" s="70"/>
+      <c r="AB1" s="70"/>
+      <c r="AC1" s="70"/>
+      <c r="AD1" s="70"/>
+      <c r="AE1" s="70"/>
+      <c r="AF1" s="70"/>
+      <c r="AG1" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="AH1" s="69"/>
-      <c r="AI1" s="69"/>
-      <c r="AJ1" s="69"/>
-      <c r="AK1" s="69"/>
-      <c r="AL1" s="69"/>
-      <c r="AM1" s="69"/>
-      <c r="AN1" s="66" t="s">
+      <c r="AH1" s="70"/>
+      <c r="AI1" s="70"/>
+      <c r="AJ1" s="70"/>
+      <c r="AK1" s="70"/>
+      <c r="AL1" s="70"/>
+      <c r="AM1" s="70"/>
+      <c r="AN1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="66" t="s">
+      <c r="AO1" s="68"/>
+      <c r="AP1" s="68"/>
+      <c r="AQ1" s="68"/>
+      <c r="AR1" s="68"/>
+      <c r="AS1" s="68"/>
+      <c r="AT1" s="68"/>
+      <c r="AU1" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="AV1" s="67"/>
-      <c r="AW1" s="67"/>
-      <c r="AX1" s="67"/>
-      <c r="AY1" s="67"/>
-      <c r="AZ1" s="67"/>
-      <c r="BA1" s="67"/>
-      <c r="BB1" s="66" t="s">
+      <c r="AV1" s="68"/>
+      <c r="AW1" s="68"/>
+      <c r="AX1" s="68"/>
+      <c r="AY1" s="68"/>
+      <c r="AZ1" s="68"/>
+      <c r="BA1" s="68"/>
+      <c r="BB1" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="BC1" s="67"/>
-      <c r="BD1" s="67"/>
-      <c r="BE1" s="67"/>
-      <c r="BF1" s="67"/>
-      <c r="BG1" s="67"/>
-      <c r="BH1" s="67"/>
-      <c r="BI1" s="66" t="s">
+      <c r="BC1" s="68"/>
+      <c r="BD1" s="68"/>
+      <c r="BE1" s="68"/>
+      <c r="BF1" s="68"/>
+      <c r="BG1" s="68"/>
+      <c r="BH1" s="68"/>
+      <c r="BI1" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="BJ1" s="67"/>
-      <c r="BK1" s="67"/>
-      <c r="BL1" s="67"/>
-      <c r="BM1" s="67"/>
-      <c r="BN1" s="67"/>
-      <c r="BO1" s="67"/>
-      <c r="BP1" s="66" t="s">
+      <c r="BJ1" s="68"/>
+      <c r="BK1" s="68"/>
+      <c r="BL1" s="68"/>
+      <c r="BM1" s="68"/>
+      <c r="BN1" s="68"/>
+      <c r="BO1" s="68"/>
+      <c r="BP1" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="BQ1" s="67"/>
-      <c r="BR1" s="67"/>
-      <c r="BS1" s="67"/>
-      <c r="BT1" s="67"/>
-      <c r="BU1" s="67"/>
-      <c r="BV1" s="67"/>
-      <c r="BW1" s="66" t="s">
+      <c r="BQ1" s="68"/>
+      <c r="BR1" s="68"/>
+      <c r="BS1" s="68"/>
+      <c r="BT1" s="68"/>
+      <c r="BU1" s="68"/>
+      <c r="BV1" s="68"/>
+      <c r="BW1" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="BX1" s="67"/>
-      <c r="BY1" s="67"/>
-      <c r="BZ1" s="67"/>
-      <c r="CA1" s="67"/>
-      <c r="CB1" s="67"/>
-      <c r="CC1" s="67"/>
-      <c r="CD1" s="66" t="s">
+      <c r="BX1" s="68"/>
+      <c r="BY1" s="68"/>
+      <c r="BZ1" s="68"/>
+      <c r="CA1" s="68"/>
+      <c r="CB1" s="68"/>
+      <c r="CC1" s="68"/>
+      <c r="CD1" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="CE1" s="67"/>
-      <c r="CF1" s="67"/>
-      <c r="CG1" s="67"/>
-      <c r="CH1" s="67"/>
-      <c r="CI1" s="67"/>
-      <c r="CJ1" s="67"/>
-      <c r="CK1" s="66" t="s">
+      <c r="CE1" s="68"/>
+      <c r="CF1" s="68"/>
+      <c r="CG1" s="68"/>
+      <c r="CH1" s="68"/>
+      <c r="CI1" s="68"/>
+      <c r="CJ1" s="68"/>
+      <c r="CK1" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="CL1" s="67"/>
-      <c r="CM1" s="67"/>
-      <c r="CN1" s="67"/>
-      <c r="CO1" s="67"/>
-      <c r="CP1" s="67"/>
-      <c r="CQ1" s="67"/>
-      <c r="CR1" s="66" t="s">
+      <c r="CL1" s="68"/>
+      <c r="CM1" s="68"/>
+      <c r="CN1" s="68"/>
+      <c r="CO1" s="68"/>
+      <c r="CP1" s="68"/>
+      <c r="CQ1" s="68"/>
+      <c r="CR1" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="CS1" s="67"/>
-      <c r="CT1" s="67"/>
-      <c r="CU1" s="67"/>
-      <c r="CV1" s="67"/>
-      <c r="CW1" s="67"/>
-      <c r="CX1" s="67"/>
-      <c r="CY1" s="66" t="s">
+      <c r="CS1" s="68"/>
+      <c r="CT1" s="68"/>
+      <c r="CU1" s="68"/>
+      <c r="CV1" s="68"/>
+      <c r="CW1" s="68"/>
+      <c r="CX1" s="68"/>
+      <c r="CY1" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="CZ1" s="67"/>
-      <c r="DA1" s="67"/>
-      <c r="DB1" s="67"/>
-      <c r="DC1" s="67"/>
-      <c r="DD1" s="67"/>
-      <c r="DE1" s="67"/>
+      <c r="CZ1" s="68"/>
+      <c r="DA1" s="68"/>
+      <c r="DB1" s="68"/>
+      <c r="DC1" s="68"/>
+      <c r="DD1" s="68"/>
+      <c r="DE1" s="68"/>
       <c r="DF1" s="2"/>
       <c r="DG1" s="2"/>
       <c r="DH1" s="2"/>
@@ -5350,7 +5350,7 @@
     </row>
     <row r="46" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
-      <c r="B46" s="70" t="s">
+      <c r="B46" s="66" t="s">
         <v>54</v>
       </c>
       <c r="C46" s="15" t="s">
@@ -5359,21 +5359,21 @@
     </row>
     <row r="47" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
-      <c r="B47" s="70"/>
+      <c r="B47" s="66"/>
       <c r="C47" s="15" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
-      <c r="B48" s="70"/>
+      <c r="B48" s="66"/>
       <c r="C48" s="15" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A49" s="6"/>
-      <c r="B49" s="70"/>
+      <c r="B49" s="66"/>
       <c r="C49" s="15" t="s">
         <v>224</v>
       </c>
@@ -5383,229 +5383,229 @@
     </row>
     <row r="50" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A50" s="6"/>
-      <c r="B50" s="70"/>
+      <c r="B50" s="66"/>
       <c r="C50" s="15" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A51" s="6"/>
-      <c r="B51" s="70"/>
+      <c r="B51" s="66"/>
       <c r="C51" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B52" s="70"/>
+      <c r="B52" s="66"/>
       <c r="C52" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B53" s="70"/>
+      <c r="B53" s="66"/>
       <c r="C53" s="15" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A54" s="6"/>
-      <c r="B54" s="70"/>
+      <c r="B54" s="66"/>
       <c r="C54" s="15" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A55" s="6"/>
-      <c r="B55" s="70"/>
+      <c r="B55" s="66"/>
       <c r="C55" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A56" s="6"/>
-      <c r="B56" s="70"/>
+      <c r="B56" s="66"/>
       <c r="C56" s="15" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
-      <c r="B57" s="70"/>
+      <c r="B57" s="66"/>
       <c r="C57" s="15" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="70"/>
+      <c r="B58" s="66"/>
       <c r="C58" s="15" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B59" s="70"/>
+      <c r="B59" s="66"/>
       <c r="C59" s="15" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="60" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B60" s="70"/>
+      <c r="B60" s="66"/>
       <c r="C60" s="15" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="61" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B61" s="70"/>
+      <c r="B61" s="66"/>
       <c r="C61" s="15" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B62" s="70"/>
+      <c r="B62" s="66"/>
       <c r="C62" s="59" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="63" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B63" s="70"/>
+      <c r="B63" s="66"/>
       <c r="C63" s="65" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="64" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B64" s="70"/>
+      <c r="B64" s="66"/>
       <c r="C64" s="65" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B65" s="70"/>
+      <c r="B65" s="66"/>
       <c r="C65" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B66" s="70"/>
+      <c r="B66" s="66"/>
       <c r="C66" s="15" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B67" s="70"/>
+      <c r="B67" s="66"/>
       <c r="C67" s="15"/>
     </row>
     <row r="68" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B68" s="70"/>
+      <c r="B68" s="66"/>
       <c r="C68" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B69" s="70"/>
+      <c r="B69" s="66"/>
       <c r="C69" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B70" s="70"/>
+      <c r="B70" s="66"/>
       <c r="C70" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="71" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B71" s="70"/>
+      <c r="B71" s="66"/>
       <c r="C71" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="72" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B72" s="70"/>
+      <c r="B72" s="66"/>
       <c r="C72" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="73" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B73" s="70"/>
+      <c r="B73" s="66"/>
       <c r="C73" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="74" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B74" s="70"/>
+      <c r="B74" s="66"/>
       <c r="C74" s="15" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B75" s="70"/>
+      <c r="B75" s="66"/>
       <c r="C75" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B76" s="70"/>
+      <c r="B76" s="66"/>
       <c r="C76" s="15" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B77" s="70"/>
+      <c r="B77" s="66"/>
       <c r="C77" s="16"/>
     </row>
     <row r="78" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B78" s="70"/>
+      <c r="B78" s="66"/>
       <c r="C78" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B79" s="70"/>
+      <c r="B79" s="66"/>
       <c r="C79" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B80" s="70"/>
+      <c r="B80" s="66"/>
       <c r="C80" s="15" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="81" spans="2:75" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B81" s="70"/>
+      <c r="B81" s="66"/>
       <c r="C81" s="15" t="s">
         <v>72</v>
       </c>
       <c r="BA81" s="6"/>
     </row>
     <row r="82" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B82" s="70"/>
+      <c r="B82" s="66"/>
       <c r="C82" s="16"/>
     </row>
     <row r="83" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B83" s="70"/>
+      <c r="B83" s="66"/>
       <c r="C83" s="15" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="84" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B84" s="70"/>
+      <c r="B84" s="66"/>
       <c r="C84" s="59" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="85" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B85" s="70"/>
+      <c r="B85" s="66"/>
       <c r="C85" s="59" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="86" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B86" s="70"/>
+      <c r="B86" s="66"/>
       <c r="C86" s="59" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="87" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B87" s="70"/>
+      <c r="B87" s="66"/>
       <c r="C87" s="15" t="s">
         <v>258</v>
       </c>
@@ -8360,6 +8360,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="CD1:CJ1"/>
     <mergeCell ref="B82:B87"/>
     <mergeCell ref="B46:B81"/>
     <mergeCell ref="CK1:CQ1"/>
@@ -8376,7 +8377,6 @@
     <mergeCell ref="BI1:BO1"/>
     <mergeCell ref="BP1:BV1"/>
     <mergeCell ref="BW1:CC1"/>
-    <mergeCell ref="CD1:CJ1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:J4 L4:CW4 CY4:EV4">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
@@ -8411,194 +8411,194 @@
   <sheetData>
     <row r="1" spans="1:158" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="1"/>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="66" t="s">
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="66" t="s">
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="67"/>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="66" t="s">
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="68"/>
+      <c r="W1" s="68"/>
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="67" t="s">
         <v>76</v>
       </c>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="67"/>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="66" t="s">
+      <c r="AA1" s="68"/>
+      <c r="AB1" s="68"/>
+      <c r="AC1" s="68"/>
+      <c r="AD1" s="68"/>
+      <c r="AE1" s="68"/>
+      <c r="AF1" s="68"/>
+      <c r="AG1" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="AH1" s="67"/>
-      <c r="AI1" s="67"/>
-      <c r="AJ1" s="67"/>
-      <c r="AK1" s="67"/>
-      <c r="AL1" s="67"/>
-      <c r="AM1" s="67"/>
-      <c r="AN1" s="66" t="s">
+      <c r="AH1" s="68"/>
+      <c r="AI1" s="68"/>
+      <c r="AJ1" s="68"/>
+      <c r="AK1" s="68"/>
+      <c r="AL1" s="68"/>
+      <c r="AM1" s="68"/>
+      <c r="AN1" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="66" t="s">
+      <c r="AO1" s="68"/>
+      <c r="AP1" s="68"/>
+      <c r="AQ1" s="68"/>
+      <c r="AR1" s="68"/>
+      <c r="AS1" s="68"/>
+      <c r="AT1" s="68"/>
+      <c r="AU1" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="AV1" s="67"/>
-      <c r="AW1" s="67"/>
-      <c r="AX1" s="67"/>
-      <c r="AY1" s="67"/>
-      <c r="AZ1" s="67"/>
-      <c r="BA1" s="67"/>
-      <c r="BB1" s="66" t="s">
+      <c r="AV1" s="68"/>
+      <c r="AW1" s="68"/>
+      <c r="AX1" s="68"/>
+      <c r="AY1" s="68"/>
+      <c r="AZ1" s="68"/>
+      <c r="BA1" s="68"/>
+      <c r="BB1" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="BC1" s="67"/>
-      <c r="BD1" s="67"/>
-      <c r="BE1" s="67"/>
-      <c r="BF1" s="67"/>
-      <c r="BG1" s="67"/>
-      <c r="BH1" s="67"/>
-      <c r="BI1" s="66" t="s">
+      <c r="BC1" s="68"/>
+      <c r="BD1" s="68"/>
+      <c r="BE1" s="68"/>
+      <c r="BF1" s="68"/>
+      <c r="BG1" s="68"/>
+      <c r="BH1" s="68"/>
+      <c r="BI1" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="BJ1" s="67"/>
-      <c r="BK1" s="67"/>
-      <c r="BL1" s="67"/>
-      <c r="BM1" s="67"/>
-      <c r="BN1" s="67"/>
-      <c r="BO1" s="67"/>
-      <c r="BP1" s="66" t="s">
+      <c r="BJ1" s="68"/>
+      <c r="BK1" s="68"/>
+      <c r="BL1" s="68"/>
+      <c r="BM1" s="68"/>
+      <c r="BN1" s="68"/>
+      <c r="BO1" s="68"/>
+      <c r="BP1" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="BQ1" s="67"/>
-      <c r="BR1" s="67"/>
-      <c r="BS1" s="67"/>
-      <c r="BT1" s="67"/>
-      <c r="BU1" s="67"/>
-      <c r="BV1" s="67"/>
-      <c r="BW1" s="66" t="s">
+      <c r="BQ1" s="68"/>
+      <c r="BR1" s="68"/>
+      <c r="BS1" s="68"/>
+      <c r="BT1" s="68"/>
+      <c r="BU1" s="68"/>
+      <c r="BV1" s="68"/>
+      <c r="BW1" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="BX1" s="67"/>
-      <c r="BY1" s="67"/>
-      <c r="BZ1" s="67"/>
-      <c r="CA1" s="67"/>
-      <c r="CB1" s="67"/>
-      <c r="CC1" s="67"/>
-      <c r="CD1" s="66" t="s">
+      <c r="BX1" s="68"/>
+      <c r="BY1" s="68"/>
+      <c r="BZ1" s="68"/>
+      <c r="CA1" s="68"/>
+      <c r="CB1" s="68"/>
+      <c r="CC1" s="68"/>
+      <c r="CD1" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="CE1" s="67"/>
-      <c r="CF1" s="67"/>
-      <c r="CG1" s="67"/>
-      <c r="CH1" s="67"/>
-      <c r="CI1" s="67"/>
-      <c r="CJ1" s="67"/>
-      <c r="CK1" s="66" t="s">
+      <c r="CE1" s="68"/>
+      <c r="CF1" s="68"/>
+      <c r="CG1" s="68"/>
+      <c r="CH1" s="68"/>
+      <c r="CI1" s="68"/>
+      <c r="CJ1" s="68"/>
+      <c r="CK1" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="CL1" s="67"/>
-      <c r="CM1" s="67"/>
-      <c r="CN1" s="67"/>
-      <c r="CO1" s="67"/>
-      <c r="CP1" s="67"/>
-      <c r="CQ1" s="67"/>
-      <c r="CR1" s="66" t="s">
+      <c r="CL1" s="68"/>
+      <c r="CM1" s="68"/>
+      <c r="CN1" s="68"/>
+      <c r="CO1" s="68"/>
+      <c r="CP1" s="68"/>
+      <c r="CQ1" s="68"/>
+      <c r="CR1" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="CS1" s="67"/>
-      <c r="CT1" s="67"/>
-      <c r="CU1" s="67"/>
-      <c r="CV1" s="67"/>
-      <c r="CW1" s="67"/>
-      <c r="CX1" s="67"/>
-      <c r="CY1" s="66" t="s">
+      <c r="CS1" s="68"/>
+      <c r="CT1" s="68"/>
+      <c r="CU1" s="68"/>
+      <c r="CV1" s="68"/>
+      <c r="CW1" s="68"/>
+      <c r="CX1" s="68"/>
+      <c r="CY1" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="CZ1" s="67"/>
-      <c r="DA1" s="67"/>
-      <c r="DB1" s="67"/>
-      <c r="DC1" s="67"/>
-      <c r="DD1" s="67"/>
-      <c r="DE1" s="67"/>
-      <c r="DF1" s="66" t="s">
+      <c r="CZ1" s="68"/>
+      <c r="DA1" s="68"/>
+      <c r="DB1" s="68"/>
+      <c r="DC1" s="68"/>
+      <c r="DD1" s="68"/>
+      <c r="DE1" s="68"/>
+      <c r="DF1" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="DG1" s="67"/>
-      <c r="DH1" s="67"/>
-      <c r="DI1" s="67"/>
-      <c r="DJ1" s="67"/>
-      <c r="DK1" s="67"/>
-      <c r="DL1" s="67"/>
-      <c r="DM1" s="66" t="s">
+      <c r="DG1" s="68"/>
+      <c r="DH1" s="68"/>
+      <c r="DI1" s="68"/>
+      <c r="DJ1" s="68"/>
+      <c r="DK1" s="68"/>
+      <c r="DL1" s="68"/>
+      <c r="DM1" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="DN1" s="67"/>
-      <c r="DO1" s="67"/>
-      <c r="DP1" s="67"/>
-      <c r="DQ1" s="67"/>
-      <c r="DR1" s="67"/>
-      <c r="DS1" s="67"/>
-      <c r="DT1" s="66"/>
-      <c r="DU1" s="67"/>
-      <c r="DV1" s="67"/>
-      <c r="DW1" s="67"/>
-      <c r="DX1" s="67"/>
-      <c r="DY1" s="67"/>
-      <c r="DZ1" s="67"/>
-      <c r="EA1" s="66"/>
-      <c r="EB1" s="67"/>
-      <c r="EC1" s="67"/>
-      <c r="ED1" s="67"/>
-      <c r="EE1" s="67"/>
-      <c r="EF1" s="67"/>
-      <c r="EG1" s="67"/>
-      <c r="EH1" s="66"/>
-      <c r="EI1" s="67"/>
-      <c r="EJ1" s="67"/>
-      <c r="EK1" s="67"/>
-      <c r="EL1" s="67"/>
-      <c r="EM1" s="67"/>
-      <c r="EN1" s="67"/>
-      <c r="EO1" s="66"/>
-      <c r="EP1" s="67"/>
-      <c r="EQ1" s="67"/>
-      <c r="ER1" s="67"/>
-      <c r="ES1" s="67"/>
-      <c r="ET1" s="67"/>
-      <c r="EU1" s="67"/>
-      <c r="EV1" s="66"/>
-      <c r="EW1" s="67"/>
-      <c r="EX1" s="67"/>
-      <c r="EY1" s="67"/>
-      <c r="EZ1" s="67"/>
-      <c r="FA1" s="67"/>
-      <c r="FB1" s="67"/>
+      <c r="DN1" s="68"/>
+      <c r="DO1" s="68"/>
+      <c r="DP1" s="68"/>
+      <c r="DQ1" s="68"/>
+      <c r="DR1" s="68"/>
+      <c r="DS1" s="68"/>
+      <c r="DT1" s="67"/>
+      <c r="DU1" s="68"/>
+      <c r="DV1" s="68"/>
+      <c r="DW1" s="68"/>
+      <c r="DX1" s="68"/>
+      <c r="DY1" s="68"/>
+      <c r="DZ1" s="68"/>
+      <c r="EA1" s="67"/>
+      <c r="EB1" s="68"/>
+      <c r="EC1" s="68"/>
+      <c r="ED1" s="68"/>
+      <c r="EE1" s="68"/>
+      <c r="EF1" s="68"/>
+      <c r="EG1" s="68"/>
+      <c r="EH1" s="67"/>
+      <c r="EI1" s="68"/>
+      <c r="EJ1" s="68"/>
+      <c r="EK1" s="68"/>
+      <c r="EL1" s="68"/>
+      <c r="EM1" s="68"/>
+      <c r="EN1" s="68"/>
+      <c r="EO1" s="67"/>
+      <c r="EP1" s="68"/>
+      <c r="EQ1" s="68"/>
+      <c r="ER1" s="68"/>
+      <c r="ES1" s="68"/>
+      <c r="ET1" s="68"/>
+      <c r="EU1" s="68"/>
+      <c r="EV1" s="67"/>
+      <c r="EW1" s="68"/>
+      <c r="EX1" s="68"/>
+      <c r="EY1" s="68"/>
+      <c r="EZ1" s="68"/>
+      <c r="FA1" s="68"/>
+      <c r="FB1" s="68"/>
     </row>
     <row r="2" spans="1:158" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="1"/>
@@ -10507,13 +10507,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AN1:AT1"/>
-    <mergeCell ref="AU1:BA1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AM1"/>
     <mergeCell ref="EH1:EN1"/>
     <mergeCell ref="EO1:EU1"/>
     <mergeCell ref="EV1:FB1"/>
@@ -10529,6 +10522,13 @@
     <mergeCell ref="DM1:DS1"/>
     <mergeCell ref="DT1:DZ1"/>
     <mergeCell ref="EA1:EG1"/>
+    <mergeCell ref="AN1:AT1"/>
+    <mergeCell ref="AU1:BA1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Spielername in Spielfiguranzeige darstellen
</commit_message>
<xml_diff>
--- a/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
+++ b/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Besitzer\Dropbox\Studium\Semester 6\FRONT\FRONT_Projekt\front-projekt\documents\Projektmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA17ABF-8DFC-440D-B850-8FA977C56ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8143C605-C894-4633-92AD-AF40DF86C579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1247,13 +1247,13 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="180"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1490,8 +1490,8 @@
   <dimension ref="A1:V81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
+      <pane ySplit="7" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="H6" s="30">
         <f>SUM(H10:H77)</f>
-        <v>87</v>
+        <v>87.5</v>
       </c>
       <c r="I6" s="27">
         <f>SUM(I10:I77)</f>
@@ -1662,7 +1662,7 @@
       </c>
       <c r="H7" s="30">
         <f t="shared" ref="H7:J7" si="1">H5-H6</f>
-        <v>33</v>
+        <v>32.5</v>
       </c>
       <c r="I7" s="27">
         <f t="shared" si="1"/>
@@ -2806,7 +2806,7 @@
         <v>206</v>
       </c>
       <c r="H46" s="22">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="I46" s="22"/>
       <c r="J46" s="22"/>
@@ -2885,7 +2885,9 @@
       <c r="G49" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="H49" s="22"/>
+      <c r="H49" s="22">
+        <v>0.25</v>
+      </c>
       <c r="I49" s="22">
         <v>1.5</v>
       </c>
@@ -3786,96 +3788,96 @@
       <c r="AK1" s="70"/>
       <c r="AL1" s="70"/>
       <c r="AM1" s="70"/>
-      <c r="AN1" s="67" t="s">
+      <c r="AN1" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="AO1" s="68"/>
-      <c r="AP1" s="68"/>
-      <c r="AQ1" s="68"/>
-      <c r="AR1" s="68"/>
-      <c r="AS1" s="68"/>
-      <c r="AT1" s="68"/>
-      <c r="AU1" s="67" t="s">
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="67"/>
+      <c r="AT1" s="67"/>
+      <c r="AU1" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="AV1" s="68"/>
-      <c r="AW1" s="68"/>
-      <c r="AX1" s="68"/>
-      <c r="AY1" s="68"/>
-      <c r="AZ1" s="68"/>
-      <c r="BA1" s="68"/>
-      <c r="BB1" s="67" t="s">
+      <c r="AV1" s="67"/>
+      <c r="AW1" s="67"/>
+      <c r="AX1" s="67"/>
+      <c r="AY1" s="67"/>
+      <c r="AZ1" s="67"/>
+      <c r="BA1" s="67"/>
+      <c r="BB1" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="BC1" s="68"/>
-      <c r="BD1" s="68"/>
-      <c r="BE1" s="68"/>
-      <c r="BF1" s="68"/>
-      <c r="BG1" s="68"/>
-      <c r="BH1" s="68"/>
-      <c r="BI1" s="67" t="s">
+      <c r="BC1" s="67"/>
+      <c r="BD1" s="67"/>
+      <c r="BE1" s="67"/>
+      <c r="BF1" s="67"/>
+      <c r="BG1" s="67"/>
+      <c r="BH1" s="67"/>
+      <c r="BI1" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="BJ1" s="68"/>
-      <c r="BK1" s="68"/>
-      <c r="BL1" s="68"/>
-      <c r="BM1" s="68"/>
-      <c r="BN1" s="68"/>
-      <c r="BO1" s="68"/>
-      <c r="BP1" s="67" t="s">
+      <c r="BJ1" s="67"/>
+      <c r="BK1" s="67"/>
+      <c r="BL1" s="67"/>
+      <c r="BM1" s="67"/>
+      <c r="BN1" s="67"/>
+      <c r="BO1" s="67"/>
+      <c r="BP1" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="BQ1" s="68"/>
-      <c r="BR1" s="68"/>
-      <c r="BS1" s="68"/>
-      <c r="BT1" s="68"/>
-      <c r="BU1" s="68"/>
-      <c r="BV1" s="68"/>
-      <c r="BW1" s="67" t="s">
+      <c r="BQ1" s="67"/>
+      <c r="BR1" s="67"/>
+      <c r="BS1" s="67"/>
+      <c r="BT1" s="67"/>
+      <c r="BU1" s="67"/>
+      <c r="BV1" s="67"/>
+      <c r="BW1" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="BX1" s="68"/>
-      <c r="BY1" s="68"/>
-      <c r="BZ1" s="68"/>
-      <c r="CA1" s="68"/>
-      <c r="CB1" s="68"/>
-      <c r="CC1" s="68"/>
-      <c r="CD1" s="67" t="s">
+      <c r="BX1" s="67"/>
+      <c r="BY1" s="67"/>
+      <c r="BZ1" s="67"/>
+      <c r="CA1" s="67"/>
+      <c r="CB1" s="67"/>
+      <c r="CC1" s="67"/>
+      <c r="CD1" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="CE1" s="68"/>
-      <c r="CF1" s="68"/>
-      <c r="CG1" s="68"/>
-      <c r="CH1" s="68"/>
-      <c r="CI1" s="68"/>
-      <c r="CJ1" s="68"/>
-      <c r="CK1" s="67" t="s">
+      <c r="CE1" s="67"/>
+      <c r="CF1" s="67"/>
+      <c r="CG1" s="67"/>
+      <c r="CH1" s="67"/>
+      <c r="CI1" s="67"/>
+      <c r="CJ1" s="67"/>
+      <c r="CK1" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="CL1" s="68"/>
-      <c r="CM1" s="68"/>
-      <c r="CN1" s="68"/>
-      <c r="CO1" s="68"/>
-      <c r="CP1" s="68"/>
-      <c r="CQ1" s="68"/>
-      <c r="CR1" s="67" t="s">
+      <c r="CL1" s="67"/>
+      <c r="CM1" s="67"/>
+      <c r="CN1" s="67"/>
+      <c r="CO1" s="67"/>
+      <c r="CP1" s="67"/>
+      <c r="CQ1" s="67"/>
+      <c r="CR1" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="CS1" s="68"/>
-      <c r="CT1" s="68"/>
-      <c r="CU1" s="68"/>
-      <c r="CV1" s="68"/>
-      <c r="CW1" s="68"/>
-      <c r="CX1" s="68"/>
-      <c r="CY1" s="67" t="s">
+      <c r="CS1" s="67"/>
+      <c r="CT1" s="67"/>
+      <c r="CU1" s="67"/>
+      <c r="CV1" s="67"/>
+      <c r="CW1" s="67"/>
+      <c r="CX1" s="67"/>
+      <c r="CY1" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="CZ1" s="68"/>
-      <c r="DA1" s="68"/>
-      <c r="DB1" s="68"/>
-      <c r="DC1" s="68"/>
-      <c r="DD1" s="68"/>
-      <c r="DE1" s="68"/>
+      <c r="CZ1" s="67"/>
+      <c r="DA1" s="67"/>
+      <c r="DB1" s="67"/>
+      <c r="DC1" s="67"/>
+      <c r="DD1" s="67"/>
+      <c r="DE1" s="67"/>
       <c r="DF1" s="2"/>
       <c r="DG1" s="2"/>
       <c r="DH1" s="2"/>
@@ -5350,7 +5352,7 @@
     </row>
     <row r="46" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
-      <c r="B46" s="66" t="s">
+      <c r="B46" s="68" t="s">
         <v>54</v>
       </c>
       <c r="C46" s="15" t="s">
@@ -5359,21 +5361,21 @@
     </row>
     <row r="47" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
-      <c r="B47" s="66"/>
+      <c r="B47" s="68"/>
       <c r="C47" s="15" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
-      <c r="B48" s="66"/>
+      <c r="B48" s="68"/>
       <c r="C48" s="15" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A49" s="6"/>
-      <c r="B49" s="66"/>
+      <c r="B49" s="68"/>
       <c r="C49" s="15" t="s">
         <v>224</v>
       </c>
@@ -5383,229 +5385,229 @@
     </row>
     <row r="50" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A50" s="6"/>
-      <c r="B50" s="66"/>
+      <c r="B50" s="68"/>
       <c r="C50" s="15" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A51" s="6"/>
-      <c r="B51" s="66"/>
+      <c r="B51" s="68"/>
       <c r="C51" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B52" s="66"/>
+      <c r="B52" s="68"/>
       <c r="C52" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B53" s="66"/>
+      <c r="B53" s="68"/>
       <c r="C53" s="15" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A54" s="6"/>
-      <c r="B54" s="66"/>
+      <c r="B54" s="68"/>
       <c r="C54" s="15" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A55" s="6"/>
-      <c r="B55" s="66"/>
+      <c r="B55" s="68"/>
       <c r="C55" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A56" s="6"/>
-      <c r="B56" s="66"/>
+      <c r="B56" s="68"/>
       <c r="C56" s="15" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
-      <c r="B57" s="66"/>
+      <c r="B57" s="68"/>
       <c r="C57" s="15" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="66"/>
+      <c r="B58" s="68"/>
       <c r="C58" s="15" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B59" s="66"/>
+      <c r="B59" s="68"/>
       <c r="C59" s="15" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="60" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B60" s="66"/>
+      <c r="B60" s="68"/>
       <c r="C60" s="15" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="61" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B61" s="66"/>
+      <c r="B61" s="68"/>
       <c r="C61" s="15" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B62" s="66"/>
+      <c r="B62" s="68"/>
       <c r="C62" s="59" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="63" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B63" s="66"/>
+      <c r="B63" s="68"/>
       <c r="C63" s="65" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="64" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B64" s="66"/>
+      <c r="B64" s="68"/>
       <c r="C64" s="65" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B65" s="66"/>
+      <c r="B65" s="68"/>
       <c r="C65" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B66" s="66"/>
+      <c r="B66" s="68"/>
       <c r="C66" s="15" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B67" s="66"/>
+      <c r="B67" s="68"/>
       <c r="C67" s="15"/>
     </row>
     <row r="68" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B68" s="66"/>
+      <c r="B68" s="68"/>
       <c r="C68" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B69" s="66"/>
+      <c r="B69" s="68"/>
       <c r="C69" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B70" s="66"/>
+      <c r="B70" s="68"/>
       <c r="C70" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="71" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B71" s="66"/>
+      <c r="B71" s="68"/>
       <c r="C71" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="72" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B72" s="66"/>
+      <c r="B72" s="68"/>
       <c r="C72" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="73" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B73" s="66"/>
+      <c r="B73" s="68"/>
       <c r="C73" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="74" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B74" s="66"/>
+      <c r="B74" s="68"/>
       <c r="C74" s="15" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B75" s="66"/>
+      <c r="B75" s="68"/>
       <c r="C75" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B76" s="66"/>
+      <c r="B76" s="68"/>
       <c r="C76" s="15" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B77" s="66"/>
+      <c r="B77" s="68"/>
       <c r="C77" s="16"/>
     </row>
     <row r="78" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B78" s="66"/>
+      <c r="B78" s="68"/>
       <c r="C78" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B79" s="66"/>
+      <c r="B79" s="68"/>
       <c r="C79" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B80" s="66"/>
+      <c r="B80" s="68"/>
       <c r="C80" s="15" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="81" spans="2:75" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B81" s="66"/>
+      <c r="B81" s="68"/>
       <c r="C81" s="15" t="s">
         <v>72</v>
       </c>
       <c r="BA81" s="6"/>
     </row>
     <row r="82" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B82" s="66"/>
+      <c r="B82" s="68"/>
       <c r="C82" s="16"/>
     </row>
     <row r="83" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B83" s="66"/>
+      <c r="B83" s="68"/>
       <c r="C83" s="15" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="84" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B84" s="66"/>
+      <c r="B84" s="68"/>
       <c r="C84" s="59" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="85" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B85" s="66"/>
+      <c r="B85" s="68"/>
       <c r="C85" s="59" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="86" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B86" s="66"/>
+      <c r="B86" s="68"/>
       <c r="C86" s="59" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="87" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B87" s="66"/>
+      <c r="B87" s="68"/>
       <c r="C87" s="15" t="s">
         <v>258</v>
       </c>
@@ -8360,11 +8362,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="CD1:CJ1"/>
-    <mergeCell ref="B82:B87"/>
-    <mergeCell ref="B46:B81"/>
-    <mergeCell ref="CK1:CQ1"/>
-    <mergeCell ref="CR1:CX1"/>
     <mergeCell ref="CY1:DE1"/>
     <mergeCell ref="E1:K1"/>
     <mergeCell ref="L1:R1"/>
@@ -8377,6 +8374,11 @@
     <mergeCell ref="BI1:BO1"/>
     <mergeCell ref="BP1:BV1"/>
     <mergeCell ref="BW1:CC1"/>
+    <mergeCell ref="CD1:CJ1"/>
+    <mergeCell ref="B82:B87"/>
+    <mergeCell ref="B46:B81"/>
+    <mergeCell ref="CK1:CQ1"/>
+    <mergeCell ref="CR1:CX1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:J4 L4:CW4 CY4:EV4">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
@@ -8411,194 +8413,194 @@
   <sheetData>
     <row r="1" spans="1:158" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="1"/>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="67" t="s">
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="67" t="s">
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="67" t="s">
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="AA1" s="68"/>
-      <c r="AB1" s="68"/>
-      <c r="AC1" s="68"/>
-      <c r="AD1" s="68"/>
-      <c r="AE1" s="68"/>
-      <c r="AF1" s="68"/>
-      <c r="AG1" s="67" t="s">
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="AH1" s="68"/>
-      <c r="AI1" s="68"/>
-      <c r="AJ1" s="68"/>
-      <c r="AK1" s="68"/>
-      <c r="AL1" s="68"/>
-      <c r="AM1" s="68"/>
-      <c r="AN1" s="67" t="s">
+      <c r="AH1" s="67"/>
+      <c r="AI1" s="67"/>
+      <c r="AJ1" s="67"/>
+      <c r="AK1" s="67"/>
+      <c r="AL1" s="67"/>
+      <c r="AM1" s="67"/>
+      <c r="AN1" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="AO1" s="68"/>
-      <c r="AP1" s="68"/>
-      <c r="AQ1" s="68"/>
-      <c r="AR1" s="68"/>
-      <c r="AS1" s="68"/>
-      <c r="AT1" s="68"/>
-      <c r="AU1" s="67" t="s">
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="67"/>
+      <c r="AT1" s="67"/>
+      <c r="AU1" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="AV1" s="68"/>
-      <c r="AW1" s="68"/>
-      <c r="AX1" s="68"/>
-      <c r="AY1" s="68"/>
-      <c r="AZ1" s="68"/>
-      <c r="BA1" s="68"/>
-      <c r="BB1" s="67" t="s">
+      <c r="AV1" s="67"/>
+      <c r="AW1" s="67"/>
+      <c r="AX1" s="67"/>
+      <c r="AY1" s="67"/>
+      <c r="AZ1" s="67"/>
+      <c r="BA1" s="67"/>
+      <c r="BB1" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="BC1" s="68"/>
-      <c r="BD1" s="68"/>
-      <c r="BE1" s="68"/>
-      <c r="BF1" s="68"/>
-      <c r="BG1" s="68"/>
-      <c r="BH1" s="68"/>
-      <c r="BI1" s="67" t="s">
+      <c r="BC1" s="67"/>
+      <c r="BD1" s="67"/>
+      <c r="BE1" s="67"/>
+      <c r="BF1" s="67"/>
+      <c r="BG1" s="67"/>
+      <c r="BH1" s="67"/>
+      <c r="BI1" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="BJ1" s="68"/>
-      <c r="BK1" s="68"/>
-      <c r="BL1" s="68"/>
-      <c r="BM1" s="68"/>
-      <c r="BN1" s="68"/>
-      <c r="BO1" s="68"/>
-      <c r="BP1" s="67" t="s">
+      <c r="BJ1" s="67"/>
+      <c r="BK1" s="67"/>
+      <c r="BL1" s="67"/>
+      <c r="BM1" s="67"/>
+      <c r="BN1" s="67"/>
+      <c r="BO1" s="67"/>
+      <c r="BP1" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="BQ1" s="68"/>
-      <c r="BR1" s="68"/>
-      <c r="BS1" s="68"/>
-      <c r="BT1" s="68"/>
-      <c r="BU1" s="68"/>
-      <c r="BV1" s="68"/>
-      <c r="BW1" s="67" t="s">
+      <c r="BQ1" s="67"/>
+      <c r="BR1" s="67"/>
+      <c r="BS1" s="67"/>
+      <c r="BT1" s="67"/>
+      <c r="BU1" s="67"/>
+      <c r="BV1" s="67"/>
+      <c r="BW1" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="BX1" s="68"/>
-      <c r="BY1" s="68"/>
-      <c r="BZ1" s="68"/>
-      <c r="CA1" s="68"/>
-      <c r="CB1" s="68"/>
-      <c r="CC1" s="68"/>
-      <c r="CD1" s="67" t="s">
+      <c r="BX1" s="67"/>
+      <c r="BY1" s="67"/>
+      <c r="BZ1" s="67"/>
+      <c r="CA1" s="67"/>
+      <c r="CB1" s="67"/>
+      <c r="CC1" s="67"/>
+      <c r="CD1" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="CE1" s="68"/>
-      <c r="CF1" s="68"/>
-      <c r="CG1" s="68"/>
-      <c r="CH1" s="68"/>
-      <c r="CI1" s="68"/>
-      <c r="CJ1" s="68"/>
-      <c r="CK1" s="67" t="s">
+      <c r="CE1" s="67"/>
+      <c r="CF1" s="67"/>
+      <c r="CG1" s="67"/>
+      <c r="CH1" s="67"/>
+      <c r="CI1" s="67"/>
+      <c r="CJ1" s="67"/>
+      <c r="CK1" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="CL1" s="68"/>
-      <c r="CM1" s="68"/>
-      <c r="CN1" s="68"/>
-      <c r="CO1" s="68"/>
-      <c r="CP1" s="68"/>
-      <c r="CQ1" s="68"/>
-      <c r="CR1" s="67" t="s">
+      <c r="CL1" s="67"/>
+      <c r="CM1" s="67"/>
+      <c r="CN1" s="67"/>
+      <c r="CO1" s="67"/>
+      <c r="CP1" s="67"/>
+      <c r="CQ1" s="67"/>
+      <c r="CR1" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="CS1" s="68"/>
-      <c r="CT1" s="68"/>
-      <c r="CU1" s="68"/>
-      <c r="CV1" s="68"/>
-      <c r="CW1" s="68"/>
-      <c r="CX1" s="68"/>
-      <c r="CY1" s="67" t="s">
+      <c r="CS1" s="67"/>
+      <c r="CT1" s="67"/>
+      <c r="CU1" s="67"/>
+      <c r="CV1" s="67"/>
+      <c r="CW1" s="67"/>
+      <c r="CX1" s="67"/>
+      <c r="CY1" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="CZ1" s="68"/>
-      <c r="DA1" s="68"/>
-      <c r="DB1" s="68"/>
-      <c r="DC1" s="68"/>
-      <c r="DD1" s="68"/>
-      <c r="DE1" s="68"/>
-      <c r="DF1" s="67" t="s">
+      <c r="CZ1" s="67"/>
+      <c r="DA1" s="67"/>
+      <c r="DB1" s="67"/>
+      <c r="DC1" s="67"/>
+      <c r="DD1" s="67"/>
+      <c r="DE1" s="67"/>
+      <c r="DF1" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="DG1" s="68"/>
-      <c r="DH1" s="68"/>
-      <c r="DI1" s="68"/>
-      <c r="DJ1" s="68"/>
-      <c r="DK1" s="68"/>
-      <c r="DL1" s="68"/>
-      <c r="DM1" s="67" t="s">
+      <c r="DG1" s="67"/>
+      <c r="DH1" s="67"/>
+      <c r="DI1" s="67"/>
+      <c r="DJ1" s="67"/>
+      <c r="DK1" s="67"/>
+      <c r="DL1" s="67"/>
+      <c r="DM1" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="DN1" s="68"/>
-      <c r="DO1" s="68"/>
-      <c r="DP1" s="68"/>
-      <c r="DQ1" s="68"/>
-      <c r="DR1" s="68"/>
-      <c r="DS1" s="68"/>
-      <c r="DT1" s="67"/>
-      <c r="DU1" s="68"/>
-      <c r="DV1" s="68"/>
-      <c r="DW1" s="68"/>
-      <c r="DX1" s="68"/>
-      <c r="DY1" s="68"/>
-      <c r="DZ1" s="68"/>
-      <c r="EA1" s="67"/>
-      <c r="EB1" s="68"/>
-      <c r="EC1" s="68"/>
-      <c r="ED1" s="68"/>
-      <c r="EE1" s="68"/>
-      <c r="EF1" s="68"/>
-      <c r="EG1" s="68"/>
-      <c r="EH1" s="67"/>
-      <c r="EI1" s="68"/>
-      <c r="EJ1" s="68"/>
-      <c r="EK1" s="68"/>
-      <c r="EL1" s="68"/>
-      <c r="EM1" s="68"/>
-      <c r="EN1" s="68"/>
-      <c r="EO1" s="67"/>
-      <c r="EP1" s="68"/>
-      <c r="EQ1" s="68"/>
-      <c r="ER1" s="68"/>
-      <c r="ES1" s="68"/>
-      <c r="ET1" s="68"/>
-      <c r="EU1" s="68"/>
-      <c r="EV1" s="67"/>
-      <c r="EW1" s="68"/>
-      <c r="EX1" s="68"/>
-      <c r="EY1" s="68"/>
-      <c r="EZ1" s="68"/>
-      <c r="FA1" s="68"/>
-      <c r="FB1" s="68"/>
+      <c r="DN1" s="67"/>
+      <c r="DO1" s="67"/>
+      <c r="DP1" s="67"/>
+      <c r="DQ1" s="67"/>
+      <c r="DR1" s="67"/>
+      <c r="DS1" s="67"/>
+      <c r="DT1" s="66"/>
+      <c r="DU1" s="67"/>
+      <c r="DV1" s="67"/>
+      <c r="DW1" s="67"/>
+      <c r="DX1" s="67"/>
+      <c r="DY1" s="67"/>
+      <c r="DZ1" s="67"/>
+      <c r="EA1" s="66"/>
+      <c r="EB1" s="67"/>
+      <c r="EC1" s="67"/>
+      <c r="ED1" s="67"/>
+      <c r="EE1" s="67"/>
+      <c r="EF1" s="67"/>
+      <c r="EG1" s="67"/>
+      <c r="EH1" s="66"/>
+      <c r="EI1" s="67"/>
+      <c r="EJ1" s="67"/>
+      <c r="EK1" s="67"/>
+      <c r="EL1" s="67"/>
+      <c r="EM1" s="67"/>
+      <c r="EN1" s="67"/>
+      <c r="EO1" s="66"/>
+      <c r="EP1" s="67"/>
+      <c r="EQ1" s="67"/>
+      <c r="ER1" s="67"/>
+      <c r="ES1" s="67"/>
+      <c r="ET1" s="67"/>
+      <c r="EU1" s="67"/>
+      <c r="EV1" s="66"/>
+      <c r="EW1" s="67"/>
+      <c r="EX1" s="67"/>
+      <c r="EY1" s="67"/>
+      <c r="EZ1" s="67"/>
+      <c r="FA1" s="67"/>
+      <c r="FB1" s="67"/>
     </row>
     <row r="2" spans="1:158" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="1"/>
@@ -10507,6 +10509,13 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="AN1:AT1"/>
+    <mergeCell ref="AU1:BA1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AM1"/>
     <mergeCell ref="EH1:EN1"/>
     <mergeCell ref="EO1:EU1"/>
     <mergeCell ref="EV1:FB1"/>
@@ -10522,13 +10531,6 @@
     <mergeCell ref="DM1:DS1"/>
     <mergeCell ref="DT1:DZ1"/>
     <mergeCell ref="EA1:EG1"/>
-    <mergeCell ref="AN1:AT1"/>
-    <mergeCell ref="AU1:BA1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Option 'Nochmal spielen' nach Sieg
</commit_message>
<xml_diff>
--- a/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
+++ b/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Besitzer\Dropbox\Studium\Semester 6\FRONT\FRONT_Projekt\front-projekt\documents\Projektmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8143C605-C894-4633-92AD-AF40DF86C579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18C4025-27A4-4C6D-9CF6-DF87C1E2ECD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1251,13 +1251,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="180"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1490,8 +1490,8 @@
   <dimension ref="A1:V81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M50" sqref="M50"/>
+      <pane ySplit="7" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="H6" s="30">
         <f>SUM(H10:H77)</f>
-        <v>87.5</v>
+        <v>87.75</v>
       </c>
       <c r="I6" s="27">
         <f>SUM(I10:I77)</f>
@@ -1662,7 +1662,7 @@
       </c>
       <c r="H7" s="30">
         <f t="shared" ref="H7:J7" si="1">H5-H6</f>
-        <v>32.5</v>
+        <v>32.25</v>
       </c>
       <c r="I7" s="27">
         <f t="shared" si="1"/>
@@ -2976,7 +2976,7 @@
         <v>211</v>
       </c>
       <c r="H52" s="22">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="I52" s="22">
         <v>0.25</v>
@@ -3743,51 +3743,51 @@
   <sheetData>
     <row r="1" spans="1:166" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="1"/>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="69" t="s">
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="69" t="s">
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="70"/>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="69" t="s">
+      <c r="T1" s="69"/>
+      <c r="U1" s="69"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="69"/>
+      <c r="X1" s="69"/>
+      <c r="Y1" s="69"/>
+      <c r="Z1" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="70"/>
-      <c r="AD1" s="70"/>
-      <c r="AE1" s="70"/>
-      <c r="AF1" s="70"/>
-      <c r="AG1" s="69" t="s">
+      <c r="AA1" s="69"/>
+      <c r="AB1" s="69"/>
+      <c r="AC1" s="69"/>
+      <c r="AD1" s="69"/>
+      <c r="AE1" s="69"/>
+      <c r="AF1" s="69"/>
+      <c r="AG1" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="AH1" s="70"/>
-      <c r="AI1" s="70"/>
-      <c r="AJ1" s="70"/>
-      <c r="AK1" s="70"/>
-      <c r="AL1" s="70"/>
-      <c r="AM1" s="70"/>
+      <c r="AH1" s="69"/>
+      <c r="AI1" s="69"/>
+      <c r="AJ1" s="69"/>
+      <c r="AK1" s="69"/>
+      <c r="AL1" s="69"/>
+      <c r="AM1" s="69"/>
       <c r="AN1" s="66" t="s">
         <v>5</v>
       </c>
@@ -5352,7 +5352,7 @@
     </row>
     <row r="46" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
-      <c r="B46" s="68" t="s">
+      <c r="B46" s="70" t="s">
         <v>54</v>
       </c>
       <c r="C46" s="15" t="s">
@@ -5361,21 +5361,21 @@
     </row>
     <row r="47" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
-      <c r="B47" s="68"/>
+      <c r="B47" s="70"/>
       <c r="C47" s="15" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
-      <c r="B48" s="68"/>
+      <c r="B48" s="70"/>
       <c r="C48" s="15" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A49" s="6"/>
-      <c r="B49" s="68"/>
+      <c r="B49" s="70"/>
       <c r="C49" s="15" t="s">
         <v>224</v>
       </c>
@@ -5385,229 +5385,229 @@
     </row>
     <row r="50" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A50" s="6"/>
-      <c r="B50" s="68"/>
+      <c r="B50" s="70"/>
       <c r="C50" s="15" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A51" s="6"/>
-      <c r="B51" s="68"/>
+      <c r="B51" s="70"/>
       <c r="C51" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B52" s="68"/>
+      <c r="B52" s="70"/>
       <c r="C52" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B53" s="68"/>
+      <c r="B53" s="70"/>
       <c r="C53" s="15" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A54" s="6"/>
-      <c r="B54" s="68"/>
+      <c r="B54" s="70"/>
       <c r="C54" s="15" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A55" s="6"/>
-      <c r="B55" s="68"/>
+      <c r="B55" s="70"/>
       <c r="C55" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A56" s="6"/>
-      <c r="B56" s="68"/>
+      <c r="B56" s="70"/>
       <c r="C56" s="15" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
-      <c r="B57" s="68"/>
+      <c r="B57" s="70"/>
       <c r="C57" s="15" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="68"/>
+      <c r="B58" s="70"/>
       <c r="C58" s="15" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B59" s="68"/>
+      <c r="B59" s="70"/>
       <c r="C59" s="15" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="60" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B60" s="68"/>
+      <c r="B60" s="70"/>
       <c r="C60" s="15" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="61" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B61" s="68"/>
+      <c r="B61" s="70"/>
       <c r="C61" s="15" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B62" s="68"/>
+      <c r="B62" s="70"/>
       <c r="C62" s="59" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="63" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B63" s="68"/>
+      <c r="B63" s="70"/>
       <c r="C63" s="65" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="64" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B64" s="68"/>
+      <c r="B64" s="70"/>
       <c r="C64" s="65" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B65" s="68"/>
+      <c r="B65" s="70"/>
       <c r="C65" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B66" s="68"/>
+      <c r="B66" s="70"/>
       <c r="C66" s="15" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B67" s="68"/>
+      <c r="B67" s="70"/>
       <c r="C67" s="15"/>
     </row>
     <row r="68" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B68" s="68"/>
+      <c r="B68" s="70"/>
       <c r="C68" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B69" s="68"/>
+      <c r="B69" s="70"/>
       <c r="C69" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B70" s="68"/>
+      <c r="B70" s="70"/>
       <c r="C70" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="71" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B71" s="68"/>
+      <c r="B71" s="70"/>
       <c r="C71" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="72" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B72" s="68"/>
+      <c r="B72" s="70"/>
       <c r="C72" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="73" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B73" s="68"/>
+      <c r="B73" s="70"/>
       <c r="C73" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="74" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B74" s="68"/>
+      <c r="B74" s="70"/>
       <c r="C74" s="15" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B75" s="68"/>
+      <c r="B75" s="70"/>
       <c r="C75" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B76" s="68"/>
+      <c r="B76" s="70"/>
       <c r="C76" s="15" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B77" s="68"/>
+      <c r="B77" s="70"/>
       <c r="C77" s="16"/>
     </row>
     <row r="78" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B78" s="68"/>
+      <c r="B78" s="70"/>
       <c r="C78" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B79" s="68"/>
+      <c r="B79" s="70"/>
       <c r="C79" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B80" s="68"/>
+      <c r="B80" s="70"/>
       <c r="C80" s="15" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="81" spans="2:75" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B81" s="68"/>
+      <c r="B81" s="70"/>
       <c r="C81" s="15" t="s">
         <v>72</v>
       </c>
       <c r="BA81" s="6"/>
     </row>
     <row r="82" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B82" s="68"/>
+      <c r="B82" s="70"/>
       <c r="C82" s="16"/>
     </row>
     <row r="83" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B83" s="68"/>
+      <c r="B83" s="70"/>
       <c r="C83" s="15" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="84" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B84" s="68"/>
+      <c r="B84" s="70"/>
       <c r="C84" s="59" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="85" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B85" s="68"/>
+      <c r="B85" s="70"/>
       <c r="C85" s="59" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="86" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B86" s="68"/>
+      <c r="B86" s="70"/>
       <c r="C86" s="59" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="87" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B87" s="68"/>
+      <c r="B87" s="70"/>
       <c r="C87" s="15" t="s">
         <v>258</v>
       </c>
@@ -8362,6 +8362,10 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B82:B87"/>
+    <mergeCell ref="B46:B81"/>
+    <mergeCell ref="CK1:CQ1"/>
+    <mergeCell ref="CR1:CX1"/>
     <mergeCell ref="CY1:DE1"/>
     <mergeCell ref="E1:K1"/>
     <mergeCell ref="L1:R1"/>
@@ -8375,10 +8379,6 @@
     <mergeCell ref="BP1:BV1"/>
     <mergeCell ref="BW1:CC1"/>
     <mergeCell ref="CD1:CJ1"/>
-    <mergeCell ref="B82:B87"/>
-    <mergeCell ref="B46:B81"/>
-    <mergeCell ref="CK1:CQ1"/>
-    <mergeCell ref="CR1:CX1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:J4 L4:CW4 CY4:EV4">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
@@ -10509,13 +10509,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AN1:AT1"/>
-    <mergeCell ref="AU1:BA1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AM1"/>
     <mergeCell ref="EH1:EN1"/>
     <mergeCell ref="EO1:EU1"/>
     <mergeCell ref="EV1:FB1"/>
@@ -10531,6 +10524,13 @@
     <mergeCell ref="DM1:DS1"/>
     <mergeCell ref="DT1:DZ1"/>
     <mergeCell ref="EA1:EG1"/>
+    <mergeCell ref="AN1:AT1"/>
+    <mergeCell ref="AU1:BA1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Zwischenstand Drag & Drop: draggable und droppable nach Zug entfernen
</commit_message>
<xml_diff>
--- a/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
+++ b/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Besitzer\Dropbox\Studium\Semester 6\FRONT\FRONT_Projekt\front-projekt\documents\Projektmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43DA7E8-42F0-4707-B5E2-276CC1A25390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E71F537-2787-45EA-BFF6-3ED4E334344F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1247,6 +1247,9 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1255,9 +1258,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="180"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="H6" s="30">
         <f>SUM(H10:H77)</f>
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I6" s="27">
         <f>SUM(I10:I77)</f>
@@ -1662,7 +1662,7 @@
       </c>
       <c r="H7" s="30">
         <f t="shared" ref="H7:J7" si="1">H5-H6</f>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I7" s="27">
         <f t="shared" si="1"/>
@@ -2918,7 +2918,7 @@
         <v>209</v>
       </c>
       <c r="H50" s="22">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I50" s="22">
         <v>4.5</v>
@@ -3743,141 +3743,141 @@
   <sheetData>
     <row r="1" spans="1:166" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="1"/>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="68" t="s">
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="68" t="s">
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="69"/>
-      <c r="X1" s="69"/>
-      <c r="Y1" s="69"/>
-      <c r="Z1" s="68" t="s">
+      <c r="T1" s="70"/>
+      <c r="U1" s="70"/>
+      <c r="V1" s="70"/>
+      <c r="W1" s="70"/>
+      <c r="X1" s="70"/>
+      <c r="Y1" s="70"/>
+      <c r="Z1" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="AA1" s="69"/>
-      <c r="AB1" s="69"/>
-      <c r="AC1" s="69"/>
-      <c r="AD1" s="69"/>
-      <c r="AE1" s="69"/>
-      <c r="AF1" s="69"/>
-      <c r="AG1" s="68" t="s">
+      <c r="AA1" s="70"/>
+      <c r="AB1" s="70"/>
+      <c r="AC1" s="70"/>
+      <c r="AD1" s="70"/>
+      <c r="AE1" s="70"/>
+      <c r="AF1" s="70"/>
+      <c r="AG1" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="AH1" s="69"/>
-      <c r="AI1" s="69"/>
-      <c r="AJ1" s="69"/>
-      <c r="AK1" s="69"/>
-      <c r="AL1" s="69"/>
-      <c r="AM1" s="69"/>
-      <c r="AN1" s="66" t="s">
+      <c r="AH1" s="70"/>
+      <c r="AI1" s="70"/>
+      <c r="AJ1" s="70"/>
+      <c r="AK1" s="70"/>
+      <c r="AL1" s="70"/>
+      <c r="AM1" s="70"/>
+      <c r="AN1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="66" t="s">
+      <c r="AO1" s="68"/>
+      <c r="AP1" s="68"/>
+      <c r="AQ1" s="68"/>
+      <c r="AR1" s="68"/>
+      <c r="AS1" s="68"/>
+      <c r="AT1" s="68"/>
+      <c r="AU1" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="AV1" s="67"/>
-      <c r="AW1" s="67"/>
-      <c r="AX1" s="67"/>
-      <c r="AY1" s="67"/>
-      <c r="AZ1" s="67"/>
-      <c r="BA1" s="67"/>
-      <c r="BB1" s="66" t="s">
+      <c r="AV1" s="68"/>
+      <c r="AW1" s="68"/>
+      <c r="AX1" s="68"/>
+      <c r="AY1" s="68"/>
+      <c r="AZ1" s="68"/>
+      <c r="BA1" s="68"/>
+      <c r="BB1" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="BC1" s="67"/>
-      <c r="BD1" s="67"/>
-      <c r="BE1" s="67"/>
-      <c r="BF1" s="67"/>
-      <c r="BG1" s="67"/>
-      <c r="BH1" s="67"/>
-      <c r="BI1" s="66" t="s">
+      <c r="BC1" s="68"/>
+      <c r="BD1" s="68"/>
+      <c r="BE1" s="68"/>
+      <c r="BF1" s="68"/>
+      <c r="BG1" s="68"/>
+      <c r="BH1" s="68"/>
+      <c r="BI1" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="BJ1" s="67"/>
-      <c r="BK1" s="67"/>
-      <c r="BL1" s="67"/>
-      <c r="BM1" s="67"/>
-      <c r="BN1" s="67"/>
-      <c r="BO1" s="67"/>
-      <c r="BP1" s="66" t="s">
+      <c r="BJ1" s="68"/>
+      <c r="BK1" s="68"/>
+      <c r="BL1" s="68"/>
+      <c r="BM1" s="68"/>
+      <c r="BN1" s="68"/>
+      <c r="BO1" s="68"/>
+      <c r="BP1" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="BQ1" s="67"/>
-      <c r="BR1" s="67"/>
-      <c r="BS1" s="67"/>
-      <c r="BT1" s="67"/>
-      <c r="BU1" s="67"/>
-      <c r="BV1" s="67"/>
-      <c r="BW1" s="66" t="s">
+      <c r="BQ1" s="68"/>
+      <c r="BR1" s="68"/>
+      <c r="BS1" s="68"/>
+      <c r="BT1" s="68"/>
+      <c r="BU1" s="68"/>
+      <c r="BV1" s="68"/>
+      <c r="BW1" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="BX1" s="67"/>
-      <c r="BY1" s="67"/>
-      <c r="BZ1" s="67"/>
-      <c r="CA1" s="67"/>
-      <c r="CB1" s="67"/>
-      <c r="CC1" s="67"/>
-      <c r="CD1" s="66" t="s">
+      <c r="BX1" s="68"/>
+      <c r="BY1" s="68"/>
+      <c r="BZ1" s="68"/>
+      <c r="CA1" s="68"/>
+      <c r="CB1" s="68"/>
+      <c r="CC1" s="68"/>
+      <c r="CD1" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="CE1" s="67"/>
-      <c r="CF1" s="67"/>
-      <c r="CG1" s="67"/>
-      <c r="CH1" s="67"/>
-      <c r="CI1" s="67"/>
-      <c r="CJ1" s="67"/>
-      <c r="CK1" s="66" t="s">
+      <c r="CE1" s="68"/>
+      <c r="CF1" s="68"/>
+      <c r="CG1" s="68"/>
+      <c r="CH1" s="68"/>
+      <c r="CI1" s="68"/>
+      <c r="CJ1" s="68"/>
+      <c r="CK1" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="CL1" s="67"/>
-      <c r="CM1" s="67"/>
-      <c r="CN1" s="67"/>
-      <c r="CO1" s="67"/>
-      <c r="CP1" s="67"/>
-      <c r="CQ1" s="67"/>
-      <c r="CR1" s="66" t="s">
+      <c r="CL1" s="68"/>
+      <c r="CM1" s="68"/>
+      <c r="CN1" s="68"/>
+      <c r="CO1" s="68"/>
+      <c r="CP1" s="68"/>
+      <c r="CQ1" s="68"/>
+      <c r="CR1" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="CS1" s="67"/>
-      <c r="CT1" s="67"/>
-      <c r="CU1" s="67"/>
-      <c r="CV1" s="67"/>
-      <c r="CW1" s="67"/>
-      <c r="CX1" s="67"/>
-      <c r="CY1" s="66" t="s">
+      <c r="CS1" s="68"/>
+      <c r="CT1" s="68"/>
+      <c r="CU1" s="68"/>
+      <c r="CV1" s="68"/>
+      <c r="CW1" s="68"/>
+      <c r="CX1" s="68"/>
+      <c r="CY1" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="CZ1" s="67"/>
-      <c r="DA1" s="67"/>
-      <c r="DB1" s="67"/>
-      <c r="DC1" s="67"/>
-      <c r="DD1" s="67"/>
-      <c r="DE1" s="67"/>
+      <c r="CZ1" s="68"/>
+      <c r="DA1" s="68"/>
+      <c r="DB1" s="68"/>
+      <c r="DC1" s="68"/>
+      <c r="DD1" s="68"/>
+      <c r="DE1" s="68"/>
       <c r="DF1" s="2"/>
       <c r="DG1" s="2"/>
       <c r="DH1" s="2"/>
@@ -5352,7 +5352,7 @@
     </row>
     <row r="46" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
-      <c r="B46" s="70" t="s">
+      <c r="B46" s="66" t="s">
         <v>54</v>
       </c>
       <c r="C46" s="15" t="s">
@@ -5361,21 +5361,21 @@
     </row>
     <row r="47" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
-      <c r="B47" s="70"/>
+      <c r="B47" s="66"/>
       <c r="C47" s="15" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
-      <c r="B48" s="70"/>
+      <c r="B48" s="66"/>
       <c r="C48" s="15" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A49" s="6"/>
-      <c r="B49" s="70"/>
+      <c r="B49" s="66"/>
       <c r="C49" s="15" t="s">
         <v>224</v>
       </c>
@@ -5385,229 +5385,229 @@
     </row>
     <row r="50" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A50" s="6"/>
-      <c r="B50" s="70"/>
+      <c r="B50" s="66"/>
       <c r="C50" s="15" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A51" s="6"/>
-      <c r="B51" s="70"/>
+      <c r="B51" s="66"/>
       <c r="C51" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B52" s="70"/>
+      <c r="B52" s="66"/>
       <c r="C52" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B53" s="70"/>
+      <c r="B53" s="66"/>
       <c r="C53" s="15" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A54" s="6"/>
-      <c r="B54" s="70"/>
+      <c r="B54" s="66"/>
       <c r="C54" s="15" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A55" s="6"/>
-      <c r="B55" s="70"/>
+      <c r="B55" s="66"/>
       <c r="C55" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A56" s="6"/>
-      <c r="B56" s="70"/>
+      <c r="B56" s="66"/>
       <c r="C56" s="15" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
-      <c r="B57" s="70"/>
+      <c r="B57" s="66"/>
       <c r="C57" s="15" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="70"/>
+      <c r="B58" s="66"/>
       <c r="C58" s="15" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B59" s="70"/>
+      <c r="B59" s="66"/>
       <c r="C59" s="15" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="60" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B60" s="70"/>
+      <c r="B60" s="66"/>
       <c r="C60" s="15" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="61" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B61" s="70"/>
+      <c r="B61" s="66"/>
       <c r="C61" s="15" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B62" s="70"/>
+      <c r="B62" s="66"/>
       <c r="C62" s="59" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="63" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B63" s="70"/>
+      <c r="B63" s="66"/>
       <c r="C63" s="65" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="64" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B64" s="70"/>
+      <c r="B64" s="66"/>
       <c r="C64" s="65" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B65" s="70"/>
+      <c r="B65" s="66"/>
       <c r="C65" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B66" s="70"/>
+      <c r="B66" s="66"/>
       <c r="C66" s="15" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B67" s="70"/>
+      <c r="B67" s="66"/>
       <c r="C67" s="15"/>
     </row>
     <row r="68" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B68" s="70"/>
+      <c r="B68" s="66"/>
       <c r="C68" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B69" s="70"/>
+      <c r="B69" s="66"/>
       <c r="C69" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B70" s="70"/>
+      <c r="B70" s="66"/>
       <c r="C70" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="71" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B71" s="70"/>
+      <c r="B71" s="66"/>
       <c r="C71" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="72" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B72" s="70"/>
+      <c r="B72" s="66"/>
       <c r="C72" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="73" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B73" s="70"/>
+      <c r="B73" s="66"/>
       <c r="C73" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="74" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B74" s="70"/>
+      <c r="B74" s="66"/>
       <c r="C74" s="15" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B75" s="70"/>
+      <c r="B75" s="66"/>
       <c r="C75" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B76" s="70"/>
+      <c r="B76" s="66"/>
       <c r="C76" s="15" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B77" s="70"/>
+      <c r="B77" s="66"/>
       <c r="C77" s="16"/>
     </row>
     <row r="78" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B78" s="70"/>
+      <c r="B78" s="66"/>
       <c r="C78" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B79" s="70"/>
+      <c r="B79" s="66"/>
       <c r="C79" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B80" s="70"/>
+      <c r="B80" s="66"/>
       <c r="C80" s="15" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="81" spans="2:75" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B81" s="70"/>
+      <c r="B81" s="66"/>
       <c r="C81" s="15" t="s">
         <v>72</v>
       </c>
       <c r="BA81" s="6"/>
     </row>
     <row r="82" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B82" s="70"/>
+      <c r="B82" s="66"/>
       <c r="C82" s="16"/>
     </row>
     <row r="83" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B83" s="70"/>
+      <c r="B83" s="66"/>
       <c r="C83" s="15" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="84" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B84" s="70"/>
+      <c r="B84" s="66"/>
       <c r="C84" s="59" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="85" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B85" s="70"/>
+      <c r="B85" s="66"/>
       <c r="C85" s="59" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="86" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B86" s="70"/>
+      <c r="B86" s="66"/>
       <c r="C86" s="59" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="87" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B87" s="70"/>
+      <c r="B87" s="66"/>
       <c r="C87" s="15" t="s">
         <v>258</v>
       </c>
@@ -8362,6 +8362,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="CD1:CJ1"/>
     <mergeCell ref="B82:B87"/>
     <mergeCell ref="B46:B81"/>
     <mergeCell ref="CK1:CQ1"/>
@@ -8378,7 +8379,6 @@
     <mergeCell ref="BI1:BO1"/>
     <mergeCell ref="BP1:BV1"/>
     <mergeCell ref="BW1:CC1"/>
-    <mergeCell ref="CD1:CJ1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:J4 L4:CW4 CY4:EV4">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
@@ -8413,194 +8413,194 @@
   <sheetData>
     <row r="1" spans="1:158" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="1"/>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="66" t="s">
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="66" t="s">
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="67"/>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="66" t="s">
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="68"/>
+      <c r="W1" s="68"/>
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="67" t="s">
         <v>76</v>
       </c>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="67"/>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="66" t="s">
+      <c r="AA1" s="68"/>
+      <c r="AB1" s="68"/>
+      <c r="AC1" s="68"/>
+      <c r="AD1" s="68"/>
+      <c r="AE1" s="68"/>
+      <c r="AF1" s="68"/>
+      <c r="AG1" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="AH1" s="67"/>
-      <c r="AI1" s="67"/>
-      <c r="AJ1" s="67"/>
-      <c r="AK1" s="67"/>
-      <c r="AL1" s="67"/>
-      <c r="AM1" s="67"/>
-      <c r="AN1" s="66" t="s">
+      <c r="AH1" s="68"/>
+      <c r="AI1" s="68"/>
+      <c r="AJ1" s="68"/>
+      <c r="AK1" s="68"/>
+      <c r="AL1" s="68"/>
+      <c r="AM1" s="68"/>
+      <c r="AN1" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="66" t="s">
+      <c r="AO1" s="68"/>
+      <c r="AP1" s="68"/>
+      <c r="AQ1" s="68"/>
+      <c r="AR1" s="68"/>
+      <c r="AS1" s="68"/>
+      <c r="AT1" s="68"/>
+      <c r="AU1" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="AV1" s="67"/>
-      <c r="AW1" s="67"/>
-      <c r="AX1" s="67"/>
-      <c r="AY1" s="67"/>
-      <c r="AZ1" s="67"/>
-      <c r="BA1" s="67"/>
-      <c r="BB1" s="66" t="s">
+      <c r="AV1" s="68"/>
+      <c r="AW1" s="68"/>
+      <c r="AX1" s="68"/>
+      <c r="AY1" s="68"/>
+      <c r="AZ1" s="68"/>
+      <c r="BA1" s="68"/>
+      <c r="BB1" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="BC1" s="67"/>
-      <c r="BD1" s="67"/>
-      <c r="BE1" s="67"/>
-      <c r="BF1" s="67"/>
-      <c r="BG1" s="67"/>
-      <c r="BH1" s="67"/>
-      <c r="BI1" s="66" t="s">
+      <c r="BC1" s="68"/>
+      <c r="BD1" s="68"/>
+      <c r="BE1" s="68"/>
+      <c r="BF1" s="68"/>
+      <c r="BG1" s="68"/>
+      <c r="BH1" s="68"/>
+      <c r="BI1" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="BJ1" s="67"/>
-      <c r="BK1" s="67"/>
-      <c r="BL1" s="67"/>
-      <c r="BM1" s="67"/>
-      <c r="BN1" s="67"/>
-      <c r="BO1" s="67"/>
-      <c r="BP1" s="66" t="s">
+      <c r="BJ1" s="68"/>
+      <c r="BK1" s="68"/>
+      <c r="BL1" s="68"/>
+      <c r="BM1" s="68"/>
+      <c r="BN1" s="68"/>
+      <c r="BO1" s="68"/>
+      <c r="BP1" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="BQ1" s="67"/>
-      <c r="BR1" s="67"/>
-      <c r="BS1" s="67"/>
-      <c r="BT1" s="67"/>
-      <c r="BU1" s="67"/>
-      <c r="BV1" s="67"/>
-      <c r="BW1" s="66" t="s">
+      <c r="BQ1" s="68"/>
+      <c r="BR1" s="68"/>
+      <c r="BS1" s="68"/>
+      <c r="BT1" s="68"/>
+      <c r="BU1" s="68"/>
+      <c r="BV1" s="68"/>
+      <c r="BW1" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="BX1" s="67"/>
-      <c r="BY1" s="67"/>
-      <c r="BZ1" s="67"/>
-      <c r="CA1" s="67"/>
-      <c r="CB1" s="67"/>
-      <c r="CC1" s="67"/>
-      <c r="CD1" s="66" t="s">
+      <c r="BX1" s="68"/>
+      <c r="BY1" s="68"/>
+      <c r="BZ1" s="68"/>
+      <c r="CA1" s="68"/>
+      <c r="CB1" s="68"/>
+      <c r="CC1" s="68"/>
+      <c r="CD1" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="CE1" s="67"/>
-      <c r="CF1" s="67"/>
-      <c r="CG1" s="67"/>
-      <c r="CH1" s="67"/>
-      <c r="CI1" s="67"/>
-      <c r="CJ1" s="67"/>
-      <c r="CK1" s="66" t="s">
+      <c r="CE1" s="68"/>
+      <c r="CF1" s="68"/>
+      <c r="CG1" s="68"/>
+      <c r="CH1" s="68"/>
+      <c r="CI1" s="68"/>
+      <c r="CJ1" s="68"/>
+      <c r="CK1" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="CL1" s="67"/>
-      <c r="CM1" s="67"/>
-      <c r="CN1" s="67"/>
-      <c r="CO1" s="67"/>
-      <c r="CP1" s="67"/>
-      <c r="CQ1" s="67"/>
-      <c r="CR1" s="66" t="s">
+      <c r="CL1" s="68"/>
+      <c r="CM1" s="68"/>
+      <c r="CN1" s="68"/>
+      <c r="CO1" s="68"/>
+      <c r="CP1" s="68"/>
+      <c r="CQ1" s="68"/>
+      <c r="CR1" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="CS1" s="67"/>
-      <c r="CT1" s="67"/>
-      <c r="CU1" s="67"/>
-      <c r="CV1" s="67"/>
-      <c r="CW1" s="67"/>
-      <c r="CX1" s="67"/>
-      <c r="CY1" s="66" t="s">
+      <c r="CS1" s="68"/>
+      <c r="CT1" s="68"/>
+      <c r="CU1" s="68"/>
+      <c r="CV1" s="68"/>
+      <c r="CW1" s="68"/>
+      <c r="CX1" s="68"/>
+      <c r="CY1" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="CZ1" s="67"/>
-      <c r="DA1" s="67"/>
-      <c r="DB1" s="67"/>
-      <c r="DC1" s="67"/>
-      <c r="DD1" s="67"/>
-      <c r="DE1" s="67"/>
-      <c r="DF1" s="66" t="s">
+      <c r="CZ1" s="68"/>
+      <c r="DA1" s="68"/>
+      <c r="DB1" s="68"/>
+      <c r="DC1" s="68"/>
+      <c r="DD1" s="68"/>
+      <c r="DE1" s="68"/>
+      <c r="DF1" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="DG1" s="67"/>
-      <c r="DH1" s="67"/>
-      <c r="DI1" s="67"/>
-      <c r="DJ1" s="67"/>
-      <c r="DK1" s="67"/>
-      <c r="DL1" s="67"/>
-      <c r="DM1" s="66" t="s">
+      <c r="DG1" s="68"/>
+      <c r="DH1" s="68"/>
+      <c r="DI1" s="68"/>
+      <c r="DJ1" s="68"/>
+      <c r="DK1" s="68"/>
+      <c r="DL1" s="68"/>
+      <c r="DM1" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="DN1" s="67"/>
-      <c r="DO1" s="67"/>
-      <c r="DP1" s="67"/>
-      <c r="DQ1" s="67"/>
-      <c r="DR1" s="67"/>
-      <c r="DS1" s="67"/>
-      <c r="DT1" s="66"/>
-      <c r="DU1" s="67"/>
-      <c r="DV1" s="67"/>
-      <c r="DW1" s="67"/>
-      <c r="DX1" s="67"/>
-      <c r="DY1" s="67"/>
-      <c r="DZ1" s="67"/>
-      <c r="EA1" s="66"/>
-      <c r="EB1" s="67"/>
-      <c r="EC1" s="67"/>
-      <c r="ED1" s="67"/>
-      <c r="EE1" s="67"/>
-      <c r="EF1" s="67"/>
-      <c r="EG1" s="67"/>
-      <c r="EH1" s="66"/>
-      <c r="EI1" s="67"/>
-      <c r="EJ1" s="67"/>
-      <c r="EK1" s="67"/>
-      <c r="EL1" s="67"/>
-      <c r="EM1" s="67"/>
-      <c r="EN1" s="67"/>
-      <c r="EO1" s="66"/>
-      <c r="EP1" s="67"/>
-      <c r="EQ1" s="67"/>
-      <c r="ER1" s="67"/>
-      <c r="ES1" s="67"/>
-      <c r="ET1" s="67"/>
-      <c r="EU1" s="67"/>
-      <c r="EV1" s="66"/>
-      <c r="EW1" s="67"/>
-      <c r="EX1" s="67"/>
-      <c r="EY1" s="67"/>
-      <c r="EZ1" s="67"/>
-      <c r="FA1" s="67"/>
-      <c r="FB1" s="67"/>
+      <c r="DN1" s="68"/>
+      <c r="DO1" s="68"/>
+      <c r="DP1" s="68"/>
+      <c r="DQ1" s="68"/>
+      <c r="DR1" s="68"/>
+      <c r="DS1" s="68"/>
+      <c r="DT1" s="67"/>
+      <c r="DU1" s="68"/>
+      <c r="DV1" s="68"/>
+      <c r="DW1" s="68"/>
+      <c r="DX1" s="68"/>
+      <c r="DY1" s="68"/>
+      <c r="DZ1" s="68"/>
+      <c r="EA1" s="67"/>
+      <c r="EB1" s="68"/>
+      <c r="EC1" s="68"/>
+      <c r="ED1" s="68"/>
+      <c r="EE1" s="68"/>
+      <c r="EF1" s="68"/>
+      <c r="EG1" s="68"/>
+      <c r="EH1" s="67"/>
+      <c r="EI1" s="68"/>
+      <c r="EJ1" s="68"/>
+      <c r="EK1" s="68"/>
+      <c r="EL1" s="68"/>
+      <c r="EM1" s="68"/>
+      <c r="EN1" s="68"/>
+      <c r="EO1" s="67"/>
+      <c r="EP1" s="68"/>
+      <c r="EQ1" s="68"/>
+      <c r="ER1" s="68"/>
+      <c r="ES1" s="68"/>
+      <c r="ET1" s="68"/>
+      <c r="EU1" s="68"/>
+      <c r="EV1" s="67"/>
+      <c r="EW1" s="68"/>
+      <c r="EX1" s="68"/>
+      <c r="EY1" s="68"/>
+      <c r="EZ1" s="68"/>
+      <c r="FA1" s="68"/>
+      <c r="FB1" s="68"/>
     </row>
     <row r="2" spans="1:158" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="1"/>
@@ -10509,13 +10509,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AN1:AT1"/>
-    <mergeCell ref="AU1:BA1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AM1"/>
     <mergeCell ref="EH1:EN1"/>
     <mergeCell ref="EO1:EU1"/>
     <mergeCell ref="EV1:FB1"/>
@@ -10531,6 +10524,13 @@
     <mergeCell ref="DM1:DS1"/>
     <mergeCell ref="DT1:DZ1"/>
     <mergeCell ref="EA1:EG1"/>
+    <mergeCell ref="AN1:AT1"/>
+    <mergeCell ref="AU1:BA1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Zwischenstand drag & drop
</commit_message>
<xml_diff>
--- a/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
+++ b/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Besitzer\Dropbox\Studium\Semester 6\FRONT\FRONT_Projekt\front-projekt\documents\Projektmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E71F537-2787-45EA-BFF6-3ED4E334344F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934614E4-F651-4205-A927-CA219816E3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1247,13 +1247,13 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="180"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1626,15 +1626,15 @@
       </c>
       <c r="H6" s="30">
         <f>SUM(H10:H77)</f>
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I6" s="27">
         <f>SUM(I10:I77)</f>
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="J6" s="28">
         <f>SUM(J10:J77)</f>
-        <v>75.75</v>
+        <v>77.75</v>
       </c>
       <c r="K6" s="22"/>
       <c r="L6" s="22"/>
@@ -1662,15 +1662,15 @@
       </c>
       <c r="H7" s="30">
         <f t="shared" ref="H7:J7" si="1">H5-H6</f>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I7" s="27">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J7" s="28">
         <f t="shared" si="1"/>
-        <v>44.25</v>
+        <v>42.25</v>
       </c>
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
@@ -2918,13 +2918,13 @@
         <v>209</v>
       </c>
       <c r="H50" s="22">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I50" s="22">
-        <v>4.5</v>
+        <v>6.5</v>
       </c>
       <c r="J50" s="22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K50" s="22"/>
       <c r="L50" s="22"/>
@@ -3788,96 +3788,96 @@
       <c r="AK1" s="70"/>
       <c r="AL1" s="70"/>
       <c r="AM1" s="70"/>
-      <c r="AN1" s="67" t="s">
+      <c r="AN1" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="AO1" s="68"/>
-      <c r="AP1" s="68"/>
-      <c r="AQ1" s="68"/>
-      <c r="AR1" s="68"/>
-      <c r="AS1" s="68"/>
-      <c r="AT1" s="68"/>
-      <c r="AU1" s="67" t="s">
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="67"/>
+      <c r="AT1" s="67"/>
+      <c r="AU1" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="AV1" s="68"/>
-      <c r="AW1" s="68"/>
-      <c r="AX1" s="68"/>
-      <c r="AY1" s="68"/>
-      <c r="AZ1" s="68"/>
-      <c r="BA1" s="68"/>
-      <c r="BB1" s="67" t="s">
+      <c r="AV1" s="67"/>
+      <c r="AW1" s="67"/>
+      <c r="AX1" s="67"/>
+      <c r="AY1" s="67"/>
+      <c r="AZ1" s="67"/>
+      <c r="BA1" s="67"/>
+      <c r="BB1" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="BC1" s="68"/>
-      <c r="BD1" s="68"/>
-      <c r="BE1" s="68"/>
-      <c r="BF1" s="68"/>
-      <c r="BG1" s="68"/>
-      <c r="BH1" s="68"/>
-      <c r="BI1" s="67" t="s">
+      <c r="BC1" s="67"/>
+      <c r="BD1" s="67"/>
+      <c r="BE1" s="67"/>
+      <c r="BF1" s="67"/>
+      <c r="BG1" s="67"/>
+      <c r="BH1" s="67"/>
+      <c r="BI1" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="BJ1" s="68"/>
-      <c r="BK1" s="68"/>
-      <c r="BL1" s="68"/>
-      <c r="BM1" s="68"/>
-      <c r="BN1" s="68"/>
-      <c r="BO1" s="68"/>
-      <c r="BP1" s="67" t="s">
+      <c r="BJ1" s="67"/>
+      <c r="BK1" s="67"/>
+      <c r="BL1" s="67"/>
+      <c r="BM1" s="67"/>
+      <c r="BN1" s="67"/>
+      <c r="BO1" s="67"/>
+      <c r="BP1" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="BQ1" s="68"/>
-      <c r="BR1" s="68"/>
-      <c r="BS1" s="68"/>
-      <c r="BT1" s="68"/>
-      <c r="BU1" s="68"/>
-      <c r="BV1" s="68"/>
-      <c r="BW1" s="67" t="s">
+      <c r="BQ1" s="67"/>
+      <c r="BR1" s="67"/>
+      <c r="BS1" s="67"/>
+      <c r="BT1" s="67"/>
+      <c r="BU1" s="67"/>
+      <c r="BV1" s="67"/>
+      <c r="BW1" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="BX1" s="68"/>
-      <c r="BY1" s="68"/>
-      <c r="BZ1" s="68"/>
-      <c r="CA1" s="68"/>
-      <c r="CB1" s="68"/>
-      <c r="CC1" s="68"/>
-      <c r="CD1" s="67" t="s">
+      <c r="BX1" s="67"/>
+      <c r="BY1" s="67"/>
+      <c r="BZ1" s="67"/>
+      <c r="CA1" s="67"/>
+      <c r="CB1" s="67"/>
+      <c r="CC1" s="67"/>
+      <c r="CD1" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="CE1" s="68"/>
-      <c r="CF1" s="68"/>
-      <c r="CG1" s="68"/>
-      <c r="CH1" s="68"/>
-      <c r="CI1" s="68"/>
-      <c r="CJ1" s="68"/>
-      <c r="CK1" s="67" t="s">
+      <c r="CE1" s="67"/>
+      <c r="CF1" s="67"/>
+      <c r="CG1" s="67"/>
+      <c r="CH1" s="67"/>
+      <c r="CI1" s="67"/>
+      <c r="CJ1" s="67"/>
+      <c r="CK1" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="CL1" s="68"/>
-      <c r="CM1" s="68"/>
-      <c r="CN1" s="68"/>
-      <c r="CO1" s="68"/>
-      <c r="CP1" s="68"/>
-      <c r="CQ1" s="68"/>
-      <c r="CR1" s="67" t="s">
+      <c r="CL1" s="67"/>
+      <c r="CM1" s="67"/>
+      <c r="CN1" s="67"/>
+      <c r="CO1" s="67"/>
+      <c r="CP1" s="67"/>
+      <c r="CQ1" s="67"/>
+      <c r="CR1" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="CS1" s="68"/>
-      <c r="CT1" s="68"/>
-      <c r="CU1" s="68"/>
-      <c r="CV1" s="68"/>
-      <c r="CW1" s="68"/>
-      <c r="CX1" s="68"/>
-      <c r="CY1" s="67" t="s">
+      <c r="CS1" s="67"/>
+      <c r="CT1" s="67"/>
+      <c r="CU1" s="67"/>
+      <c r="CV1" s="67"/>
+      <c r="CW1" s="67"/>
+      <c r="CX1" s="67"/>
+      <c r="CY1" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="CZ1" s="68"/>
-      <c r="DA1" s="68"/>
-      <c r="DB1" s="68"/>
-      <c r="DC1" s="68"/>
-      <c r="DD1" s="68"/>
-      <c r="DE1" s="68"/>
+      <c r="CZ1" s="67"/>
+      <c r="DA1" s="67"/>
+      <c r="DB1" s="67"/>
+      <c r="DC1" s="67"/>
+      <c r="DD1" s="67"/>
+      <c r="DE1" s="67"/>
       <c r="DF1" s="2"/>
       <c r="DG1" s="2"/>
       <c r="DH1" s="2"/>
@@ -5352,7 +5352,7 @@
     </row>
     <row r="46" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
-      <c r="B46" s="66" t="s">
+      <c r="B46" s="68" t="s">
         <v>54</v>
       </c>
       <c r="C46" s="15" t="s">
@@ -5361,21 +5361,21 @@
     </row>
     <row r="47" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
-      <c r="B47" s="66"/>
+      <c r="B47" s="68"/>
       <c r="C47" s="15" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
-      <c r="B48" s="66"/>
+      <c r="B48" s="68"/>
       <c r="C48" s="15" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A49" s="6"/>
-      <c r="B49" s="66"/>
+      <c r="B49" s="68"/>
       <c r="C49" s="15" t="s">
         <v>224</v>
       </c>
@@ -5385,229 +5385,229 @@
     </row>
     <row r="50" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A50" s="6"/>
-      <c r="B50" s="66"/>
+      <c r="B50" s="68"/>
       <c r="C50" s="15" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A51" s="6"/>
-      <c r="B51" s="66"/>
+      <c r="B51" s="68"/>
       <c r="C51" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B52" s="66"/>
+      <c r="B52" s="68"/>
       <c r="C52" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B53" s="66"/>
+      <c r="B53" s="68"/>
       <c r="C53" s="15" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A54" s="6"/>
-      <c r="B54" s="66"/>
+      <c r="B54" s="68"/>
       <c r="C54" s="15" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A55" s="6"/>
-      <c r="B55" s="66"/>
+      <c r="B55" s="68"/>
       <c r="C55" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A56" s="6"/>
-      <c r="B56" s="66"/>
+      <c r="B56" s="68"/>
       <c r="C56" s="15" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
-      <c r="B57" s="66"/>
+      <c r="B57" s="68"/>
       <c r="C57" s="15" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="66"/>
+      <c r="B58" s="68"/>
       <c r="C58" s="15" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B59" s="66"/>
+      <c r="B59" s="68"/>
       <c r="C59" s="15" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="60" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B60" s="66"/>
+      <c r="B60" s="68"/>
       <c r="C60" s="15" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="61" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B61" s="66"/>
+      <c r="B61" s="68"/>
       <c r="C61" s="15" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B62" s="66"/>
+      <c r="B62" s="68"/>
       <c r="C62" s="59" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="63" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B63" s="66"/>
+      <c r="B63" s="68"/>
       <c r="C63" s="65" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="64" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B64" s="66"/>
+      <c r="B64" s="68"/>
       <c r="C64" s="65" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B65" s="66"/>
+      <c r="B65" s="68"/>
       <c r="C65" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B66" s="66"/>
+      <c r="B66" s="68"/>
       <c r="C66" s="15" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B67" s="66"/>
+      <c r="B67" s="68"/>
       <c r="C67" s="15"/>
     </row>
     <row r="68" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B68" s="66"/>
+      <c r="B68" s="68"/>
       <c r="C68" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B69" s="66"/>
+      <c r="B69" s="68"/>
       <c r="C69" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B70" s="66"/>
+      <c r="B70" s="68"/>
       <c r="C70" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="71" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B71" s="66"/>
+      <c r="B71" s="68"/>
       <c r="C71" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="72" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B72" s="66"/>
+      <c r="B72" s="68"/>
       <c r="C72" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="73" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B73" s="66"/>
+      <c r="B73" s="68"/>
       <c r="C73" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="74" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B74" s="66"/>
+      <c r="B74" s="68"/>
       <c r="C74" s="15" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B75" s="66"/>
+      <c r="B75" s="68"/>
       <c r="C75" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B76" s="66"/>
+      <c r="B76" s="68"/>
       <c r="C76" s="15" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B77" s="66"/>
+      <c r="B77" s="68"/>
       <c r="C77" s="16"/>
     </row>
     <row r="78" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B78" s="66"/>
+      <c r="B78" s="68"/>
       <c r="C78" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B79" s="66"/>
+      <c r="B79" s="68"/>
       <c r="C79" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B80" s="66"/>
+      <c r="B80" s="68"/>
       <c r="C80" s="15" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="81" spans="2:75" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B81" s="66"/>
+      <c r="B81" s="68"/>
       <c r="C81" s="15" t="s">
         <v>72</v>
       </c>
       <c r="BA81" s="6"/>
     </row>
     <row r="82" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B82" s="66"/>
+      <c r="B82" s="68"/>
       <c r="C82" s="16"/>
     </row>
     <row r="83" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B83" s="66"/>
+      <c r="B83" s="68"/>
       <c r="C83" s="15" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="84" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B84" s="66"/>
+      <c r="B84" s="68"/>
       <c r="C84" s="59" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="85" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B85" s="66"/>
+      <c r="B85" s="68"/>
       <c r="C85" s="59" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="86" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B86" s="66"/>
+      <c r="B86" s="68"/>
       <c r="C86" s="59" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="87" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B87" s="66"/>
+      <c r="B87" s="68"/>
       <c r="C87" s="15" t="s">
         <v>258</v>
       </c>
@@ -8362,11 +8362,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="CD1:CJ1"/>
-    <mergeCell ref="B82:B87"/>
-    <mergeCell ref="B46:B81"/>
-    <mergeCell ref="CK1:CQ1"/>
-    <mergeCell ref="CR1:CX1"/>
     <mergeCell ref="CY1:DE1"/>
     <mergeCell ref="E1:K1"/>
     <mergeCell ref="L1:R1"/>
@@ -8379,6 +8374,11 @@
     <mergeCell ref="BI1:BO1"/>
     <mergeCell ref="BP1:BV1"/>
     <mergeCell ref="BW1:CC1"/>
+    <mergeCell ref="CD1:CJ1"/>
+    <mergeCell ref="B82:B87"/>
+    <mergeCell ref="B46:B81"/>
+    <mergeCell ref="CK1:CQ1"/>
+    <mergeCell ref="CR1:CX1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:J4 L4:CW4 CY4:EV4">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
@@ -8413,194 +8413,194 @@
   <sheetData>
     <row r="1" spans="1:158" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="1"/>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="67" t="s">
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="67" t="s">
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="67" t="s">
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="AA1" s="68"/>
-      <c r="AB1" s="68"/>
-      <c r="AC1" s="68"/>
-      <c r="AD1" s="68"/>
-      <c r="AE1" s="68"/>
-      <c r="AF1" s="68"/>
-      <c r="AG1" s="67" t="s">
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="AH1" s="68"/>
-      <c r="AI1" s="68"/>
-      <c r="AJ1" s="68"/>
-      <c r="AK1" s="68"/>
-      <c r="AL1" s="68"/>
-      <c r="AM1" s="68"/>
-      <c r="AN1" s="67" t="s">
+      <c r="AH1" s="67"/>
+      <c r="AI1" s="67"/>
+      <c r="AJ1" s="67"/>
+      <c r="AK1" s="67"/>
+      <c r="AL1" s="67"/>
+      <c r="AM1" s="67"/>
+      <c r="AN1" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="AO1" s="68"/>
-      <c r="AP1" s="68"/>
-      <c r="AQ1" s="68"/>
-      <c r="AR1" s="68"/>
-      <c r="AS1" s="68"/>
-      <c r="AT1" s="68"/>
-      <c r="AU1" s="67" t="s">
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="67"/>
+      <c r="AT1" s="67"/>
+      <c r="AU1" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="AV1" s="68"/>
-      <c r="AW1" s="68"/>
-      <c r="AX1" s="68"/>
-      <c r="AY1" s="68"/>
-      <c r="AZ1" s="68"/>
-      <c r="BA1" s="68"/>
-      <c r="BB1" s="67" t="s">
+      <c r="AV1" s="67"/>
+      <c r="AW1" s="67"/>
+      <c r="AX1" s="67"/>
+      <c r="AY1" s="67"/>
+      <c r="AZ1" s="67"/>
+      <c r="BA1" s="67"/>
+      <c r="BB1" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="BC1" s="68"/>
-      <c r="BD1" s="68"/>
-      <c r="BE1" s="68"/>
-      <c r="BF1" s="68"/>
-      <c r="BG1" s="68"/>
-      <c r="BH1" s="68"/>
-      <c r="BI1" s="67" t="s">
+      <c r="BC1" s="67"/>
+      <c r="BD1" s="67"/>
+      <c r="BE1" s="67"/>
+      <c r="BF1" s="67"/>
+      <c r="BG1" s="67"/>
+      <c r="BH1" s="67"/>
+      <c r="BI1" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="BJ1" s="68"/>
-      <c r="BK1" s="68"/>
-      <c r="BL1" s="68"/>
-      <c r="BM1" s="68"/>
-      <c r="BN1" s="68"/>
-      <c r="BO1" s="68"/>
-      <c r="BP1" s="67" t="s">
+      <c r="BJ1" s="67"/>
+      <c r="BK1" s="67"/>
+      <c r="BL1" s="67"/>
+      <c r="BM1" s="67"/>
+      <c r="BN1" s="67"/>
+      <c r="BO1" s="67"/>
+      <c r="BP1" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="BQ1" s="68"/>
-      <c r="BR1" s="68"/>
-      <c r="BS1" s="68"/>
-      <c r="BT1" s="68"/>
-      <c r="BU1" s="68"/>
-      <c r="BV1" s="68"/>
-      <c r="BW1" s="67" t="s">
+      <c r="BQ1" s="67"/>
+      <c r="BR1" s="67"/>
+      <c r="BS1" s="67"/>
+      <c r="BT1" s="67"/>
+      <c r="BU1" s="67"/>
+      <c r="BV1" s="67"/>
+      <c r="BW1" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="BX1" s="68"/>
-      <c r="BY1" s="68"/>
-      <c r="BZ1" s="68"/>
-      <c r="CA1" s="68"/>
-      <c r="CB1" s="68"/>
-      <c r="CC1" s="68"/>
-      <c r="CD1" s="67" t="s">
+      <c r="BX1" s="67"/>
+      <c r="BY1" s="67"/>
+      <c r="BZ1" s="67"/>
+      <c r="CA1" s="67"/>
+      <c r="CB1" s="67"/>
+      <c r="CC1" s="67"/>
+      <c r="CD1" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="CE1" s="68"/>
-      <c r="CF1" s="68"/>
-      <c r="CG1" s="68"/>
-      <c r="CH1" s="68"/>
-      <c r="CI1" s="68"/>
-      <c r="CJ1" s="68"/>
-      <c r="CK1" s="67" t="s">
+      <c r="CE1" s="67"/>
+      <c r="CF1" s="67"/>
+      <c r="CG1" s="67"/>
+      <c r="CH1" s="67"/>
+      <c r="CI1" s="67"/>
+      <c r="CJ1" s="67"/>
+      <c r="CK1" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="CL1" s="68"/>
-      <c r="CM1" s="68"/>
-      <c r="CN1" s="68"/>
-      <c r="CO1" s="68"/>
-      <c r="CP1" s="68"/>
-      <c r="CQ1" s="68"/>
-      <c r="CR1" s="67" t="s">
+      <c r="CL1" s="67"/>
+      <c r="CM1" s="67"/>
+      <c r="CN1" s="67"/>
+      <c r="CO1" s="67"/>
+      <c r="CP1" s="67"/>
+      <c r="CQ1" s="67"/>
+      <c r="CR1" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="CS1" s="68"/>
-      <c r="CT1" s="68"/>
-      <c r="CU1" s="68"/>
-      <c r="CV1" s="68"/>
-      <c r="CW1" s="68"/>
-      <c r="CX1" s="68"/>
-      <c r="CY1" s="67" t="s">
+      <c r="CS1" s="67"/>
+      <c r="CT1" s="67"/>
+      <c r="CU1" s="67"/>
+      <c r="CV1" s="67"/>
+      <c r="CW1" s="67"/>
+      <c r="CX1" s="67"/>
+      <c r="CY1" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="CZ1" s="68"/>
-      <c r="DA1" s="68"/>
-      <c r="DB1" s="68"/>
-      <c r="DC1" s="68"/>
-      <c r="DD1" s="68"/>
-      <c r="DE1" s="68"/>
-      <c r="DF1" s="67" t="s">
+      <c r="CZ1" s="67"/>
+      <c r="DA1" s="67"/>
+      <c r="DB1" s="67"/>
+      <c r="DC1" s="67"/>
+      <c r="DD1" s="67"/>
+      <c r="DE1" s="67"/>
+      <c r="DF1" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="DG1" s="68"/>
-      <c r="DH1" s="68"/>
-      <c r="DI1" s="68"/>
-      <c r="DJ1" s="68"/>
-      <c r="DK1" s="68"/>
-      <c r="DL1" s="68"/>
-      <c r="DM1" s="67" t="s">
+      <c r="DG1" s="67"/>
+      <c r="DH1" s="67"/>
+      <c r="DI1" s="67"/>
+      <c r="DJ1" s="67"/>
+      <c r="DK1" s="67"/>
+      <c r="DL1" s="67"/>
+      <c r="DM1" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="DN1" s="68"/>
-      <c r="DO1" s="68"/>
-      <c r="DP1" s="68"/>
-      <c r="DQ1" s="68"/>
-      <c r="DR1" s="68"/>
-      <c r="DS1" s="68"/>
-      <c r="DT1" s="67"/>
-      <c r="DU1" s="68"/>
-      <c r="DV1" s="68"/>
-      <c r="DW1" s="68"/>
-      <c r="DX1" s="68"/>
-      <c r="DY1" s="68"/>
-      <c r="DZ1" s="68"/>
-      <c r="EA1" s="67"/>
-      <c r="EB1" s="68"/>
-      <c r="EC1" s="68"/>
-      <c r="ED1" s="68"/>
-      <c r="EE1" s="68"/>
-      <c r="EF1" s="68"/>
-      <c r="EG1" s="68"/>
-      <c r="EH1" s="67"/>
-      <c r="EI1" s="68"/>
-      <c r="EJ1" s="68"/>
-      <c r="EK1" s="68"/>
-      <c r="EL1" s="68"/>
-      <c r="EM1" s="68"/>
-      <c r="EN1" s="68"/>
-      <c r="EO1" s="67"/>
-      <c r="EP1" s="68"/>
-      <c r="EQ1" s="68"/>
-      <c r="ER1" s="68"/>
-      <c r="ES1" s="68"/>
-      <c r="ET1" s="68"/>
-      <c r="EU1" s="68"/>
-      <c r="EV1" s="67"/>
-      <c r="EW1" s="68"/>
-      <c r="EX1" s="68"/>
-      <c r="EY1" s="68"/>
-      <c r="EZ1" s="68"/>
-      <c r="FA1" s="68"/>
-      <c r="FB1" s="68"/>
+      <c r="DN1" s="67"/>
+      <c r="DO1" s="67"/>
+      <c r="DP1" s="67"/>
+      <c r="DQ1" s="67"/>
+      <c r="DR1" s="67"/>
+      <c r="DS1" s="67"/>
+      <c r="DT1" s="66"/>
+      <c r="DU1" s="67"/>
+      <c r="DV1" s="67"/>
+      <c r="DW1" s="67"/>
+      <c r="DX1" s="67"/>
+      <c r="DY1" s="67"/>
+      <c r="DZ1" s="67"/>
+      <c r="EA1" s="66"/>
+      <c r="EB1" s="67"/>
+      <c r="EC1" s="67"/>
+      <c r="ED1" s="67"/>
+      <c r="EE1" s="67"/>
+      <c r="EF1" s="67"/>
+      <c r="EG1" s="67"/>
+      <c r="EH1" s="66"/>
+      <c r="EI1" s="67"/>
+      <c r="EJ1" s="67"/>
+      <c r="EK1" s="67"/>
+      <c r="EL1" s="67"/>
+      <c r="EM1" s="67"/>
+      <c r="EN1" s="67"/>
+      <c r="EO1" s="66"/>
+      <c r="EP1" s="67"/>
+      <c r="EQ1" s="67"/>
+      <c r="ER1" s="67"/>
+      <c r="ES1" s="67"/>
+      <c r="ET1" s="67"/>
+      <c r="EU1" s="67"/>
+      <c r="EV1" s="66"/>
+      <c r="EW1" s="67"/>
+      <c r="EX1" s="67"/>
+      <c r="EY1" s="67"/>
+      <c r="EZ1" s="67"/>
+      <c r="FA1" s="67"/>
+      <c r="FB1" s="67"/>
     </row>
     <row r="2" spans="1:158" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="1"/>
@@ -10509,6 +10509,13 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="AN1:AT1"/>
+    <mergeCell ref="AU1:BA1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AM1"/>
     <mergeCell ref="EH1:EN1"/>
     <mergeCell ref="EO1:EU1"/>
     <mergeCell ref="EV1:FB1"/>
@@ -10524,13 +10531,6 @@
     <mergeCell ref="DM1:DS1"/>
     <mergeCell ref="DT1:DZ1"/>
     <mergeCell ref="EA1:EG1"/>
-    <mergeCell ref="AN1:AT1"/>
-    <mergeCell ref="AU1:BA1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Zwischenstand drag & drop"
This reverts commit 4e7116fdef7292d54f57de44233b8282e9c1f7bc
</commit_message>
<xml_diff>
--- a/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
+++ b/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Besitzer\Dropbox\Studium\Semester 6\FRONT\FRONT_Projekt\front-projekt\documents\Projektmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934614E4-F651-4205-A927-CA219816E3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E71F537-2787-45EA-BFF6-3ED4E334344F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1247,13 +1247,13 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="180"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1626,15 +1626,15 @@
       </c>
       <c r="H6" s="30">
         <f>SUM(H10:H77)</f>
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I6" s="27">
         <f>SUM(I10:I77)</f>
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J6" s="28">
         <f>SUM(J10:J77)</f>
-        <v>77.75</v>
+        <v>75.75</v>
       </c>
       <c r="K6" s="22"/>
       <c r="L6" s="22"/>
@@ -1662,15 +1662,15 @@
       </c>
       <c r="H7" s="30">
         <f t="shared" ref="H7:J7" si="1">H5-H6</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I7" s="27">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J7" s="28">
         <f t="shared" si="1"/>
-        <v>42.25</v>
+        <v>44.25</v>
       </c>
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
@@ -2918,13 +2918,13 @@
         <v>209</v>
       </c>
       <c r="H50" s="22">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I50" s="22">
-        <v>6.5</v>
+        <v>4.5</v>
       </c>
       <c r="J50" s="22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K50" s="22"/>
       <c r="L50" s="22"/>
@@ -3788,96 +3788,96 @@
       <c r="AK1" s="70"/>
       <c r="AL1" s="70"/>
       <c r="AM1" s="70"/>
-      <c r="AN1" s="66" t="s">
+      <c r="AN1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="66" t="s">
+      <c r="AO1" s="68"/>
+      <c r="AP1" s="68"/>
+      <c r="AQ1" s="68"/>
+      <c r="AR1" s="68"/>
+      <c r="AS1" s="68"/>
+      <c r="AT1" s="68"/>
+      <c r="AU1" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="AV1" s="67"/>
-      <c r="AW1" s="67"/>
-      <c r="AX1" s="67"/>
-      <c r="AY1" s="67"/>
-      <c r="AZ1" s="67"/>
-      <c r="BA1" s="67"/>
-      <c r="BB1" s="66" t="s">
+      <c r="AV1" s="68"/>
+      <c r="AW1" s="68"/>
+      <c r="AX1" s="68"/>
+      <c r="AY1" s="68"/>
+      <c r="AZ1" s="68"/>
+      <c r="BA1" s="68"/>
+      <c r="BB1" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="BC1" s="67"/>
-      <c r="BD1" s="67"/>
-      <c r="BE1" s="67"/>
-      <c r="BF1" s="67"/>
-      <c r="BG1" s="67"/>
-      <c r="BH1" s="67"/>
-      <c r="BI1" s="66" t="s">
+      <c r="BC1" s="68"/>
+      <c r="BD1" s="68"/>
+      <c r="BE1" s="68"/>
+      <c r="BF1" s="68"/>
+      <c r="BG1" s="68"/>
+      <c r="BH1" s="68"/>
+      <c r="BI1" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="BJ1" s="67"/>
-      <c r="BK1" s="67"/>
-      <c r="BL1" s="67"/>
-      <c r="BM1" s="67"/>
-      <c r="BN1" s="67"/>
-      <c r="BO1" s="67"/>
-      <c r="BP1" s="66" t="s">
+      <c r="BJ1" s="68"/>
+      <c r="BK1" s="68"/>
+      <c r="BL1" s="68"/>
+      <c r="BM1" s="68"/>
+      <c r="BN1" s="68"/>
+      <c r="BO1" s="68"/>
+      <c r="BP1" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="BQ1" s="67"/>
-      <c r="BR1" s="67"/>
-      <c r="BS1" s="67"/>
-      <c r="BT1" s="67"/>
-      <c r="BU1" s="67"/>
-      <c r="BV1" s="67"/>
-      <c r="BW1" s="66" t="s">
+      <c r="BQ1" s="68"/>
+      <c r="BR1" s="68"/>
+      <c r="BS1" s="68"/>
+      <c r="BT1" s="68"/>
+      <c r="BU1" s="68"/>
+      <c r="BV1" s="68"/>
+      <c r="BW1" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="BX1" s="67"/>
-      <c r="BY1" s="67"/>
-      <c r="BZ1" s="67"/>
-      <c r="CA1" s="67"/>
-      <c r="CB1" s="67"/>
-      <c r="CC1" s="67"/>
-      <c r="CD1" s="66" t="s">
+      <c r="BX1" s="68"/>
+      <c r="BY1" s="68"/>
+      <c r="BZ1" s="68"/>
+      <c r="CA1" s="68"/>
+      <c r="CB1" s="68"/>
+      <c r="CC1" s="68"/>
+      <c r="CD1" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="CE1" s="67"/>
-      <c r="CF1" s="67"/>
-      <c r="CG1" s="67"/>
-      <c r="CH1" s="67"/>
-      <c r="CI1" s="67"/>
-      <c r="CJ1" s="67"/>
-      <c r="CK1" s="66" t="s">
+      <c r="CE1" s="68"/>
+      <c r="CF1" s="68"/>
+      <c r="CG1" s="68"/>
+      <c r="CH1" s="68"/>
+      <c r="CI1" s="68"/>
+      <c r="CJ1" s="68"/>
+      <c r="CK1" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="CL1" s="67"/>
-      <c r="CM1" s="67"/>
-      <c r="CN1" s="67"/>
-      <c r="CO1" s="67"/>
-      <c r="CP1" s="67"/>
-      <c r="CQ1" s="67"/>
-      <c r="CR1" s="66" t="s">
+      <c r="CL1" s="68"/>
+      <c r="CM1" s="68"/>
+      <c r="CN1" s="68"/>
+      <c r="CO1" s="68"/>
+      <c r="CP1" s="68"/>
+      <c r="CQ1" s="68"/>
+      <c r="CR1" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="CS1" s="67"/>
-      <c r="CT1" s="67"/>
-      <c r="CU1" s="67"/>
-      <c r="CV1" s="67"/>
-      <c r="CW1" s="67"/>
-      <c r="CX1" s="67"/>
-      <c r="CY1" s="66" t="s">
+      <c r="CS1" s="68"/>
+      <c r="CT1" s="68"/>
+      <c r="CU1" s="68"/>
+      <c r="CV1" s="68"/>
+      <c r="CW1" s="68"/>
+      <c r="CX1" s="68"/>
+      <c r="CY1" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="CZ1" s="67"/>
-      <c r="DA1" s="67"/>
-      <c r="DB1" s="67"/>
-      <c r="DC1" s="67"/>
-      <c r="DD1" s="67"/>
-      <c r="DE1" s="67"/>
+      <c r="CZ1" s="68"/>
+      <c r="DA1" s="68"/>
+      <c r="DB1" s="68"/>
+      <c r="DC1" s="68"/>
+      <c r="DD1" s="68"/>
+      <c r="DE1" s="68"/>
       <c r="DF1" s="2"/>
       <c r="DG1" s="2"/>
       <c r="DH1" s="2"/>
@@ -5352,7 +5352,7 @@
     </row>
     <row r="46" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
-      <c r="B46" s="68" t="s">
+      <c r="B46" s="66" t="s">
         <v>54</v>
       </c>
       <c r="C46" s="15" t="s">
@@ -5361,21 +5361,21 @@
     </row>
     <row r="47" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
-      <c r="B47" s="68"/>
+      <c r="B47" s="66"/>
       <c r="C47" s="15" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
-      <c r="B48" s="68"/>
+      <c r="B48" s="66"/>
       <c r="C48" s="15" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A49" s="6"/>
-      <c r="B49" s="68"/>
+      <c r="B49" s="66"/>
       <c r="C49" s="15" t="s">
         <v>224</v>
       </c>
@@ -5385,229 +5385,229 @@
     </row>
     <row r="50" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A50" s="6"/>
-      <c r="B50" s="68"/>
+      <c r="B50" s="66"/>
       <c r="C50" s="15" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A51" s="6"/>
-      <c r="B51" s="68"/>
+      <c r="B51" s="66"/>
       <c r="C51" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B52" s="68"/>
+      <c r="B52" s="66"/>
       <c r="C52" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B53" s="68"/>
+      <c r="B53" s="66"/>
       <c r="C53" s="15" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A54" s="6"/>
-      <c r="B54" s="68"/>
+      <c r="B54" s="66"/>
       <c r="C54" s="15" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A55" s="6"/>
-      <c r="B55" s="68"/>
+      <c r="B55" s="66"/>
       <c r="C55" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A56" s="6"/>
-      <c r="B56" s="68"/>
+      <c r="B56" s="66"/>
       <c r="C56" s="15" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
-      <c r="B57" s="68"/>
+      <c r="B57" s="66"/>
       <c r="C57" s="15" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="68"/>
+      <c r="B58" s="66"/>
       <c r="C58" s="15" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B59" s="68"/>
+      <c r="B59" s="66"/>
       <c r="C59" s="15" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="60" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B60" s="68"/>
+      <c r="B60" s="66"/>
       <c r="C60" s="15" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="61" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B61" s="68"/>
+      <c r="B61" s="66"/>
       <c r="C61" s="15" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B62" s="68"/>
+      <c r="B62" s="66"/>
       <c r="C62" s="59" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="63" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B63" s="68"/>
+      <c r="B63" s="66"/>
       <c r="C63" s="65" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="64" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B64" s="68"/>
+      <c r="B64" s="66"/>
       <c r="C64" s="65" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B65" s="68"/>
+      <c r="B65" s="66"/>
       <c r="C65" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B66" s="68"/>
+      <c r="B66" s="66"/>
       <c r="C66" s="15" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B67" s="68"/>
+      <c r="B67" s="66"/>
       <c r="C67" s="15"/>
     </row>
     <row r="68" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B68" s="68"/>
+      <c r="B68" s="66"/>
       <c r="C68" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B69" s="68"/>
+      <c r="B69" s="66"/>
       <c r="C69" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B70" s="68"/>
+      <c r="B70" s="66"/>
       <c r="C70" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="71" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B71" s="68"/>
+      <c r="B71" s="66"/>
       <c r="C71" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="72" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B72" s="68"/>
+      <c r="B72" s="66"/>
       <c r="C72" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="73" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B73" s="68"/>
+      <c r="B73" s="66"/>
       <c r="C73" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="74" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B74" s="68"/>
+      <c r="B74" s="66"/>
       <c r="C74" s="15" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B75" s="68"/>
+      <c r="B75" s="66"/>
       <c r="C75" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B76" s="68"/>
+      <c r="B76" s="66"/>
       <c r="C76" s="15" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B77" s="68"/>
+      <c r="B77" s="66"/>
       <c r="C77" s="16"/>
     </row>
     <row r="78" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B78" s="68"/>
+      <c r="B78" s="66"/>
       <c r="C78" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B79" s="68"/>
+      <c r="B79" s="66"/>
       <c r="C79" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B80" s="68"/>
+      <c r="B80" s="66"/>
       <c r="C80" s="15" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="81" spans="2:75" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B81" s="68"/>
+      <c r="B81" s="66"/>
       <c r="C81" s="15" t="s">
         <v>72</v>
       </c>
       <c r="BA81" s="6"/>
     </row>
     <row r="82" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B82" s="68"/>
+      <c r="B82" s="66"/>
       <c r="C82" s="16"/>
     </row>
     <row r="83" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B83" s="68"/>
+      <c r="B83" s="66"/>
       <c r="C83" s="15" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="84" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B84" s="68"/>
+      <c r="B84" s="66"/>
       <c r="C84" s="59" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="85" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B85" s="68"/>
+      <c r="B85" s="66"/>
       <c r="C85" s="59" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="86" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B86" s="68"/>
+      <c r="B86" s="66"/>
       <c r="C86" s="59" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="87" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B87" s="68"/>
+      <c r="B87" s="66"/>
       <c r="C87" s="15" t="s">
         <v>258</v>
       </c>
@@ -8362,6 +8362,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="CD1:CJ1"/>
+    <mergeCell ref="B82:B87"/>
+    <mergeCell ref="B46:B81"/>
+    <mergeCell ref="CK1:CQ1"/>
+    <mergeCell ref="CR1:CX1"/>
     <mergeCell ref="CY1:DE1"/>
     <mergeCell ref="E1:K1"/>
     <mergeCell ref="L1:R1"/>
@@ -8374,11 +8379,6 @@
     <mergeCell ref="BI1:BO1"/>
     <mergeCell ref="BP1:BV1"/>
     <mergeCell ref="BW1:CC1"/>
-    <mergeCell ref="CD1:CJ1"/>
-    <mergeCell ref="B82:B87"/>
-    <mergeCell ref="B46:B81"/>
-    <mergeCell ref="CK1:CQ1"/>
-    <mergeCell ref="CR1:CX1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:J4 L4:CW4 CY4:EV4">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
@@ -8413,194 +8413,194 @@
   <sheetData>
     <row r="1" spans="1:158" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="1"/>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="66" t="s">
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="66" t="s">
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="67"/>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="66" t="s">
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="68"/>
+      <c r="W1" s="68"/>
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="67" t="s">
         <v>76</v>
       </c>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="67"/>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="66" t="s">
+      <c r="AA1" s="68"/>
+      <c r="AB1" s="68"/>
+      <c r="AC1" s="68"/>
+      <c r="AD1" s="68"/>
+      <c r="AE1" s="68"/>
+      <c r="AF1" s="68"/>
+      <c r="AG1" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="AH1" s="67"/>
-      <c r="AI1" s="67"/>
-      <c r="AJ1" s="67"/>
-      <c r="AK1" s="67"/>
-      <c r="AL1" s="67"/>
-      <c r="AM1" s="67"/>
-      <c r="AN1" s="66" t="s">
+      <c r="AH1" s="68"/>
+      <c r="AI1" s="68"/>
+      <c r="AJ1" s="68"/>
+      <c r="AK1" s="68"/>
+      <c r="AL1" s="68"/>
+      <c r="AM1" s="68"/>
+      <c r="AN1" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="66" t="s">
+      <c r="AO1" s="68"/>
+      <c r="AP1" s="68"/>
+      <c r="AQ1" s="68"/>
+      <c r="AR1" s="68"/>
+      <c r="AS1" s="68"/>
+      <c r="AT1" s="68"/>
+      <c r="AU1" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="AV1" s="67"/>
-      <c r="AW1" s="67"/>
-      <c r="AX1" s="67"/>
-      <c r="AY1" s="67"/>
-      <c r="AZ1" s="67"/>
-      <c r="BA1" s="67"/>
-      <c r="BB1" s="66" t="s">
+      <c r="AV1" s="68"/>
+      <c r="AW1" s="68"/>
+      <c r="AX1" s="68"/>
+      <c r="AY1" s="68"/>
+      <c r="AZ1" s="68"/>
+      <c r="BA1" s="68"/>
+      <c r="BB1" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="BC1" s="67"/>
-      <c r="BD1" s="67"/>
-      <c r="BE1" s="67"/>
-      <c r="BF1" s="67"/>
-      <c r="BG1" s="67"/>
-      <c r="BH1" s="67"/>
-      <c r="BI1" s="66" t="s">
+      <c r="BC1" s="68"/>
+      <c r="BD1" s="68"/>
+      <c r="BE1" s="68"/>
+      <c r="BF1" s="68"/>
+      <c r="BG1" s="68"/>
+      <c r="BH1" s="68"/>
+      <c r="BI1" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="BJ1" s="67"/>
-      <c r="BK1" s="67"/>
-      <c r="BL1" s="67"/>
-      <c r="BM1" s="67"/>
-      <c r="BN1" s="67"/>
-      <c r="BO1" s="67"/>
-      <c r="BP1" s="66" t="s">
+      <c r="BJ1" s="68"/>
+      <c r="BK1" s="68"/>
+      <c r="BL1" s="68"/>
+      <c r="BM1" s="68"/>
+      <c r="BN1" s="68"/>
+      <c r="BO1" s="68"/>
+      <c r="BP1" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="BQ1" s="67"/>
-      <c r="BR1" s="67"/>
-      <c r="BS1" s="67"/>
-      <c r="BT1" s="67"/>
-      <c r="BU1" s="67"/>
-      <c r="BV1" s="67"/>
-      <c r="BW1" s="66" t="s">
+      <c r="BQ1" s="68"/>
+      <c r="BR1" s="68"/>
+      <c r="BS1" s="68"/>
+      <c r="BT1" s="68"/>
+      <c r="BU1" s="68"/>
+      <c r="BV1" s="68"/>
+      <c r="BW1" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="BX1" s="67"/>
-      <c r="BY1" s="67"/>
-      <c r="BZ1" s="67"/>
-      <c r="CA1" s="67"/>
-      <c r="CB1" s="67"/>
-      <c r="CC1" s="67"/>
-      <c r="CD1" s="66" t="s">
+      <c r="BX1" s="68"/>
+      <c r="BY1" s="68"/>
+      <c r="BZ1" s="68"/>
+      <c r="CA1" s="68"/>
+      <c r="CB1" s="68"/>
+      <c r="CC1" s="68"/>
+      <c r="CD1" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="CE1" s="67"/>
-      <c r="CF1" s="67"/>
-      <c r="CG1" s="67"/>
-      <c r="CH1" s="67"/>
-      <c r="CI1" s="67"/>
-      <c r="CJ1" s="67"/>
-      <c r="CK1" s="66" t="s">
+      <c r="CE1" s="68"/>
+      <c r="CF1" s="68"/>
+      <c r="CG1" s="68"/>
+      <c r="CH1" s="68"/>
+      <c r="CI1" s="68"/>
+      <c r="CJ1" s="68"/>
+      <c r="CK1" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="CL1" s="67"/>
-      <c r="CM1" s="67"/>
-      <c r="CN1" s="67"/>
-      <c r="CO1" s="67"/>
-      <c r="CP1" s="67"/>
-      <c r="CQ1" s="67"/>
-      <c r="CR1" s="66" t="s">
+      <c r="CL1" s="68"/>
+      <c r="CM1" s="68"/>
+      <c r="CN1" s="68"/>
+      <c r="CO1" s="68"/>
+      <c r="CP1" s="68"/>
+      <c r="CQ1" s="68"/>
+      <c r="CR1" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="CS1" s="67"/>
-      <c r="CT1" s="67"/>
-      <c r="CU1" s="67"/>
-      <c r="CV1" s="67"/>
-      <c r="CW1" s="67"/>
-      <c r="CX1" s="67"/>
-      <c r="CY1" s="66" t="s">
+      <c r="CS1" s="68"/>
+      <c r="CT1" s="68"/>
+      <c r="CU1" s="68"/>
+      <c r="CV1" s="68"/>
+      <c r="CW1" s="68"/>
+      <c r="CX1" s="68"/>
+      <c r="CY1" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="CZ1" s="67"/>
-      <c r="DA1" s="67"/>
-      <c r="DB1" s="67"/>
-      <c r="DC1" s="67"/>
-      <c r="DD1" s="67"/>
-      <c r="DE1" s="67"/>
-      <c r="DF1" s="66" t="s">
+      <c r="CZ1" s="68"/>
+      <c r="DA1" s="68"/>
+      <c r="DB1" s="68"/>
+      <c r="DC1" s="68"/>
+      <c r="DD1" s="68"/>
+      <c r="DE1" s="68"/>
+      <c r="DF1" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="DG1" s="67"/>
-      <c r="DH1" s="67"/>
-      <c r="DI1" s="67"/>
-      <c r="DJ1" s="67"/>
-      <c r="DK1" s="67"/>
-      <c r="DL1" s="67"/>
-      <c r="DM1" s="66" t="s">
+      <c r="DG1" s="68"/>
+      <c r="DH1" s="68"/>
+      <c r="DI1" s="68"/>
+      <c r="DJ1" s="68"/>
+      <c r="DK1" s="68"/>
+      <c r="DL1" s="68"/>
+      <c r="DM1" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="DN1" s="67"/>
-      <c r="DO1" s="67"/>
-      <c r="DP1" s="67"/>
-      <c r="DQ1" s="67"/>
-      <c r="DR1" s="67"/>
-      <c r="DS1" s="67"/>
-      <c r="DT1" s="66"/>
-      <c r="DU1" s="67"/>
-      <c r="DV1" s="67"/>
-      <c r="DW1" s="67"/>
-      <c r="DX1" s="67"/>
-      <c r="DY1" s="67"/>
-      <c r="DZ1" s="67"/>
-      <c r="EA1" s="66"/>
-      <c r="EB1" s="67"/>
-      <c r="EC1" s="67"/>
-      <c r="ED1" s="67"/>
-      <c r="EE1" s="67"/>
-      <c r="EF1" s="67"/>
-      <c r="EG1" s="67"/>
-      <c r="EH1" s="66"/>
-      <c r="EI1" s="67"/>
-      <c r="EJ1" s="67"/>
-      <c r="EK1" s="67"/>
-      <c r="EL1" s="67"/>
-      <c r="EM1" s="67"/>
-      <c r="EN1" s="67"/>
-      <c r="EO1" s="66"/>
-      <c r="EP1" s="67"/>
-      <c r="EQ1" s="67"/>
-      <c r="ER1" s="67"/>
-      <c r="ES1" s="67"/>
-      <c r="ET1" s="67"/>
-      <c r="EU1" s="67"/>
-      <c r="EV1" s="66"/>
-      <c r="EW1" s="67"/>
-      <c r="EX1" s="67"/>
-      <c r="EY1" s="67"/>
-      <c r="EZ1" s="67"/>
-      <c r="FA1" s="67"/>
-      <c r="FB1" s="67"/>
+      <c r="DN1" s="68"/>
+      <c r="DO1" s="68"/>
+      <c r="DP1" s="68"/>
+      <c r="DQ1" s="68"/>
+      <c r="DR1" s="68"/>
+      <c r="DS1" s="68"/>
+      <c r="DT1" s="67"/>
+      <c r="DU1" s="68"/>
+      <c r="DV1" s="68"/>
+      <c r="DW1" s="68"/>
+      <c r="DX1" s="68"/>
+      <c r="DY1" s="68"/>
+      <c r="DZ1" s="68"/>
+      <c r="EA1" s="67"/>
+      <c r="EB1" s="68"/>
+      <c r="EC1" s="68"/>
+      <c r="ED1" s="68"/>
+      <c r="EE1" s="68"/>
+      <c r="EF1" s="68"/>
+      <c r="EG1" s="68"/>
+      <c r="EH1" s="67"/>
+      <c r="EI1" s="68"/>
+      <c r="EJ1" s="68"/>
+      <c r="EK1" s="68"/>
+      <c r="EL1" s="68"/>
+      <c r="EM1" s="68"/>
+      <c r="EN1" s="68"/>
+      <c r="EO1" s="67"/>
+      <c r="EP1" s="68"/>
+      <c r="EQ1" s="68"/>
+      <c r="ER1" s="68"/>
+      <c r="ES1" s="68"/>
+      <c r="ET1" s="68"/>
+      <c r="EU1" s="68"/>
+      <c r="EV1" s="67"/>
+      <c r="EW1" s="68"/>
+      <c r="EX1" s="68"/>
+      <c r="EY1" s="68"/>
+      <c r="EZ1" s="68"/>
+      <c r="FA1" s="68"/>
+      <c r="FB1" s="68"/>
     </row>
     <row r="2" spans="1:158" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="1"/>
@@ -10509,13 +10509,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AN1:AT1"/>
-    <mergeCell ref="AU1:BA1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AM1"/>
     <mergeCell ref="EH1:EN1"/>
     <mergeCell ref="EO1:EU1"/>
     <mergeCell ref="EV1:FB1"/>
@@ -10531,6 +10524,13 @@
     <mergeCell ref="DM1:DS1"/>
     <mergeCell ref="DT1:DZ1"/>
     <mergeCell ref="EA1:EG1"/>
+    <mergeCell ref="AN1:AT1"/>
+    <mergeCell ref="AU1:BA1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Zwischenstand Drag & Drop: draggable und droppable nach Zug entfernen"
This reverts commit e245264b41f5897845eaaca8e59461c008a04569
</commit_message>
<xml_diff>
--- a/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
+++ b/documents/Projektmanagement/Zeitbudget, -plan und Meilensteine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Besitzer\Dropbox\Studium\Semester 6\FRONT\FRONT_Projekt\front-projekt\documents\Projektmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E71F537-2787-45EA-BFF6-3ED4E334344F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43DA7E8-42F0-4707-B5E2-276CC1A25390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1247,9 +1247,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="180"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1258,6 +1255,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="180"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="H6" s="30">
         <f>SUM(H10:H77)</f>
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I6" s="27">
         <f>SUM(I10:I77)</f>
@@ -1662,7 +1662,7 @@
       </c>
       <c r="H7" s="30">
         <f t="shared" ref="H7:J7" si="1">H5-H6</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I7" s="27">
         <f t="shared" si="1"/>
@@ -2918,7 +2918,7 @@
         <v>209</v>
       </c>
       <c r="H50" s="22">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I50" s="22">
         <v>4.5</v>
@@ -3743,141 +3743,141 @@
   <sheetData>
     <row r="1" spans="1:166" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="1"/>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="69" t="s">
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="69" t="s">
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="70"/>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="69" t="s">
+      <c r="T1" s="69"/>
+      <c r="U1" s="69"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="69"/>
+      <c r="X1" s="69"/>
+      <c r="Y1" s="69"/>
+      <c r="Z1" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="70"/>
-      <c r="AD1" s="70"/>
-      <c r="AE1" s="70"/>
-      <c r="AF1" s="70"/>
-      <c r="AG1" s="69" t="s">
+      <c r="AA1" s="69"/>
+      <c r="AB1" s="69"/>
+      <c r="AC1" s="69"/>
+      <c r="AD1" s="69"/>
+      <c r="AE1" s="69"/>
+      <c r="AF1" s="69"/>
+      <c r="AG1" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="AH1" s="70"/>
-      <c r="AI1" s="70"/>
-      <c r="AJ1" s="70"/>
-      <c r="AK1" s="70"/>
-      <c r="AL1" s="70"/>
-      <c r="AM1" s="70"/>
-      <c r="AN1" s="67" t="s">
+      <c r="AH1" s="69"/>
+      <c r="AI1" s="69"/>
+      <c r="AJ1" s="69"/>
+      <c r="AK1" s="69"/>
+      <c r="AL1" s="69"/>
+      <c r="AM1" s="69"/>
+      <c r="AN1" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="AO1" s="68"/>
-      <c r="AP1" s="68"/>
-      <c r="AQ1" s="68"/>
-      <c r="AR1" s="68"/>
-      <c r="AS1" s="68"/>
-      <c r="AT1" s="68"/>
-      <c r="AU1" s="67" t="s">
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="67"/>
+      <c r="AT1" s="67"/>
+      <c r="AU1" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="AV1" s="68"/>
-      <c r="AW1" s="68"/>
-      <c r="AX1" s="68"/>
-      <c r="AY1" s="68"/>
-      <c r="AZ1" s="68"/>
-      <c r="BA1" s="68"/>
-      <c r="BB1" s="67" t="s">
+      <c r="AV1" s="67"/>
+      <c r="AW1" s="67"/>
+      <c r="AX1" s="67"/>
+      <c r="AY1" s="67"/>
+      <c r="AZ1" s="67"/>
+      <c r="BA1" s="67"/>
+      <c r="BB1" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="BC1" s="68"/>
-      <c r="BD1" s="68"/>
-      <c r="BE1" s="68"/>
-      <c r="BF1" s="68"/>
-      <c r="BG1" s="68"/>
-      <c r="BH1" s="68"/>
-      <c r="BI1" s="67" t="s">
+      <c r="BC1" s="67"/>
+      <c r="BD1" s="67"/>
+      <c r="BE1" s="67"/>
+      <c r="BF1" s="67"/>
+      <c r="BG1" s="67"/>
+      <c r="BH1" s="67"/>
+      <c r="BI1" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="BJ1" s="68"/>
-      <c r="BK1" s="68"/>
-      <c r="BL1" s="68"/>
-      <c r="BM1" s="68"/>
-      <c r="BN1" s="68"/>
-      <c r="BO1" s="68"/>
-      <c r="BP1" s="67" t="s">
+      <c r="BJ1" s="67"/>
+      <c r="BK1" s="67"/>
+      <c r="BL1" s="67"/>
+      <c r="BM1" s="67"/>
+      <c r="BN1" s="67"/>
+      <c r="BO1" s="67"/>
+      <c r="BP1" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="BQ1" s="68"/>
-      <c r="BR1" s="68"/>
-      <c r="BS1" s="68"/>
-      <c r="BT1" s="68"/>
-      <c r="BU1" s="68"/>
-      <c r="BV1" s="68"/>
-      <c r="BW1" s="67" t="s">
+      <c r="BQ1" s="67"/>
+      <c r="BR1" s="67"/>
+      <c r="BS1" s="67"/>
+      <c r="BT1" s="67"/>
+      <c r="BU1" s="67"/>
+      <c r="BV1" s="67"/>
+      <c r="BW1" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="BX1" s="68"/>
-      <c r="BY1" s="68"/>
-      <c r="BZ1" s="68"/>
-      <c r="CA1" s="68"/>
-      <c r="CB1" s="68"/>
-      <c r="CC1" s="68"/>
-      <c r="CD1" s="67" t="s">
+      <c r="BX1" s="67"/>
+      <c r="BY1" s="67"/>
+      <c r="BZ1" s="67"/>
+      <c r="CA1" s="67"/>
+      <c r="CB1" s="67"/>
+      <c r="CC1" s="67"/>
+      <c r="CD1" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="CE1" s="68"/>
-      <c r="CF1" s="68"/>
-      <c r="CG1" s="68"/>
-      <c r="CH1" s="68"/>
-      <c r="CI1" s="68"/>
-      <c r="CJ1" s="68"/>
-      <c r="CK1" s="67" t="s">
+      <c r="CE1" s="67"/>
+      <c r="CF1" s="67"/>
+      <c r="CG1" s="67"/>
+      <c r="CH1" s="67"/>
+      <c r="CI1" s="67"/>
+      <c r="CJ1" s="67"/>
+      <c r="CK1" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="CL1" s="68"/>
-      <c r="CM1" s="68"/>
-      <c r="CN1" s="68"/>
-      <c r="CO1" s="68"/>
-      <c r="CP1" s="68"/>
-      <c r="CQ1" s="68"/>
-      <c r="CR1" s="67" t="s">
+      <c r="CL1" s="67"/>
+      <c r="CM1" s="67"/>
+      <c r="CN1" s="67"/>
+      <c r="CO1" s="67"/>
+      <c r="CP1" s="67"/>
+      <c r="CQ1" s="67"/>
+      <c r="CR1" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="CS1" s="68"/>
-      <c r="CT1" s="68"/>
-      <c r="CU1" s="68"/>
-      <c r="CV1" s="68"/>
-      <c r="CW1" s="68"/>
-      <c r="CX1" s="68"/>
-      <c r="CY1" s="67" t="s">
+      <c r="CS1" s="67"/>
+      <c r="CT1" s="67"/>
+      <c r="CU1" s="67"/>
+      <c r="CV1" s="67"/>
+      <c r="CW1" s="67"/>
+      <c r="CX1" s="67"/>
+      <c r="CY1" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="CZ1" s="68"/>
-      <c r="DA1" s="68"/>
-      <c r="DB1" s="68"/>
-      <c r="DC1" s="68"/>
-      <c r="DD1" s="68"/>
-      <c r="DE1" s="68"/>
+      <c r="CZ1" s="67"/>
+      <c r="DA1" s="67"/>
+      <c r="DB1" s="67"/>
+      <c r="DC1" s="67"/>
+      <c r="DD1" s="67"/>
+      <c r="DE1" s="67"/>
       <c r="DF1" s="2"/>
       <c r="DG1" s="2"/>
       <c r="DH1" s="2"/>
@@ -5352,7 +5352,7 @@
     </row>
     <row r="46" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
-      <c r="B46" s="66" t="s">
+      <c r="B46" s="70" t="s">
         <v>54</v>
       </c>
       <c r="C46" s="15" t="s">
@@ -5361,21 +5361,21 @@
     </row>
     <row r="47" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
-      <c r="B47" s="66"/>
+      <c r="B47" s="70"/>
       <c r="C47" s="15" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
-      <c r="B48" s="66"/>
+      <c r="B48" s="70"/>
       <c r="C48" s="15" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A49" s="6"/>
-      <c r="B49" s="66"/>
+      <c r="B49" s="70"/>
       <c r="C49" s="15" t="s">
         <v>224</v>
       </c>
@@ -5385,229 +5385,229 @@
     </row>
     <row r="50" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A50" s="6"/>
-      <c r="B50" s="66"/>
+      <c r="B50" s="70"/>
       <c r="C50" s="15" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A51" s="6"/>
-      <c r="B51" s="66"/>
+      <c r="B51" s="70"/>
       <c r="C51" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B52" s="66"/>
+      <c r="B52" s="70"/>
       <c r="C52" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B53" s="66"/>
+      <c r="B53" s="70"/>
       <c r="C53" s="15" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A54" s="6"/>
-      <c r="B54" s="66"/>
+      <c r="B54" s="70"/>
       <c r="C54" s="15" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A55" s="6"/>
-      <c r="B55" s="66"/>
+      <c r="B55" s="70"/>
       <c r="C55" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A56" s="6"/>
-      <c r="B56" s="66"/>
+      <c r="B56" s="70"/>
       <c r="C56" s="15" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:71" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
-      <c r="B57" s="66"/>
+      <c r="B57" s="70"/>
       <c r="C57" s="15" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="66"/>
+      <c r="B58" s="70"/>
       <c r="C58" s="15" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B59" s="66"/>
+      <c r="B59" s="70"/>
       <c r="C59" s="15" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="60" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B60" s="66"/>
+      <c r="B60" s="70"/>
       <c r="C60" s="15" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="61" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B61" s="66"/>
+      <c r="B61" s="70"/>
       <c r="C61" s="15" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B62" s="66"/>
+      <c r="B62" s="70"/>
       <c r="C62" s="59" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="63" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B63" s="66"/>
+      <c r="B63" s="70"/>
       <c r="C63" s="65" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="64" spans="1:71" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B64" s="66"/>
+      <c r="B64" s="70"/>
       <c r="C64" s="65" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B65" s="66"/>
+      <c r="B65" s="70"/>
       <c r="C65" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B66" s="66"/>
+      <c r="B66" s="70"/>
       <c r="C66" s="15" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B67" s="66"/>
+      <c r="B67" s="70"/>
       <c r="C67" s="15"/>
     </row>
     <row r="68" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B68" s="66"/>
+      <c r="B68" s="70"/>
       <c r="C68" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B69" s="66"/>
+      <c r="B69" s="70"/>
       <c r="C69" s="15" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B70" s="66"/>
+      <c r="B70" s="70"/>
       <c r="C70" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="71" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B71" s="66"/>
+      <c r="B71" s="70"/>
       <c r="C71" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="72" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B72" s="66"/>
+      <c r="B72" s="70"/>
       <c r="C72" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="73" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B73" s="66"/>
+      <c r="B73" s="70"/>
       <c r="C73" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="74" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B74" s="66"/>
+      <c r="B74" s="70"/>
       <c r="C74" s="15" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B75" s="66"/>
+      <c r="B75" s="70"/>
       <c r="C75" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B76" s="66"/>
+      <c r="B76" s="70"/>
       <c r="C76" s="15" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B77" s="66"/>
+      <c r="B77" s="70"/>
       <c r="C77" s="16"/>
     </row>
     <row r="78" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B78" s="66"/>
+      <c r="B78" s="70"/>
       <c r="C78" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B79" s="66"/>
+      <c r="B79" s="70"/>
       <c r="C79" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B80" s="66"/>
+      <c r="B80" s="70"/>
       <c r="C80" s="15" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="81" spans="2:75" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="B81" s="66"/>
+      <c r="B81" s="70"/>
       <c r="C81" s="15" t="s">
         <v>72</v>
       </c>
       <c r="BA81" s="6"/>
     </row>
     <row r="82" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B82" s="66"/>
+      <c r="B82" s="70"/>
       <c r="C82" s="16"/>
     </row>
     <row r="83" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B83" s="66"/>
+      <c r="B83" s="70"/>
       <c r="C83" s="15" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="84" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B84" s="66"/>
+      <c r="B84" s="70"/>
       <c r="C84" s="59" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="85" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B85" s="66"/>
+      <c r="B85" s="70"/>
       <c r="C85" s="59" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="86" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B86" s="66"/>
+      <c r="B86" s="70"/>
       <c r="C86" s="59" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="87" spans="2:75" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="B87" s="66"/>
+      <c r="B87" s="70"/>
       <c r="C87" s="15" t="s">
         <v>258</v>
       </c>
@@ -8362,7 +8362,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="CD1:CJ1"/>
     <mergeCell ref="B82:B87"/>
     <mergeCell ref="B46:B81"/>
     <mergeCell ref="CK1:CQ1"/>
@@ -8379,6 +8378,7 @@
     <mergeCell ref="BI1:BO1"/>
     <mergeCell ref="BP1:BV1"/>
     <mergeCell ref="BW1:CC1"/>
+    <mergeCell ref="CD1:CJ1"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:J4 L4:CW4 CY4:EV4">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
@@ -8413,194 +8413,194 @@
   <sheetData>
     <row r="1" spans="1:158" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="1"/>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="67" t="s">
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="67" t="s">
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="67" t="s">
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="AA1" s="68"/>
-      <c r="AB1" s="68"/>
-      <c r="AC1" s="68"/>
-      <c r="AD1" s="68"/>
-      <c r="AE1" s="68"/>
-      <c r="AF1" s="68"/>
-      <c r="AG1" s="67" t="s">
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="AH1" s="68"/>
-      <c r="AI1" s="68"/>
-      <c r="AJ1" s="68"/>
-      <c r="AK1" s="68"/>
-      <c r="AL1" s="68"/>
-      <c r="AM1" s="68"/>
-      <c r="AN1" s="67" t="s">
+      <c r="AH1" s="67"/>
+      <c r="AI1" s="67"/>
+      <c r="AJ1" s="67"/>
+      <c r="AK1" s="67"/>
+      <c r="AL1" s="67"/>
+      <c r="AM1" s="67"/>
+      <c r="AN1" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="AO1" s="68"/>
-      <c r="AP1" s="68"/>
-      <c r="AQ1" s="68"/>
-      <c r="AR1" s="68"/>
-      <c r="AS1" s="68"/>
-      <c r="AT1" s="68"/>
-      <c r="AU1" s="67" t="s">
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="67"/>
+      <c r="AT1" s="67"/>
+      <c r="AU1" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="AV1" s="68"/>
-      <c r="AW1" s="68"/>
-      <c r="AX1" s="68"/>
-      <c r="AY1" s="68"/>
-      <c r="AZ1" s="68"/>
-      <c r="BA1" s="68"/>
-      <c r="BB1" s="67" t="s">
+      <c r="AV1" s="67"/>
+      <c r="AW1" s="67"/>
+      <c r="AX1" s="67"/>
+      <c r="AY1" s="67"/>
+      <c r="AZ1" s="67"/>
+      <c r="BA1" s="67"/>
+      <c r="BB1" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="BC1" s="68"/>
-      <c r="BD1" s="68"/>
-      <c r="BE1" s="68"/>
-      <c r="BF1" s="68"/>
-      <c r="BG1" s="68"/>
-      <c r="BH1" s="68"/>
-      <c r="BI1" s="67" t="s">
+      <c r="BC1" s="67"/>
+      <c r="BD1" s="67"/>
+      <c r="BE1" s="67"/>
+      <c r="BF1" s="67"/>
+      <c r="BG1" s="67"/>
+      <c r="BH1" s="67"/>
+      <c r="BI1" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="BJ1" s="68"/>
-      <c r="BK1" s="68"/>
-      <c r="BL1" s="68"/>
-      <c r="BM1" s="68"/>
-      <c r="BN1" s="68"/>
-      <c r="BO1" s="68"/>
-      <c r="BP1" s="67" t="s">
+      <c r="BJ1" s="67"/>
+      <c r="BK1" s="67"/>
+      <c r="BL1" s="67"/>
+      <c r="BM1" s="67"/>
+      <c r="BN1" s="67"/>
+      <c r="BO1" s="67"/>
+      <c r="BP1" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="BQ1" s="68"/>
-      <c r="BR1" s="68"/>
-      <c r="BS1" s="68"/>
-      <c r="BT1" s="68"/>
-      <c r="BU1" s="68"/>
-      <c r="BV1" s="68"/>
-      <c r="BW1" s="67" t="s">
+      <c r="BQ1" s="67"/>
+      <c r="BR1" s="67"/>
+      <c r="BS1" s="67"/>
+      <c r="BT1" s="67"/>
+      <c r="BU1" s="67"/>
+      <c r="BV1" s="67"/>
+      <c r="BW1" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="BX1" s="68"/>
-      <c r="BY1" s="68"/>
-      <c r="BZ1" s="68"/>
-      <c r="CA1" s="68"/>
-      <c r="CB1" s="68"/>
-      <c r="CC1" s="68"/>
-      <c r="CD1" s="67" t="s">
+      <c r="BX1" s="67"/>
+      <c r="BY1" s="67"/>
+      <c r="BZ1" s="67"/>
+      <c r="CA1" s="67"/>
+      <c r="CB1" s="67"/>
+      <c r="CC1" s="67"/>
+      <c r="CD1" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="CE1" s="68"/>
-      <c r="CF1" s="68"/>
-      <c r="CG1" s="68"/>
-      <c r="CH1" s="68"/>
-      <c r="CI1" s="68"/>
-      <c r="CJ1" s="68"/>
-      <c r="CK1" s="67" t="s">
+      <c r="CE1" s="67"/>
+      <c r="CF1" s="67"/>
+      <c r="CG1" s="67"/>
+      <c r="CH1" s="67"/>
+      <c r="CI1" s="67"/>
+      <c r="CJ1" s="67"/>
+      <c r="CK1" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="CL1" s="68"/>
-      <c r="CM1" s="68"/>
-      <c r="CN1" s="68"/>
-      <c r="CO1" s="68"/>
-      <c r="CP1" s="68"/>
-      <c r="CQ1" s="68"/>
-      <c r="CR1" s="67" t="s">
+      <c r="CL1" s="67"/>
+      <c r="CM1" s="67"/>
+      <c r="CN1" s="67"/>
+      <c r="CO1" s="67"/>
+      <c r="CP1" s="67"/>
+      <c r="CQ1" s="67"/>
+      <c r="CR1" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="CS1" s="68"/>
-      <c r="CT1" s="68"/>
-      <c r="CU1" s="68"/>
-      <c r="CV1" s="68"/>
-      <c r="CW1" s="68"/>
-      <c r="CX1" s="68"/>
-      <c r="CY1" s="67" t="s">
+      <c r="CS1" s="67"/>
+      <c r="CT1" s="67"/>
+      <c r="CU1" s="67"/>
+      <c r="CV1" s="67"/>
+      <c r="CW1" s="67"/>
+      <c r="CX1" s="67"/>
+      <c r="CY1" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="CZ1" s="68"/>
-      <c r="DA1" s="68"/>
-      <c r="DB1" s="68"/>
-      <c r="DC1" s="68"/>
-      <c r="DD1" s="68"/>
-      <c r="DE1" s="68"/>
-      <c r="DF1" s="67" t="s">
+      <c r="CZ1" s="67"/>
+      <c r="DA1" s="67"/>
+      <c r="DB1" s="67"/>
+      <c r="DC1" s="67"/>
+      <c r="DD1" s="67"/>
+      <c r="DE1" s="67"/>
+      <c r="DF1" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="DG1" s="68"/>
-      <c r="DH1" s="68"/>
-      <c r="DI1" s="68"/>
-      <c r="DJ1" s="68"/>
-      <c r="DK1" s="68"/>
-      <c r="DL1" s="68"/>
-      <c r="DM1" s="67" t="s">
+      <c r="DG1" s="67"/>
+      <c r="DH1" s="67"/>
+      <c r="DI1" s="67"/>
+      <c r="DJ1" s="67"/>
+      <c r="DK1" s="67"/>
+      <c r="DL1" s="67"/>
+      <c r="DM1" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="DN1" s="68"/>
-      <c r="DO1" s="68"/>
-      <c r="DP1" s="68"/>
-      <c r="DQ1" s="68"/>
-      <c r="DR1" s="68"/>
-      <c r="DS1" s="68"/>
-      <c r="DT1" s="67"/>
-      <c r="DU1" s="68"/>
-      <c r="DV1" s="68"/>
-      <c r="DW1" s="68"/>
-      <c r="DX1" s="68"/>
-      <c r="DY1" s="68"/>
-      <c r="DZ1" s="68"/>
-      <c r="EA1" s="67"/>
-      <c r="EB1" s="68"/>
-      <c r="EC1" s="68"/>
-      <c r="ED1" s="68"/>
-      <c r="EE1" s="68"/>
-      <c r="EF1" s="68"/>
-      <c r="EG1" s="68"/>
-      <c r="EH1" s="67"/>
-      <c r="EI1" s="68"/>
-      <c r="EJ1" s="68"/>
-      <c r="EK1" s="68"/>
-      <c r="EL1" s="68"/>
-      <c r="EM1" s="68"/>
-      <c r="EN1" s="68"/>
-      <c r="EO1" s="67"/>
-      <c r="EP1" s="68"/>
-      <c r="EQ1" s="68"/>
-      <c r="ER1" s="68"/>
-      <c r="ES1" s="68"/>
-      <c r="ET1" s="68"/>
-      <c r="EU1" s="68"/>
-      <c r="EV1" s="67"/>
-      <c r="EW1" s="68"/>
-      <c r="EX1" s="68"/>
-      <c r="EY1" s="68"/>
-      <c r="EZ1" s="68"/>
-      <c r="FA1" s="68"/>
-      <c r="FB1" s="68"/>
+      <c r="DN1" s="67"/>
+      <c r="DO1" s="67"/>
+      <c r="DP1" s="67"/>
+      <c r="DQ1" s="67"/>
+      <c r="DR1" s="67"/>
+      <c r="DS1" s="67"/>
+      <c r="DT1" s="66"/>
+      <c r="DU1" s="67"/>
+      <c r="DV1" s="67"/>
+      <c r="DW1" s="67"/>
+      <c r="DX1" s="67"/>
+      <c r="DY1" s="67"/>
+      <c r="DZ1" s="67"/>
+      <c r="EA1" s="66"/>
+      <c r="EB1" s="67"/>
+      <c r="EC1" s="67"/>
+      <c r="ED1" s="67"/>
+      <c r="EE1" s="67"/>
+      <c r="EF1" s="67"/>
+      <c r="EG1" s="67"/>
+      <c r="EH1" s="66"/>
+      <c r="EI1" s="67"/>
+      <c r="EJ1" s="67"/>
+      <c r="EK1" s="67"/>
+      <c r="EL1" s="67"/>
+      <c r="EM1" s="67"/>
+      <c r="EN1" s="67"/>
+      <c r="EO1" s="66"/>
+      <c r="EP1" s="67"/>
+      <c r="EQ1" s="67"/>
+      <c r="ER1" s="67"/>
+      <c r="ES1" s="67"/>
+      <c r="ET1" s="67"/>
+      <c r="EU1" s="67"/>
+      <c r="EV1" s="66"/>
+      <c r="EW1" s="67"/>
+      <c r="EX1" s="67"/>
+      <c r="EY1" s="67"/>
+      <c r="EZ1" s="67"/>
+      <c r="FA1" s="67"/>
+      <c r="FB1" s="67"/>
     </row>
     <row r="2" spans="1:158" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="1"/>
@@ -10509,6 +10509,13 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="AN1:AT1"/>
+    <mergeCell ref="AU1:BA1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AM1"/>
     <mergeCell ref="EH1:EN1"/>
     <mergeCell ref="EO1:EU1"/>
     <mergeCell ref="EV1:FB1"/>
@@ -10524,13 +10531,6 @@
     <mergeCell ref="DM1:DS1"/>
     <mergeCell ref="DT1:DZ1"/>
     <mergeCell ref="EA1:EG1"/>
-    <mergeCell ref="AN1:AT1"/>
-    <mergeCell ref="AU1:BA1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>